<commit_message>
updating datasheet and protocol
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="29">
   <si>
     <t>Site</t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>MilfordST</t>
+  </si>
+  <si>
+    <t>Collector</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>2017-08-25</t>
+  </si>
+  <si>
+    <t>2017-08-21</t>
+  </si>
+  <si>
+    <t>2017-09-07</t>
   </si>
 </sst>
 </file>
@@ -411,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,12 +440,12 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.83203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.83203125" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,23 +467,26 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -476,7 +497,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -487,11 +508,14 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -502,7 +526,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -513,11 +537,14 @@
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -528,7 +555,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -539,11 +566,14 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -554,7 +584,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -565,11 +595,14 @@
       <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -580,7 +613,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
@@ -591,11 +624,11 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -606,7 +639,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
@@ -617,11 +650,11 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -632,7 +665,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
@@ -643,8 +676,205 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>0</v>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding randomization, and updating datasheet
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewnguyen/Circadian_rhythm_runs_seasonal_timing/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="5580" yWindow="680" windowWidth="32020" windowHeight="24600" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -14,20 +19,20 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Maggot_collections!$A$1:$I$41</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="82">
   <si>
     <t>Site</t>
   </si>
@@ -242,9 +247,6 @@
     <t>tape</t>
   </si>
   <si>
-    <t>mass</t>
-  </si>
-  <si>
     <t>purge_time</t>
   </si>
   <si>
@@ -270,6 +272,12 @@
   </si>
   <si>
     <t>Blank</t>
+  </si>
+  <si>
+    <t>mass_day10</t>
+  </si>
+  <si>
+    <t>resp_day11</t>
   </si>
 </sst>
 </file>
@@ -282,7 +290,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -337,8 +344,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -407,7 +416,7 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -428,6 +437,7 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -448,6 +458,7 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,7 +726,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -732,7 +743,7 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="5" width="10.83203125" style="1"/>
     <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -750,7 +761,7 @@
     <col min="18" max="18" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -806,7 +817,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="2" customFormat="1">
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -850,7 +861,7 @@
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
     </row>
-    <row r="3" spans="1:19" s="2" customFormat="1">
+    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -893,7 +904,7 @@
       </c>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:19" s="2" customFormat="1">
+    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -936,7 +947,7 @@
       </c>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:19" s="2" customFormat="1">
+    <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -979,7 +990,7 @@
       </c>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:19" s="2" customFormat="1">
+    <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1020,7 +1031,7 @@
       </c>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:19" s="2" customFormat="1">
+    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1061,7 +1072,7 @@
       </c>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:19" s="2" customFormat="1">
+    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1102,7 +1113,7 @@
       </c>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1143,7 +1154,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1184,7 +1195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1225,7 +1236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1266,7 +1277,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1304,7 +1315,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1342,7 +1353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1383,7 +1394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="2" customFormat="1">
+    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1437,7 @@
       </c>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="1:18" s="2" customFormat="1">
+    <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -1469,7 +1480,7 @@
       </c>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18" s="2" customFormat="1">
+    <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1510,7 +1521,7 @@
       </c>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="1:18" s="2" customFormat="1">
+    <row r="19" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1553,7 +1564,7 @@
       </c>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="1:18" s="2" customFormat="1">
+    <row r="20" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1596,7 +1607,7 @@
       </c>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1637,7 +1648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1678,7 +1689,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1717,7 +1728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1758,7 +1769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1799,7 +1810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="2" customFormat="1">
+    <row r="26" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>4</v>
       </c>
@@ -1842,7 +1853,7 @@
       </c>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="1:18" s="2" customFormat="1">
+    <row r="27" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -1885,7 +1896,7 @@
       </c>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="1:18" s="2" customFormat="1">
+    <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -1926,7 +1937,7 @@
       </c>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="1:18" s="2" customFormat="1">
+    <row r="29" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1967,7 +1978,7 @@
       </c>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="1:18" s="2" customFormat="1">
+    <row r="30" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -2010,7 +2021,7 @@
       </c>
       <c r="R30" s="3"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2051,7 +2062,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2092,7 +2103,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -2133,7 +2144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -2171,7 +2182,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -2212,7 +2223,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:18" s="2" customFormat="1">
+    <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>4</v>
       </c>
@@ -2255,7 +2266,7 @@
       </c>
       <c r="R36" s="3"/>
     </row>
-    <row r="37" spans="1:18" s="2" customFormat="1">
+    <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>4</v>
       </c>
@@ -2298,7 +2309,7 @@
       </c>
       <c r="R37" s="3"/>
     </row>
-    <row r="38" spans="1:18" s="2" customFormat="1">
+    <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
@@ -2339,7 +2350,7 @@
       </c>
       <c r="R38" s="3"/>
     </row>
-    <row r="39" spans="1:18" s="2" customFormat="1">
+    <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
@@ -2382,7 +2393,7 @@
       </c>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:18" s="2" customFormat="1">
+    <row r="40" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
@@ -2425,7 +2436,7 @@
       </c>
       <c r="R40" s="3"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -2466,7 +2477,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -2507,7 +2518,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2545,7 +2556,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2586,7 +2597,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2627,7 +2638,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:18" s="2" customFormat="1">
+    <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>4</v>
       </c>
@@ -2670,7 +2681,7 @@
       </c>
       <c r="R46" s="3"/>
     </row>
-    <row r="47" spans="1:18" s="2" customFormat="1">
+    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -2713,7 +2724,7 @@
       </c>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:18" s="2" customFormat="1">
+    <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
@@ -2756,7 +2767,7 @@
       </c>
       <c r="R48" s="3"/>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1">
+    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
@@ -2799,7 +2810,7 @@
       </c>
       <c r="R49" s="3"/>
     </row>
-    <row r="50" spans="1:18" s="2" customFormat="1">
+    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>12</v>
       </c>
@@ -2842,7 +2853,7 @@
       </c>
       <c r="R50" s="3"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -2883,7 +2894,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -2924,7 +2935,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2965,7 +2976,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -3003,7 +3014,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -3044,7 +3055,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:18" s="2" customFormat="1">
+    <row r="56" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>4</v>
       </c>
@@ -3087,7 +3098,7 @@
       </c>
       <c r="R56" s="3"/>
     </row>
-    <row r="57" spans="1:18" s="2" customFormat="1">
+    <row r="57" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>4</v>
       </c>
@@ -3130,7 +3141,7 @@
       </c>
       <c r="R57" s="3"/>
     </row>
-    <row r="58" spans="1:18" s="2" customFormat="1">
+    <row r="58" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>12</v>
       </c>
@@ -3173,7 +3184,7 @@
       </c>
       <c r="R58" s="3"/>
     </row>
-    <row r="59" spans="1:18" s="2" customFormat="1">
+    <row r="59" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>12</v>
       </c>
@@ -3214,7 +3225,7 @@
       </c>
       <c r="R59" s="3"/>
     </row>
-    <row r="60" spans="1:18" s="2" customFormat="1">
+    <row r="60" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>12</v>
       </c>
@@ -3257,7 +3268,7 @@
       </c>
       <c r="R60" s="3"/>
     </row>
-    <row r="66" spans="8:9">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H66" s="8" t="s">
         <v>42</v>
       </c>
@@ -3266,7 +3277,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="68" spans="8:9">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.2">
       <c r="I68" s="8">
         <f>SUM(I9:I15)</f>
         <v>107</v>
@@ -3276,28 +3287,23 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="8" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -3308,33 +3314,36 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>77</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -3357,13 +3366,16 @@
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="J2">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -3386,13 +3398,16 @@
       <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="J3">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -3415,13 +3430,16 @@
       <c r="I4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="J4">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3444,13 +3462,16 @@
       <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="J5">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -3473,13 +3494,16 @@
       <c r="I6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -3502,13 +3526,16 @@
       <c r="I7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -3531,13 +3558,16 @@
       <c r="I8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="J8">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -3560,13 +3590,16 @@
       <c r="I9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="J9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -3589,13 +3622,16 @@
       <c r="I10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -3618,13 +3654,16 @@
       <c r="I11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -3647,13 +3686,16 @@
       <c r="I12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -3676,13 +3718,16 @@
       <c r="I13" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -3705,13 +3750,16 @@
       <c r="I14" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="J14">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -3734,13 +3782,16 @@
       <c r="I15" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="J15">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -3763,13 +3814,16 @@
       <c r="I16" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -3792,13 +3846,16 @@
       <c r="I17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -3821,13 +3878,16 @@
       <c r="I18" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -3850,13 +3910,16 @@
       <c r="I19" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -3879,13 +3942,16 @@
       <c r="I20" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -3908,13 +3974,16 @@
       <c r="I21" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -3937,13 +4006,25 @@
       <c r="I22" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>6.4820000000000002</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0.56666666666666665</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>49</v>
@@ -3957,22 +4038,25 @@
       <c r="I23" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24">
-        <v>6.4820000000000002</v>
+        <v>9.2769999999999992</v>
       </c>
       <c r="E24" s="12">
-        <v>0.56666666666666665</v>
+        <v>0.56736111111111109</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>49</v>
@@ -3986,22 +4070,25 @@
       <c r="I24" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>9.2769999999999992</v>
+        <v>8.9060000000000006</v>
       </c>
       <c r="E25" s="12">
-        <v>0.56736111111111109</v>
+        <v>0.57708333333333328</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>49</v>
@@ -4015,81 +4102,90 @@
       <c r="I25" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>6.1210000000000004</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>9.0730000000000004</v>
+      </c>
+      <c r="E27" s="12">
+        <v>0.57361111111111118</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
         <v>5</v>
       </c>
-      <c r="D26">
-        <v>8.9060000000000006</v>
-      </c>
-      <c r="E26" s="12">
+      <c r="D28">
+        <v>9.7330000000000005</v>
+      </c>
+      <c r="E28" s="12">
         <v>0.57708333333333328</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27">
-        <v>6.1210000000000004</v>
-      </c>
-      <c r="E27" s="12">
-        <v>0.57430555555555551</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28">
-        <v>9.0730000000000004</v>
-      </c>
-      <c r="E28" s="12">
-        <v>0.57361111111111118</v>
-      </c>
       <c r="F28" s="1" t="s">
         <v>49</v>
       </c>
@@ -4102,51 +4198,57 @@
       <c r="I28" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>7.4480000000000004</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
         <v>5</v>
       </c>
-      <c r="D29">
-        <v>9.7330000000000005</v>
-      </c>
-      <c r="E29" s="12">
-        <v>0.57708333333333328</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
       <c r="D30">
-        <v>7.4480000000000004</v>
+        <v>6.1150000000000002</v>
       </c>
       <c r="E30" s="12">
-        <v>0.5625</v>
+        <v>0.5708333333333333</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>49</v>
@@ -4160,109 +4262,121 @@
       <c r="I30" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31">
+        <v>8.2729999999999997</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s">
         <v>5</v>
       </c>
-      <c r="D31">
-        <v>6.1150000000000002</v>
-      </c>
-      <c r="E31" s="12">
-        <v>0.5708333333333333</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
       <c r="D32">
-        <v>8.2729999999999997</v>
+        <v>6.5129999999999999</v>
       </c>
       <c r="E32" s="12">
+        <v>0.57777777777777783</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>8.1029999999999998</v>
+      </c>
+      <c r="E33" s="12">
         <v>0.57916666666666672</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="F33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J33">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" t="s">
         <v>5</v>
       </c>
-      <c r="D33">
-        <v>6.5129999999999999</v>
-      </c>
-      <c r="E33" s="12">
-        <v>0.57777777777777783</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
       <c r="D34">
-        <v>8.1029999999999998</v>
+        <v>10.292999999999999</v>
       </c>
       <c r="E34" s="12">
-        <v>0.57916666666666672</v>
+        <v>0.57847222222222217</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>49</v>
@@ -4276,22 +4390,25 @@
       <c r="I34" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35">
-        <v>10.292999999999999</v>
+        <v>9.6539999999999999</v>
       </c>
       <c r="E35" s="12">
-        <v>0.57847222222222217</v>
+        <v>0.57986111111111105</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>49</v>
@@ -4305,80 +4422,89 @@
       <c r="I35" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <v>4.7469999999999999</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <v>7.7530000000000001</v>
+      </c>
+      <c r="E37" s="12">
+        <v>0.56319444444444444</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
         <v>5</v>
       </c>
-      <c r="D36">
-        <v>9.6539999999999999</v>
-      </c>
-      <c r="E36" s="12">
-        <v>0.57986111111111105</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37">
-        <v>4.7469999999999999</v>
-      </c>
-      <c r="E37" s="12">
-        <v>0.5625</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
       <c r="D38">
-        <v>7.7530000000000001</v>
+        <v>10.935</v>
       </c>
       <c r="E38" s="12">
-        <v>0.56319444444444444</v>
+        <v>0.5805555555555556</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>49</v>
@@ -4392,19 +4518,22 @@
       <c r="I38" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D39">
-        <v>10.935</v>
+        <v>9.7409999999999997</v>
       </c>
       <c r="E39" s="12">
         <v>0.5805555555555556</v>
@@ -4421,22 +4550,25 @@
       <c r="I39" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D40">
-        <v>9.7409999999999997</v>
+        <v>8.2650000000000006</v>
       </c>
       <c r="E40" s="12">
-        <v>0.5805555555555556</v>
+        <v>0.56388888888888888</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>49</v>
@@ -4450,164 +4582,182 @@
       <c r="I40" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41">
+        <v>4.7910000000000004</v>
+      </c>
+      <c r="E41" s="12">
+        <v>0.56180555555555556</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42">
+        <v>6.4619999999999997</v>
+      </c>
+      <c r="E42" s="12">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43">
+        <v>6.8170000000000002</v>
+      </c>
+      <c r="E43" s="12">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J43">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44">
+        <v>7.5250000000000004</v>
+      </c>
+      <c r="E44" s="12">
+        <v>0.56041666666666667</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="12">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" t="s">
         <v>5</v>
       </c>
-      <c r="D41">
-        <v>8.2650000000000006</v>
-      </c>
-      <c r="E41" s="12">
-        <v>0.56388888888888888</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42">
-        <v>4.7910000000000004</v>
-      </c>
-      <c r="E42" s="12">
-        <v>0.56180555555555556</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43">
-        <v>6.4619999999999997</v>
-      </c>
-      <c r="E43" s="12">
-        <v>0.55902777777777779</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44">
-        <v>6.8170000000000002</v>
-      </c>
-      <c r="E44" s="12">
-        <v>0.5708333333333333</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45">
-        <v>7.5250000000000004</v>
-      </c>
-      <c r="E45" s="12">
-        <v>0.56041666666666667</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" t="s">
-        <v>80</v>
+      <c r="D46">
+        <v>11.206</v>
       </c>
       <c r="E46" s="12">
-        <v>0.54513888888888895</v>
+        <v>0.58124999999999993</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>49</v>
@@ -4621,22 +4771,25 @@
       <c r="I46" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
       <c r="D47">
-        <v>11.206</v>
+        <v>9.6329999999999991</v>
       </c>
       <c r="E47" s="12">
-        <v>0.58124999999999993</v>
+        <v>0.57638888888888895</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>49</v>
@@ -4650,22 +4803,25 @@
       <c r="I47" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D48">
-        <v>9.6329999999999991</v>
+        <v>5.2210000000000001</v>
       </c>
       <c r="E48" s="12">
-        <v>0.57638888888888895</v>
+        <v>0.56041666666666667</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>49</v>
@@ -4679,22 +4835,25 @@
       <c r="I48" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C49" t="s">
         <v>11</v>
       </c>
       <c r="D49">
-        <v>5.2210000000000001</v>
+        <v>7.6680000000000001</v>
       </c>
       <c r="E49" s="12">
-        <v>0.56041666666666667</v>
+        <v>0.55972222222222223</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>49</v>
@@ -4708,22 +4867,22 @@
       <c r="I49" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50">
-        <v>7.6680000000000001</v>
+        <v>79</v>
       </c>
       <c r="E50" s="12">
-        <v>0.55972222222222223</v>
+        <v>0.54513888888888895</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>49</v>
@@ -4737,19 +4896,25 @@
       <c r="I50" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B51" t="s">
         <v>76</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>9.9450000000000003</v>
       </c>
       <c r="E51" s="12">
-        <v>0.54513888888888895</v>
+        <v>0.54861111111111105</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>49</v>
@@ -4763,19 +4928,22 @@
       <c r="I51" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D52">
-        <v>9.9450000000000003</v>
+        <v>6.5880000000000001</v>
       </c>
       <c r="E52" s="12">
         <v>0.54861111111111105</v>
@@ -4792,22 +4960,25 @@
       <c r="I52" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D53">
-        <v>6.5880000000000001</v>
+        <v>9.3539999999999992</v>
       </c>
       <c r="E53" s="12">
-        <v>0.54861111111111105</v>
+        <v>0.5493055555555556</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>49</v>
@@ -4821,52 +4992,58 @@
       <c r="I53" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54">
+        <v>14.863</v>
+      </c>
+      <c r="E54" s="12">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55">
         <v>5</v>
       </c>
-      <c r="D54">
-        <v>9.3539999999999992</v>
-      </c>
-      <c r="E54" s="12">
+      <c r="B55" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>6.7679999999999998</v>
+      </c>
+      <c r="E55" s="12">
         <v>0.5493055555555556</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55">
-        <v>4</v>
-      </c>
-      <c r="B55" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55">
-        <v>14.863</v>
-      </c>
-      <c r="E55" s="12">
-        <v>0.54583333333333328</v>
-      </c>
       <c r="F55" s="1" t="s">
         <v>49</v>
       </c>
@@ -4879,80 +5056,89 @@
       <c r="I55" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56">
+        <v>5.899</v>
+      </c>
+      <c r="E56" s="12">
+        <v>0.54722222222222217</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57">
+        <v>5.3380000000000001</v>
+      </c>
+      <c r="E57" s="12">
+        <v>0.54791666666666672</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J57">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" t="s">
         <v>5</v>
       </c>
-      <c r="B56" t="s">
-        <v>77</v>
-      </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56">
-        <v>6.7679999999999998</v>
-      </c>
-      <c r="E56" s="12">
-        <v>0.5493055555555556</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57">
-        <v>6</v>
-      </c>
-      <c r="B57" t="s">
-        <v>77</v>
-      </c>
-      <c r="C57" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57">
-        <v>5.899</v>
-      </c>
-      <c r="E57" s="12">
-        <v>0.54722222222222217</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58">
-        <v>7</v>
-      </c>
-      <c r="B58" t="s">
-        <v>77</v>
-      </c>
-      <c r="C58" t="s">
-        <v>11</v>
-      </c>
       <c r="D58">
-        <v>5.3380000000000001</v>
+        <v>7.2279999999999998</v>
       </c>
       <c r="E58" s="12">
-        <v>0.54791666666666672</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>49</v>
@@ -4966,22 +5152,25 @@
       <c r="I58" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="D59">
-        <v>7.2279999999999998</v>
+        <v>6.6109999999999998</v>
       </c>
       <c r="E59" s="12">
-        <v>0.54999999999999993</v>
+        <v>0.55069444444444449</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>49</v>
@@ -4995,19 +5184,22 @@
       <c r="I59" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D60">
-        <v>6.6109999999999998</v>
+        <v>7.4160000000000004</v>
       </c>
       <c r="E60" s="12">
         <v>0.55069444444444449</v>
@@ -5024,19 +5216,22 @@
       <c r="I60" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C61" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D61">
-        <v>7.4160000000000004</v>
+        <v>10.782999999999999</v>
       </c>
       <c r="E61" s="12">
         <v>0.55069444444444449</v>
@@ -5053,51 +5248,57 @@
       <c r="I61" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62">
+        <v>8.69</v>
+      </c>
+      <c r="E62" s="12">
+        <v>0.54652777777777783</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>13</v>
+      </c>
+      <c r="B63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" t="s">
         <v>5</v>
       </c>
-      <c r="D62">
-        <v>10.782999999999999</v>
-      </c>
-      <c r="E62" s="12">
-        <v>0.55069444444444449</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63">
-        <v>12</v>
-      </c>
-      <c r="B63" t="s">
-        <v>77</v>
-      </c>
-      <c r="C63" t="s">
-        <v>11</v>
-      </c>
       <c r="D63">
-        <v>8.69</v>
+        <v>6.2649999999999997</v>
       </c>
       <c r="E63" s="12">
-        <v>0.54652777777777783</v>
+        <v>0.55138888888888882</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>49</v>
@@ -5111,22 +5312,25 @@
       <c r="I63" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
       <c r="D64">
-        <v>6.2649999999999997</v>
+        <v>9.2639999999999993</v>
       </c>
       <c r="E64" s="12">
-        <v>0.55138888888888882</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>49</v>
@@ -5140,324 +5344,378 @@
       <c r="I64" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65">
+        <v>6.7670000000000003</v>
+      </c>
+      <c r="E65" s="12">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J65">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" t="s">
         <v>5</v>
       </c>
-      <c r="D65">
-        <v>9.2639999999999993</v>
-      </c>
-      <c r="E65" s="12">
-        <v>0.55208333333333337</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66">
+      <c r="D66">
+        <v>10.023999999999999</v>
+      </c>
+      <c r="E66" s="12">
+        <v>0.54722222222222217</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>17</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67">
+        <v>9.1359999999999992</v>
+      </c>
+      <c r="E67" s="12">
+        <v>0.54652777777777783</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J67">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>18</v>
+      </c>
+      <c r="B68" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68">
+        <v>4.34</v>
+      </c>
+      <c r="E68" s="12">
+        <v>0.56736111111111109</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J68">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>19</v>
+      </c>
+      <c r="B69" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>7.72</v>
+      </c>
+      <c r="E69" s="12">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J69">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>22</v>
+      </c>
+      <c r="B70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70">
+        <v>8.6150000000000002</v>
+      </c>
+      <c r="E70" s="12">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J70">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>23</v>
+      </c>
+      <c r="B71" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71">
+        <v>6.9539999999999997</v>
+      </c>
+      <c r="E71" s="12">
+        <v>0.54027777777777775</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J71">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>24</v>
+      </c>
+      <c r="B72" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72">
+        <v>8.1669999999999998</v>
+      </c>
+      <c r="E72" s="12">
+        <v>0.5395833333333333</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J72">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>25</v>
+      </c>
+      <c r="B73" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73">
+        <v>9.7590000000000003</v>
+      </c>
+      <c r="E73" s="12">
+        <v>0.55625000000000002</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J73">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>26</v>
+      </c>
+      <c r="B74" t="s">
+        <v>76</v>
+      </c>
+      <c r="C74" t="s">
+        <v>78</v>
+      </c>
+      <c r="D74">
+        <v>12.097</v>
+      </c>
+      <c r="E74" s="12">
+        <v>0.55347222222222225</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B66" t="s">
-        <v>77</v>
-      </c>
-      <c r="C66" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66">
-        <v>6.7670000000000003</v>
-      </c>
-      <c r="E66" s="12">
-        <v>0.54513888888888895</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67">
-        <v>16</v>
-      </c>
-      <c r="B67" t="s">
-        <v>77</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="J74">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>27</v>
+      </c>
+      <c r="B75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75">
+        <v>7.8490000000000002</v>
+      </c>
+      <c r="E75" s="12">
+        <v>0.58194444444444449</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J75">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>28</v>
+      </c>
+      <c r="B76" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" t="s">
         <v>5</v>
       </c>
-      <c r="D67">
-        <v>10.023999999999999</v>
-      </c>
-      <c r="E67" s="12">
-        <v>0.54722222222222217</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68">
-        <v>17</v>
-      </c>
-      <c r="B68" t="s">
-        <v>77</v>
-      </c>
-      <c r="C68" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68">
-        <v>9.1359999999999992</v>
-      </c>
-      <c r="E68" s="12">
-        <v>0.54652777777777783</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69">
-        <v>18</v>
-      </c>
-      <c r="B69" t="s">
-        <v>77</v>
-      </c>
-      <c r="C69" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69">
-        <v>4.34</v>
-      </c>
-      <c r="E69" s="12">
-        <v>0.56736111111111109</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70">
-        <v>19</v>
-      </c>
-      <c r="B70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C70" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70">
-        <v>7.72</v>
-      </c>
-      <c r="E70" s="12">
-        <v>0.55277777777777781</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71">
-        <v>20</v>
-      </c>
-      <c r="B71" t="s">
-        <v>77</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72">
-        <v>21</v>
-      </c>
-      <c r="B72" t="s">
-        <v>77</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73">
-        <v>22</v>
-      </c>
-      <c r="B73" t="s">
-        <v>77</v>
-      </c>
-      <c r="C73" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73">
-        <v>8.6150000000000002</v>
-      </c>
-      <c r="E73" s="12">
+      <c r="D76">
+        <v>7.7469999999999999</v>
+      </c>
+      <c r="E76" s="12">
         <v>0.5541666666666667</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74">
-        <v>23</v>
-      </c>
-      <c r="B74" t="s">
-        <v>77</v>
-      </c>
-      <c r="C74" t="s">
-        <v>11</v>
-      </c>
-      <c r="D74">
-        <v>6.9539999999999997</v>
-      </c>
-      <c r="E74" s="12">
-        <v>0.54027777777777775</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75">
-        <v>24</v>
-      </c>
-      <c r="B75" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75">
-        <v>8.1669999999999998</v>
-      </c>
-      <c r="E75" s="12">
-        <v>0.5395833333333333</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76">
-        <v>25</v>
-      </c>
-      <c r="B76" t="s">
-        <v>77</v>
-      </c>
-      <c r="C76" t="s">
-        <v>11</v>
-      </c>
-      <c r="D76">
-        <v>9.7590000000000003</v>
-      </c>
-      <c r="E76" s="12">
-        <v>0.55625000000000002</v>
-      </c>
       <c r="F76" s="1" t="s">
         <v>49</v>
       </c>
@@ -5470,22 +5728,25 @@
       <c r="I76" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C77" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="D77">
-        <v>12.097</v>
+        <v>8.1720000000000006</v>
       </c>
       <c r="E77" s="12">
-        <v>0.55347222222222225</v>
+        <v>0.53888888888888886</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>49</v>
@@ -5497,24 +5758,27 @@
         <v>34</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+        <v>6</v>
+      </c>
+      <c r="J77">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C78" t="s">
         <v>11</v>
       </c>
       <c r="D78">
-        <v>7.8490000000000002</v>
+        <v>5.0430000000000001</v>
       </c>
       <c r="E78" s="12">
-        <v>0.58194444444444449</v>
+        <v>0.5444444444444444</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>49</v>
@@ -5528,22 +5792,25 @@
       <c r="I78" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C79" t="s">
         <v>5</v>
       </c>
       <c r="D79">
-        <v>7.7469999999999999</v>
+        <v>12.058</v>
       </c>
       <c r="E79" s="12">
-        <v>0.5541666666666667</v>
+        <v>0.55486111111111114</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>49</v>
@@ -5557,22 +5824,25 @@
       <c r="I79" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
       </c>
       <c r="D80">
-        <v>8.1720000000000006</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="E80" s="12">
-        <v>0.53888888888888886</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>49</v>
@@ -5586,22 +5856,25 @@
       <c r="I80" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D81">
-        <v>5.0430000000000001</v>
+        <v>9.8759999999999994</v>
       </c>
       <c r="E81" s="12">
-        <v>0.5444444444444444</v>
+        <v>0.55486111111111114</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>49</v>
@@ -5615,51 +5888,57 @@
       <c r="I81" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C82" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82">
+        <v>7.8869999999999996</v>
+      </c>
+      <c r="E82" s="12">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J82">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>35</v>
+      </c>
+      <c r="B83" t="s">
+        <v>76</v>
+      </c>
+      <c r="C83" t="s">
         <v>5</v>
       </c>
-      <c r="D82">
-        <v>12.058</v>
-      </c>
-      <c r="E82" s="12">
-        <v>0.55486111111111114</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83">
-        <v>32</v>
-      </c>
-      <c r="B83" t="s">
-        <v>77</v>
-      </c>
-      <c r="C83" t="s">
-        <v>11</v>
-      </c>
       <c r="D83">
-        <v>8.9700000000000006</v>
+        <v>10.409000000000001</v>
       </c>
       <c r="E83" s="12">
-        <v>0.55555555555555558</v>
+        <v>0.55763888888888891</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>49</v>
@@ -5673,22 +5952,25 @@
       <c r="I83" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
       </c>
       <c r="D84">
-        <v>9.8759999999999994</v>
+        <v>10.176</v>
       </c>
       <c r="E84" s="12">
-        <v>0.55486111111111114</v>
+        <v>0.55763888888888891</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>49</v>
@@ -5702,22 +5984,25 @@
       <c r="I84" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C85" t="s">
         <v>11</v>
       </c>
       <c r="D85">
-        <v>7.8869999999999996</v>
+        <v>7.9450000000000003</v>
       </c>
       <c r="E85" s="12">
-        <v>0.54583333333333328</v>
+        <v>0.53819444444444442</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>49</v>
@@ -5731,22 +6016,25 @@
       <c r="I85" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C86" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D86">
-        <v>10.409000000000001</v>
+        <v>8.0050000000000008</v>
       </c>
       <c r="E86" s="12">
-        <v>0.55763888888888891</v>
+        <v>0.54027777777777775</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>49</v>
@@ -5760,22 +6048,25 @@
       <c r="I86" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
       </c>
       <c r="D87">
-        <v>10.176</v>
+        <v>6.7549999999999999</v>
       </c>
       <c r="E87" s="12">
-        <v>0.55763888888888891</v>
+        <v>0.55833333333333335</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>49</v>
@@ -5789,22 +6080,25 @@
       <c r="I87" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C88" t="s">
         <v>11</v>
       </c>
       <c r="D88">
-        <v>7.9450000000000003</v>
+        <v>7.6020000000000003</v>
       </c>
       <c r="E88" s="12">
-        <v>0.53819444444444442</v>
+        <v>0.54027777777777775</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>49</v>
@@ -5818,22 +6112,25 @@
       <c r="I88" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D89">
-        <v>8.0050000000000008</v>
+        <v>10.521000000000001</v>
       </c>
       <c r="E89" s="12">
-        <v>0.54027777777777775</v>
+        <v>0.55833333333333335</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>49</v>
@@ -5847,22 +6144,22 @@
       <c r="I89" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C90" t="s">
-        <v>5</v>
-      </c>
-      <c r="D90">
-        <v>6.7549999999999999</v>
+        <v>79</v>
       </c>
       <c r="E90" s="12">
-        <v>0.55833333333333335</v>
+        <v>0.54375000000000007</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>49</v>
@@ -5876,22 +6173,25 @@
       <c r="I90" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C91" t="s">
         <v>11</v>
       </c>
       <c r="D91">
-        <v>7.6020000000000003</v>
+        <v>8.3759999999999994</v>
       </c>
       <c r="E91" s="12">
-        <v>0.54027777777777775</v>
+        <v>0.53888888888888886</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>49</v>
@@ -5905,22 +6205,25 @@
       <c r="I91" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C92" t="s">
         <v>5</v>
       </c>
       <c r="D92">
-        <v>10.521000000000001</v>
+        <v>7.7797000000000001</v>
       </c>
       <c r="E92" s="12">
-        <v>0.55833333333333335</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>49</v>
@@ -5934,13 +6237,22 @@
       <c r="I92" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B93" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C93" t="s">
+        <v>79</v>
+      </c>
+      <c r="E93" s="12">
+        <v>0.54375000000000007</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>49</v>
@@ -5954,205 +6266,13 @@
       <c r="I93" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94">
-        <v>43</v>
-      </c>
-      <c r="B94" t="s">
-        <v>77</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="A95">
-        <v>44</v>
-      </c>
-      <c r="B95" t="s">
-        <v>77</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="A96">
-        <v>45</v>
-      </c>
-      <c r="B96" t="s">
-        <v>77</v>
-      </c>
-      <c r="C96" t="s">
-        <v>80</v>
-      </c>
-      <c r="E96" s="12">
-        <v>0.54375000000000007</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97">
-        <v>46</v>
-      </c>
-      <c r="B97" t="s">
-        <v>77</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98">
-        <v>47</v>
-      </c>
-      <c r="B98" t="s">
-        <v>77</v>
-      </c>
-      <c r="C98" t="s">
-        <v>11</v>
-      </c>
-      <c r="D98">
-        <v>8.3759999999999994</v>
-      </c>
-      <c r="E98" s="12">
-        <v>0.53888888888888886</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="A99">
-        <v>48</v>
-      </c>
-      <c r="B99" t="s">
-        <v>77</v>
-      </c>
-      <c r="C99" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99">
-        <v>7.7797000000000001</v>
-      </c>
-      <c r="E99" s="12">
-        <v>0.55902777777777779</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100">
-        <v>49</v>
-      </c>
-      <c r="B100" t="s">
-        <v>77</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101">
-        <v>50</v>
-      </c>
-      <c r="B101" t="s">
-        <v>77</v>
-      </c>
-      <c r="C101" t="s">
-        <v>80</v>
-      </c>
-      <c r="E101" s="12">
-        <v>0.54375000000000007</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>6</v>
+      <c r="J93">
+        <v>7000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6164,13 +6284,8 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating work sheet; day 20 cohort
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="400" windowWidth="21700" windowHeight="26900" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="400" windowWidth="21700" windowHeight="26900" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_collections" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10251" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10492" uniqueCount="161">
   <si>
     <t>Site</t>
   </si>
@@ -510,6 +510,9 @@
   <si>
     <t>do</t>
   </si>
+  <si>
+    <t>AN PE</t>
+  </si>
 </sst>
 </file>
 
@@ -602,8 +605,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="271">
+  <cellStyleXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -952,7 +961,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="271">
+  <cellStyles count="277">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1088,6 +1097,9 @@
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1223,6 +1235,9 @@
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1490,7 +1505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1501,10 +1516,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N128"/>
+  <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView showRuler="0" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="N108" sqref="N108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5764,6 +5779,12 @@
       <c r="G106" s="4">
         <v>1</v>
       </c>
+      <c r="H106" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I106" s="4">
+        <v>98</v>
+      </c>
       <c r="J106" s="15" t="s">
         <v>133</v>
       </c>
@@ -5794,25 +5815,31 @@
         <v>84</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F107" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G107" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I107" s="4">
+        <v>24</v>
       </c>
       <c r="J107" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="K107" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="K107" s="15" t="s">
-        <v>135</v>
-      </c>
       <c r="L107" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="M107" s="15" t="s">
         <v>138</v>
-      </c>
-      <c r="M107" s="15" t="s">
-        <v>139</v>
       </c>
       <c r="N107" s="14" t="s">
         <v>159</v>
@@ -5832,184 +5859,184 @@
         <v>84</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F108" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G108" s="4">
         <v>1</v>
       </c>
       <c r="J108" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="K108" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="K108" s="15" t="s">
-        <v>136</v>
-      </c>
       <c r="L108" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="M108" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="M108" s="15" t="s">
-        <v>140</v>
       </c>
       <c r="N108" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="109" spans="1:14" s="30" customFormat="1">
-      <c r="A109" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B109" s="30" t="s">
+    <row r="109" spans="1:14">
+      <c r="A109" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C109" s="30" t="s">
+      <c r="C109" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D109" s="31" t="s">
+      <c r="D109" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E109" s="32" t="s">
+      <c r="E109" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F109" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G109" s="4">
+        <v>1</v>
+      </c>
+      <c r="J109" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="K109" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="L109" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="M109" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="N109" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" s="30" customFormat="1">
+      <c r="A110" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E110" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F109" s="31" t="s">
+      <c r="F110" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="G109" s="33">
+      <c r="G110" s="33">
         <v>1</v>
       </c>
-      <c r="H109" s="33"/>
-      <c r="I109" s="33"/>
-      <c r="J109" s="31" t="s">
+      <c r="H110" s="33"/>
+      <c r="I110" s="33"/>
+      <c r="J110" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="K109" s="31" t="s">
+      <c r="K110" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="L109" s="31" t="s">
+      <c r="L110" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="M109" s="31" t="s">
+      <c r="M110" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="N109" s="30" t="s">
+      <c r="N110" s="30" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="110" spans="1:14">
-      <c r="A110" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B110" s="14" t="s">
+    <row r="111" spans="1:14">
+      <c r="A111" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C110" s="14" t="s">
+      <c r="C111" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D110" s="15" t="s">
+      <c r="D111" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E110" s="7" t="s">
+      <c r="E111" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F110" s="15" t="s">
+      <c r="F111" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G110" s="4">
+      <c r="G111" s="4">
         <v>1</v>
       </c>
-      <c r="J110" s="15" t="s">
+      <c r="J111" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="K110" s="15" t="s">
+      <c r="K111" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="L110" s="15" t="s">
+      <c r="L111" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="M110" s="15" t="s">
+      <c r="M111" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="N110" s="14" t="s">
+      <c r="N111" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="111" spans="1:14" s="12" customFormat="1">
-      <c r="A111" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B111" s="12" t="s">
+    <row r="112" spans="1:14" s="12" customFormat="1">
+      <c r="A112" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C111" s="12" t="s">
+      <c r="C112" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D111" s="13" t="s">
+      <c r="D112" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E111" s="6" t="s">
+      <c r="E112" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F111" s="13" t="s">
+      <c r="F112" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="G111" s="3">
+      <c r="G112" s="3">
         <v>1</v>
       </c>
-      <c r="H111" s="3"/>
-      <c r="I111" s="3"/>
-      <c r="J111" s="13" t="s">
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="K111" s="13" t="s">
+      <c r="K112" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="L111" s="13" t="s">
+      <c r="L112" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="M111" s="13" t="s">
+      <c r="M112" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="N111" s="12" t="s">
+      <c r="N112" s="12" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14">
-      <c r="A112" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B112" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D112" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E112" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F112" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="G112" s="4">
-        <v>1</v>
-      </c>
-      <c r="J112" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="K112" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="L112" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="M112" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="N112" s="14" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="113" spans="1:14">
@@ -6026,103 +6053,106 @@
         <v>84</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F113" s="15" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="G113" s="4">
         <v>1</v>
       </c>
       <c r="J113" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="K113" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="K113" s="15" t="s">
+      <c r="L113" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="M113" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="N113" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="A114" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F114" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G114" s="4">
+        <v>1</v>
+      </c>
+      <c r="J114" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="K114" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="L113" s="15" t="s">
+      <c r="L114" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="M113" s="15" t="s">
+      <c r="M114" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="N113" s="14" t="s">
+      <c r="N114" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="114" spans="1:14" s="12" customFormat="1">
-      <c r="A114" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B114" s="12" t="s">
+    <row r="115" spans="1:14" s="12" customFormat="1">
+      <c r="A115" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C114" s="12" t="s">
+      <c r="C115" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D114" s="13" t="s">
+      <c r="D115" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E114" s="6" t="s">
+      <c r="E115" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F114" s="13" t="s">
+      <c r="F115" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="G114" s="3">
+      <c r="G115" s="3">
         <v>1</v>
       </c>
-      <c r="H114" s="3"/>
-      <c r="I114" s="3"/>
-      <c r="J114" s="13" t="s">
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
+      <c r="J115" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="K114" s="13" t="s">
+      <c r="K115" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="L114" s="13" t="s">
+      <c r="L115" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="M114" s="13" t="s">
+      <c r="M115" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="N114" s="12" t="s">
+      <c r="N115" s="12" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14">
-      <c r="A115" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B115" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D115" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E115" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F115" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="G115" s="4">
-        <v>1</v>
-      </c>
-      <c r="J115" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="K115" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="L115" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="M115" s="15" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:14">
@@ -6139,25 +6169,25 @@
         <v>84</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F116" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G116" s="4">
         <v>1</v>
       </c>
       <c r="J116" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="K116" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="K116" s="15" t="s">
-        <v>144</v>
-      </c>
       <c r="L116" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="M116" s="15" t="s">
         <v>147</v>
-      </c>
-      <c r="M116" s="15" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="117" spans="1:14">
@@ -6174,25 +6204,25 @@
         <v>84</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="F117" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G117" s="4">
         <v>1</v>
       </c>
       <c r="J117" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="K117" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="K117" s="15" t="s">
-        <v>145</v>
-      </c>
       <c r="L117" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="M117" s="15" t="s">
         <v>148</v>
-      </c>
-      <c r="M117" s="15" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="118" spans="1:14">
@@ -6209,26 +6239,25 @@
         <v>84</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F118" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G118" s="4">
         <v>1</v>
       </c>
-      <c r="I118" s="7"/>
       <c r="J118" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="K118" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="K118" s="15" t="s">
-        <v>146</v>
-      </c>
       <c r="L118" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="M118" s="15" t="s">
         <v>149</v>
-      </c>
-      <c r="M118" s="15" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="119" spans="1:14">
@@ -6245,25 +6274,26 @@
         <v>84</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F119" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G119" s="4">
         <v>1</v>
       </c>
+      <c r="I119" s="7"/>
       <c r="J119" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="K119" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="K119" s="15" t="s">
-        <v>147</v>
-      </c>
       <c r="L119" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="M119" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="M119" s="15" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="120" spans="1:14">
@@ -6280,25 +6310,25 @@
         <v>84</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F120" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G120" s="4">
         <v>1</v>
       </c>
       <c r="J120" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="K120" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="K120" s="15" t="s">
-        <v>148</v>
-      </c>
       <c r="L120" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="M120" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="M120" s="15" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="121" spans="1:14">
@@ -6315,25 +6345,25 @@
         <v>84</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F121" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G121" s="4">
         <v>1</v>
       </c>
       <c r="J121" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="K121" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="K121" s="15" t="s">
-        <v>149</v>
-      </c>
       <c r="L121" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="M121" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="M121" s="15" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="122" spans="1:14">
@@ -6350,25 +6380,25 @@
         <v>84</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F122" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G122" s="4">
         <v>1</v>
       </c>
       <c r="J122" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="K122" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="K122" s="15" t="s">
-        <v>150</v>
-      </c>
       <c r="L122" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="M122" s="15" t="s">
         <v>153</v>
-      </c>
-      <c r="M122" s="15" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="123" spans="1:14">
@@ -6385,25 +6415,25 @@
         <v>84</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F123" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G123" s="4">
         <v>1</v>
       </c>
       <c r="J123" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="K123" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="K123" s="15" t="s">
-        <v>151</v>
-      </c>
       <c r="L123" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="M123" s="15" t="s">
         <v>154</v>
-      </c>
-      <c r="M123" s="15" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="124" spans="1:14">
@@ -6420,25 +6450,25 @@
         <v>84</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F124" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G124" s="4">
         <v>1</v>
       </c>
       <c r="J124" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="K124" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="K124" s="15" t="s">
-        <v>152</v>
-      </c>
       <c r="L124" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="M124" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="M124" s="15" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="125" spans="1:14">
@@ -6455,37 +6485,72 @@
         <v>84</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F125" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G125" s="4">
         <v>1</v>
       </c>
       <c r="J125" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="K125" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="K125" s="15" t="s">
+      <c r="L125" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="M125" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14">
+      <c r="A126" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F126" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G126" s="4">
+        <v>1</v>
+      </c>
+      <c r="J126" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="K126" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="L125" s="15" t="s">
+      <c r="L126" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="M125" s="15" t="s">
+      <c r="M126" s="15" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="127" spans="1:14">
-      <c r="I127" s="4">
-        <f>SUM(I2:I125)</f>
-        <v>3209</v>
       </c>
     </row>
     <row r="128" spans="1:14">
       <c r="I128" s="4">
-        <f>I127*0.8</f>
-        <v>2567.2000000000003</v>
+        <f>SUM(I2:I126)</f>
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="129" spans="9:9">
+      <c r="I129" s="4">
+        <f>I128*0.8</f>
+        <v>2664.8</v>
       </c>
     </row>
   </sheetData>
@@ -6502,11 +6567,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1479"/>
+  <dimension ref="A1:S1517"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K828" sqref="K828"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1467" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1516" sqref="D1516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -53516,6 +53581,994 @@
         <v>93</v>
       </c>
       <c r="I1479" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:9">
+      <c r="A1480">
+        <v>1</v>
+      </c>
+      <c r="B1480" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1480" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1480">
+        <v>2.93</v>
+      </c>
+      <c r="E1480" s="8">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="F1480" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1480" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1480" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1480" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:9">
+      <c r="A1481">
+        <v>2</v>
+      </c>
+      <c r="B1481" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1481" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1481">
+        <v>6.0590000000000002</v>
+      </c>
+      <c r="F1481" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1481" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1481" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1481" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:9">
+      <c r="A1482">
+        <v>3</v>
+      </c>
+      <c r="B1482" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1482" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1482">
+        <v>5.593</v>
+      </c>
+      <c r="F1482" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1482" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1482" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1482" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:9">
+      <c r="A1483">
+        <v>4</v>
+      </c>
+      <c r="B1483" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1483" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1483">
+        <v>4.95</v>
+      </c>
+      <c r="F1483" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1483" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1483" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1483" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:9">
+      <c r="A1484">
+        <v>5</v>
+      </c>
+      <c r="B1484" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1484" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1484">
+        <v>5.8959999999999999</v>
+      </c>
+      <c r="F1484" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1484" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1484" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1484" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:9">
+      <c r="A1485">
+        <v>6</v>
+      </c>
+      <c r="B1485" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1485" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1485">
+        <v>6.4450000000000003</v>
+      </c>
+      <c r="F1485" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1485" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1485" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1485" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:9">
+      <c r="A1486">
+        <v>7</v>
+      </c>
+      <c r="B1486" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1486" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1486">
+        <v>6.0190000000000001</v>
+      </c>
+      <c r="F1486" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1486" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1486" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1486" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:9">
+      <c r="A1487">
+        <v>8</v>
+      </c>
+      <c r="B1487" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1487" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1487">
+        <v>8.68</v>
+      </c>
+      <c r="F1487" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1487" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1487" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1487" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:9">
+      <c r="A1488">
+        <v>9</v>
+      </c>
+      <c r="B1488" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1488" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1488">
+        <v>7.3140000000000001</v>
+      </c>
+      <c r="F1488" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1488" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1488" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1488" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:9">
+      <c r="A1489">
+        <v>10</v>
+      </c>
+      <c r="B1489" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1489" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1489">
+        <v>7.74</v>
+      </c>
+      <c r="F1489" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1489" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1489" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1489" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:9">
+      <c r="A1490">
+        <v>11</v>
+      </c>
+      <c r="B1490" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1490" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1490">
+        <v>8.782</v>
+      </c>
+      <c r="F1490" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1490" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1490" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1490" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:9">
+      <c r="A1491">
+        <v>12</v>
+      </c>
+      <c r="B1491" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1491" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1491">
+        <v>6.7069999999999999</v>
+      </c>
+      <c r="F1491" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1491" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1491" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1491" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:9">
+      <c r="A1492">
+        <v>13</v>
+      </c>
+      <c r="B1492" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1492" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1492">
+        <v>4.7539999999999996</v>
+      </c>
+      <c r="F1492" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1492" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1492" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1492" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:9">
+      <c r="A1493">
+        <v>14</v>
+      </c>
+      <c r="B1493" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1493" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1493">
+        <v>8.11</v>
+      </c>
+      <c r="F1493" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1493" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1493" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1493" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:9">
+      <c r="A1494">
+        <v>15</v>
+      </c>
+      <c r="B1494" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1494" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1494">
+        <v>7.03</v>
+      </c>
+      <c r="F1494" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1494" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1494" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1494" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:9">
+      <c r="A1495">
+        <v>16</v>
+      </c>
+      <c r="B1495" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1495" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1495">
+        <v>7.8979999999999997</v>
+      </c>
+      <c r="F1495" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1495" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1495" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1495" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:9">
+      <c r="A1496">
+        <v>17</v>
+      </c>
+      <c r="B1496" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1496" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1496">
+        <v>5.84</v>
+      </c>
+      <c r="F1496" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1496" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1496" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1496" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:9">
+      <c r="A1497">
+        <v>18</v>
+      </c>
+      <c r="B1497" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1497" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1497" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1497" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1497" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1497" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:9">
+      <c r="A1498">
+        <v>19</v>
+      </c>
+      <c r="B1498" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1498" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1498" s="8">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="F1498" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1498" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1498" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1498" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:9">
+      <c r="A1499">
+        <v>1</v>
+      </c>
+      <c r="B1499" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1499" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1499">
+        <v>7.7919999999999998</v>
+      </c>
+      <c r="E1499" s="8">
+        <v>0.62083333333333335</v>
+      </c>
+      <c r="F1499" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1499" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1499" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1499" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:9">
+      <c r="A1500">
+        <v>2</v>
+      </c>
+      <c r="B1500" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1500" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1500">
+        <v>7.8789999999999996</v>
+      </c>
+      <c r="F1500" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1500" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1500" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1500" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:9">
+      <c r="A1501">
+        <v>3</v>
+      </c>
+      <c r="B1501" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1501" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1501">
+        <v>5.0970000000000004</v>
+      </c>
+      <c r="F1501" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1501" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1501" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1501" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:9">
+      <c r="A1502">
+        <v>4</v>
+      </c>
+      <c r="B1502" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1502" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1502">
+        <v>9.3740000000000006</v>
+      </c>
+      <c r="F1502" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1502" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1502" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1502" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:9">
+      <c r="A1503">
+        <v>5</v>
+      </c>
+      <c r="B1503" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1503" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1503">
+        <v>6.6920000000000002</v>
+      </c>
+      <c r="F1503" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1503" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1503" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1503" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:9">
+      <c r="A1504">
+        <v>6</v>
+      </c>
+      <c r="B1504" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1504" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1504">
+        <v>8.8610000000000007</v>
+      </c>
+      <c r="F1504" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1504" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1504" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1504" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:9">
+      <c r="A1505">
+        <v>7</v>
+      </c>
+      <c r="B1505" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1505" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1505">
+        <v>7.9039999999999999</v>
+      </c>
+      <c r="F1505" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1505" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1505" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1505" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:9">
+      <c r="A1506">
+        <v>8</v>
+      </c>
+      <c r="B1506" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1506" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1506">
+        <v>9.5020000000000007</v>
+      </c>
+      <c r="F1506" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1506" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1506" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1506" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:9">
+      <c r="A1507">
+        <v>9</v>
+      </c>
+      <c r="B1507" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1507" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1507">
+        <v>6.6340000000000003</v>
+      </c>
+      <c r="F1507" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1507" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1507" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1507" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:9">
+      <c r="A1508">
+        <v>10</v>
+      </c>
+      <c r="B1508" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1508" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1508">
+        <v>7.07</v>
+      </c>
+      <c r="F1508" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1508" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1508" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1508" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:9">
+      <c r="A1509">
+        <v>11</v>
+      </c>
+      <c r="B1509" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1509" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1509">
+        <v>6.8460000000000001</v>
+      </c>
+      <c r="F1509" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1509" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1509" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1509" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:9">
+      <c r="A1510">
+        <v>12</v>
+      </c>
+      <c r="B1510" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1510" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1510">
+        <v>8.2949999999999999</v>
+      </c>
+      <c r="F1510" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1510" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1510" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1510" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:9">
+      <c r="A1511">
+        <v>13</v>
+      </c>
+      <c r="B1511" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1511" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1511">
+        <v>10.631</v>
+      </c>
+      <c r="F1511" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1511" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1511" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1511" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:9">
+      <c r="A1512">
+        <v>14</v>
+      </c>
+      <c r="B1512" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1512" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1512">
+        <v>7.5449999999999999</v>
+      </c>
+      <c r="F1512" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1512" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1512" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1512" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:9">
+      <c r="A1513">
+        <v>15</v>
+      </c>
+      <c r="B1513" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1513" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1513">
+        <v>2.4929999999999999</v>
+      </c>
+      <c r="F1513" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1513" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1513" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1513" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:9">
+      <c r="A1514">
+        <v>16</v>
+      </c>
+      <c r="B1514" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1514" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1514">
+        <v>5.28</v>
+      </c>
+      <c r="F1514" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1514" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1514" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1514" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:9">
+      <c r="A1515">
+        <v>17</v>
+      </c>
+      <c r="B1515" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1515" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1515">
+        <v>6.4160000000000004</v>
+      </c>
+      <c r="F1515" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1515" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1515" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1515" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:9">
+      <c r="A1516">
+        <v>18</v>
+      </c>
+      <c r="B1516" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1516" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1516" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1516" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1516" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1516" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:9">
+      <c r="A1517">
+        <v>19</v>
+      </c>
+      <c r="B1517" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1517" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1517" s="8">
+        <v>0.63472222222222219</v>
+      </c>
+      <c r="F1517" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1517" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1517" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1517" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding how many haw flies i collected
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="0" windowWidth="31320" windowHeight="27900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="31320" windowHeight="27900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_collections" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10433" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10435" uniqueCount="162">
   <si>
     <t>Site</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>AN PE</t>
+  </si>
+  <si>
+    <t>AN CH</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1693,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1703,8 +1706,8 @@
   </sheetPr>
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118:XFD118"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6052,6 +6055,12 @@
       <c r="G108" s="4">
         <v>1</v>
       </c>
+      <c r="H108" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I108" s="4">
+        <v>68</v>
+      </c>
       <c r="J108" s="15" t="s">
         <v>134</v>
       </c>
@@ -6089,6 +6098,12 @@
       </c>
       <c r="G109" s="4">
         <v>1</v>
+      </c>
+      <c r="H109" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I109" s="4">
+        <v>55</v>
       </c>
       <c r="J109" s="15" t="s">
         <v>135</v>
@@ -6741,13 +6756,13 @@
     <row r="128" spans="1:14">
       <c r="I128" s="4">
         <f>SUM(I2:I126)</f>
-        <v>3331</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="129" spans="9:9">
       <c r="I129" s="4">
         <f>I128*0.8</f>
-        <v>2664.8</v>
+        <v>2763.2000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -6766,7 +6781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1505"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1452" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T1510" sqref="T1510"/>
     </sheetView>

</xml_diff>

<commit_message>
adding day 18 cohort resp data
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="0" windowWidth="31320" windowHeight="27900" tabRatio="500"/>
+    <workbookView xWindow="1500" yWindow="0" windowWidth="31320" windowHeight="27900" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_collections" sheetId="1" r:id="rId1"/>
@@ -1693,7 +1693,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1706,8 +1706,8 @@
   </sheetPr>
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView showRuler="0" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="N117" sqref="A106:N117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6781,9 +6781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1505"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1452" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1510" sqref="T1510"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1464" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1507" sqref="L1507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
restructuring master data sheet
adding columns for exclosion date and data
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10435" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10447" uniqueCount="171">
   <si>
     <t>Site</t>
   </si>
@@ -513,6 +513,36 @@
   <si>
     <t>AN CH</t>
   </si>
+  <si>
+    <t>eclosion_date</t>
+  </si>
+  <si>
+    <t>eclosion_days</t>
+  </si>
+  <si>
+    <t>well_id</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>organism</t>
+  </si>
+  <si>
+    <t>wasp</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>fly</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
 </sst>
 </file>
 
@@ -604,7 +634,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="373">
+  <cellStyleXfs count="375">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -978,8 +1008,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1069,8 +1101,9 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="373">
+  <cellStyles count="375">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1257,6 +1290,7 @@
     <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1443,6 +1477,7 @@
     <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1710,7 +1745,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6796,11 +6831,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1505"/>
+  <dimension ref="A1:V1505"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T86" sqref="T86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6812,7 +6847,7 @@
     <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -6867,9 +6902,20 @@
       <c r="R1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="S1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6913,7 +6959,7 @@
         <v>0.1432514</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6960,7 +7006,7 @@
         <v>0.170235</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7007,7 +7053,7 @@
         <v>0.1076286</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7054,7 +7100,7 @@
         <v>1.3873899999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7101,7 +7147,7 @@
         <v>0.1182286</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7148,7 +7194,7 @@
         <v>1.468912</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7195,7 +7241,7 @@
         <v>0.16016230000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7242,7 +7288,7 @@
         <v>1.4328829999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:22">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7289,7 +7335,7 @@
         <v>8.09E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:22">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7336,7 +7382,7 @@
         <v>6.4199999999999993E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:22">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7383,7 +7429,7 @@
         <v>1.2453730000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7433,7 +7479,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>13</v>
       </c>
@@ -7480,7 +7526,7 @@
         <v>7.4800000000000005E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>14</v>
       </c>
@@ -7527,7 +7573,7 @@
         <v>0.1269034</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:22">
       <c r="A16">
         <v>15</v>
       </c>
@@ -8327,7 +8373,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:22">
       <c r="A33">
         <v>33</v>
       </c>
@@ -8374,7 +8420,7 @@
         <v>0.2100458</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:22">
       <c r="A34">
         <v>34</v>
       </c>
@@ -8421,7 +8467,7 @@
         <v>0.1083471</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:22">
       <c r="A35">
         <v>35</v>
       </c>
@@ -8468,7 +8514,7 @@
         <v>7.8299999999999995E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:22">
       <c r="A36">
         <v>36</v>
       </c>
@@ -8515,7 +8561,7 @@
         <v>0.26179160000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:22">
       <c r="A37">
         <v>37</v>
       </c>
@@ -8562,7 +8608,7 @@
         <v>0.1402832</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:22">
       <c r="A38">
         <v>38</v>
       </c>
@@ -8609,7 +8655,7 @@
         <v>1.8140689999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:22">
       <c r="A39">
         <v>39</v>
       </c>
@@ -8655,8 +8701,20 @@
       <c r="P39">
         <v>0.1573756</v>
       </c>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="S39" s="49">
+        <v>42972</v>
+      </c>
+      <c r="T39">
+        <v>31</v>
+      </c>
+      <c r="U39" t="s">
+        <v>167</v>
+      </c>
+      <c r="V39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40">
         <v>40</v>
       </c>
@@ -8703,7 +8761,7 @@
         <v>9.3366500000000005E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:22">
       <c r="A41">
         <v>41</v>
       </c>
@@ -8750,7 +8808,7 @@
         <v>1.039968</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:22">
       <c r="A42">
         <v>42</v>
       </c>
@@ -8797,7 +8855,7 @@
         <v>1.333105</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:22">
       <c r="A43">
         <v>43</v>
       </c>
@@ -8844,7 +8902,7 @@
         <v>0.92131940000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:22">
       <c r="A44">
         <v>44</v>
       </c>
@@ -8892,7 +8950,7 @@
       </c>
       <c r="Q44" s="17"/>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:22">
       <c r="A45">
         <v>45</v>
       </c>
@@ -8933,7 +8991,7 @@
         <v>1.5932200000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:22">
       <c r="A46">
         <v>46</v>
       </c>
@@ -8980,7 +9038,7 @@
         <v>0.19791529999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:22">
       <c r="A47">
         <v>47</v>
       </c>
@@ -9027,7 +9085,7 @@
         <v>0.22923370000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:22">
       <c r="A48">
         <v>48</v>
       </c>
@@ -10585,7 +10643,7 @@
         <v>0.76695579999999997</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:22">
       <c r="A81">
         <v>33</v>
       </c>
@@ -10632,7 +10690,7 @@
         <v>0.72409270000000003</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:22">
       <c r="A82">
         <v>34</v>
       </c>
@@ -10679,7 +10737,7 @@
         <v>0.1596853</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:22">
       <c r="A83">
         <v>35</v>
       </c>
@@ -10727,7 +10785,7 @@
       </c>
       <c r="Q83" s="17"/>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:22">
       <c r="A84">
         <v>36</v>
       </c>
@@ -10775,7 +10833,7 @@
       </c>
       <c r="Q84" s="17"/>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:22">
       <c r="A85">
         <v>37</v>
       </c>
@@ -10822,7 +10880,7 @@
         <v>0.28472120000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:22">
       <c r="A86">
         <v>38</v>
       </c>
@@ -10868,8 +10926,20 @@
       <c r="P86">
         <v>0.81230939999999996</v>
       </c>
-    </row>
-    <row r="87" spans="1:18">
+      <c r="S86" s="49">
+        <v>42972</v>
+      </c>
+      <c r="T86">
+        <v>31</v>
+      </c>
+      <c r="U86" t="s">
+        <v>170</v>
+      </c>
+      <c r="V86" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22">
       <c r="A87">
         <v>39</v>
       </c>
@@ -10916,7 +10986,7 @@
         <v>0.224742</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:22">
       <c r="A88">
         <v>40</v>
       </c>
@@ -10963,7 +11033,7 @@
         <v>0.1253869</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:22">
       <c r="A89">
         <v>41</v>
       </c>
@@ -11011,7 +11081,7 @@
       </c>
       <c r="Q89" s="17"/>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:22">
       <c r="A90">
         <v>45</v>
       </c>
@@ -11053,7 +11123,7 @@
       </c>
       <c r="Q90" s="17"/>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:22">
       <c r="A91">
         <v>47</v>
       </c>
@@ -11097,7 +11167,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:22">
       <c r="A92">
         <v>48</v>
       </c>
@@ -11145,7 +11215,7 @@
       </c>
       <c r="Q92" s="17"/>
     </row>
-    <row r="93" spans="1:18" s="37" customFormat="1">
+    <row r="93" spans="1:22" s="37" customFormat="1">
       <c r="A93" s="37">
         <v>50</v>
       </c>
@@ -11190,7 +11260,7 @@
       </c>
       <c r="Q93" s="41"/>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:22">
       <c r="A94">
         <v>1</v>
       </c>
@@ -11240,7 +11310,7 @@
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:22">
       <c r="A95">
         <v>2</v>
       </c>
@@ -11287,7 +11357,7 @@
         <v>3.4500000000000003E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:22">
       <c r="A96">
         <v>3</v>
       </c>
@@ -15098,7 +15168,7 @@
         <v>0.14033519999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:22">
       <c r="A177">
         <v>24</v>
       </c>
@@ -15145,7 +15215,7 @@
         <v>0.11753570000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:22">
       <c r="A178">
         <v>25</v>
       </c>
@@ -15192,7 +15262,7 @@
         <v>0.54109660000000004</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:22">
       <c r="A179">
         <v>26</v>
       </c>
@@ -15239,7 +15309,7 @@
         <v>0.39865810000000002</v>
       </c>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:22">
       <c r="A180">
         <v>27</v>
       </c>
@@ -15286,7 +15356,7 @@
         <v>0.17276520000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:22">
       <c r="A181">
         <v>28</v>
       </c>
@@ -15333,7 +15403,7 @@
         <v>0.79337570000000002</v>
       </c>
     </row>
-    <row r="182" spans="1:16">
+    <row r="182" spans="1:22">
       <c r="A182">
         <v>29</v>
       </c>
@@ -15380,7 +15450,7 @@
         <v>1.2377830000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:16">
+    <row r="183" spans="1:22">
       <c r="A183">
         <v>30</v>
       </c>
@@ -15427,7 +15497,7 @@
         <v>0.62263950000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:22">
       <c r="A184">
         <v>31</v>
       </c>
@@ -15474,7 +15544,7 @@
         <v>0.2313992</v>
       </c>
     </row>
-    <row r="185" spans="1:16">
+    <row r="185" spans="1:22">
       <c r="A185">
         <v>32</v>
       </c>
@@ -15521,7 +15591,7 @@
         <v>0.15950030000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:16">
+    <row r="186" spans="1:22">
       <c r="A186">
         <v>33</v>
       </c>
@@ -15568,7 +15638,7 @@
         <v>0.69007909999999995</v>
       </c>
     </row>
-    <row r="187" spans="1:16">
+    <row r="187" spans="1:22">
       <c r="A187">
         <v>34</v>
       </c>
@@ -15615,7 +15685,7 @@
         <v>8.7560299999999994E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:16">
+    <row r="188" spans="1:22">
       <c r="A188">
         <v>35</v>
       </c>
@@ -15661,8 +15731,20 @@
       <c r="P188">
         <v>0.88073170000000001</v>
       </c>
-    </row>
-    <row r="189" spans="1:16">
+      <c r="S188" s="49">
+        <v>43003</v>
+      </c>
+      <c r="T188">
+        <v>30</v>
+      </c>
+      <c r="U188" t="s">
+        <v>164</v>
+      </c>
+      <c r="V188" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="189" spans="1:22">
       <c r="A189">
         <v>36</v>
       </c>
@@ -15709,7 +15791,7 @@
         <v>1.330835</v>
       </c>
     </row>
-    <row r="190" spans="1:16">
+    <row r="190" spans="1:22">
       <c r="A190">
         <v>37</v>
       </c>
@@ -15756,7 +15838,7 @@
         <v>0.92665640000000005</v>
       </c>
     </row>
-    <row r="191" spans="1:16">
+    <row r="191" spans="1:22">
       <c r="A191">
         <v>38</v>
       </c>
@@ -15803,7 +15885,7 @@
         <v>0.1380371</v>
       </c>
     </row>
-    <row r="192" spans="1:16">
+    <row r="192" spans="1:22">
       <c r="A192">
         <v>39</v>
       </c>
@@ -18717,7 +18799,7 @@
         <v>9.6199999999999994E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:18">
+    <row r="257" spans="1:22">
       <c r="A257">
         <v>45</v>
       </c>
@@ -18761,7 +18843,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:18">
+    <row r="258" spans="1:22">
       <c r="A258">
         <v>46</v>
       </c>
@@ -18805,7 +18887,7 @@
         <v>9.6600000000000005E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:18">
+    <row r="259" spans="1:22">
       <c r="A259">
         <v>47</v>
       </c>
@@ -18845,7 +18927,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="260" spans="1:18">
+    <row r="260" spans="1:22">
       <c r="A260">
         <v>48</v>
       </c>
@@ -18889,7 +18971,7 @@
         <v>0.12652169999999999</v>
       </c>
     </row>
-    <row r="261" spans="1:18">
+    <row r="261" spans="1:22">
       <c r="A261">
         <v>49</v>
       </c>
@@ -18933,7 +19015,7 @@
         <v>6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:18">
+    <row r="262" spans="1:22">
       <c r="A262">
         <v>50</v>
       </c>
@@ -18977,7 +19059,7 @@
         <v>7.7310500000000004E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:18">
+    <row r="263" spans="1:22">
       <c r="A263">
         <v>51</v>
       </c>
@@ -19021,7 +19103,7 @@
         <v>0.57230990000000004</v>
       </c>
     </row>
-    <row r="264" spans="1:18">
+    <row r="264" spans="1:22">
       <c r="A264">
         <v>52</v>
       </c>
@@ -19065,7 +19147,7 @@
         <v>8.6300000000000002E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:18">
+    <row r="265" spans="1:22">
       <c r="A265">
         <v>53</v>
       </c>
@@ -19109,7 +19191,7 @@
         <v>1.0067029999999999</v>
       </c>
     </row>
-    <row r="266" spans="1:18">
+    <row r="266" spans="1:22">
       <c r="A266">
         <v>54</v>
       </c>
@@ -19153,7 +19235,7 @@
         <v>0.2008924</v>
       </c>
     </row>
-    <row r="267" spans="1:18">
+    <row r="267" spans="1:22">
       <c r="A267">
         <v>55</v>
       </c>
@@ -19197,7 +19279,7 @@
         <v>7.6200000000000004E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:18">
+    <row r="268" spans="1:22">
       <c r="A268">
         <v>56</v>
       </c>
@@ -19241,7 +19323,7 @@
         <v>8.3699999999999997E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:18">
+    <row r="269" spans="1:22">
       <c r="A269">
         <v>57</v>
       </c>
@@ -19285,7 +19367,7 @@
         <v>0.1177217</v>
       </c>
     </row>
-    <row r="270" spans="1:18">
+    <row r="270" spans="1:22">
       <c r="A270">
         <v>58</v>
       </c>
@@ -19329,7 +19411,7 @@
         <v>1.110716</v>
       </c>
     </row>
-    <row r="271" spans="1:18">
+    <row r="271" spans="1:22">
       <c r="A271">
         <v>59</v>
       </c>
@@ -19373,7 +19455,7 @@
         <v>8.7900000000000006E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:18">
+    <row r="272" spans="1:22">
       <c r="A272">
         <v>60</v>
       </c>
@@ -19415,6 +19497,18 @@
       </c>
       <c r="P272">
         <v>1.0483279999999999</v>
+      </c>
+      <c r="S272" s="49">
+        <v>43003</v>
+      </c>
+      <c r="T272">
+        <v>29</v>
+      </c>
+      <c r="U272" t="s">
+        <v>169</v>
+      </c>
+      <c r="V272" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="273" spans="1:18">

</xml_diff>

<commit_message>
mass data for cohort 2-4 haws
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12939" uniqueCount="1745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13292" uniqueCount="1749">
   <si>
     <t>Site</t>
   </si>
@@ -5265,6 +5265,18 @@
   </si>
   <si>
     <t>no 62?</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>dirty syringe</t>
   </si>
 </sst>
 </file>
@@ -5363,8 +5375,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="433">
+  <cellStyleXfs count="447">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5925,7 +5951,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="433">
+  <cellStyles count="447">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6142,6 +6168,13 @@
     <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6358,6 +6391,13 @@
     <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6625,7 +6665,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6639,7 +6679,7 @@
   <dimension ref="A1:N129"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+      <selection activeCell="I111" sqref="I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10836,7 +10876,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="1:14" s="23" customFormat="1" ht="17" thickBot="1">
+    <row r="105" spans="1:14" s="23" customFormat="1" ht="16" thickBot="1">
       <c r="A105" s="23" t="s">
         <v>12</v>
       </c>
@@ -11756,11 +11796,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE1631"/>
+  <dimension ref="A1:AE1684"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1613" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1631" sqref="D1631"/>
+      <pane ySplit="1" topLeftCell="A1649" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1684" sqref="I1684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11781,7 +11821,8 @@
     <col min="23" max="23" width="12.5" style="4" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="10.83203125" style="4"/>
     <col min="26" max="26" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="10.83203125" style="4"/>
+    <col min="27" max="27" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
@@ -12309,6 +12350,12 @@
       <c r="AB9" s="53">
         <v>0.67222222222222217</v>
       </c>
+      <c r="AC9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD9" s="53">
+        <v>0.53125</v>
+      </c>
     </row>
     <row r="10" spans="1:31">
       <c r="A10">
@@ -13735,8 +13782,32 @@
       <c r="Q36">
         <v>0.26179160000000001</v>
       </c>
+      <c r="T36" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="U36" s="4" t="s">
         <v>236</v>
+      </c>
+      <c r="V36" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W36" s="4">
+        <v>42</v>
+      </c>
+      <c r="X36" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="Y36" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z36" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA36" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="53">
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="37" spans="1:28">
@@ -29411,7 +29482,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="337" spans="1:21">
+    <row r="337" spans="1:30">
       <c r="A337">
         <v>47</v>
       </c>
@@ -29461,7 +29532,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="338" spans="1:21">
+    <row r="338" spans="1:30">
       <c r="A338">
         <v>48</v>
       </c>
@@ -29511,7 +29582,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="339" spans="1:21">
+    <row r="339" spans="1:30">
       <c r="A339">
         <v>49</v>
       </c>
@@ -29561,7 +29632,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="340" spans="1:21">
+    <row r="340" spans="1:30">
       <c r="A340">
         <v>50</v>
       </c>
@@ -29611,7 +29682,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="341" spans="1:21">
+    <row r="341" spans="1:30">
       <c r="A341">
         <v>51</v>
       </c>
@@ -29657,11 +29728,39 @@
       <c r="Q341">
         <v>1.5705720000000001</v>
       </c>
+      <c r="T341" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="U341" s="4" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="342" spans="1:21">
+      <c r="V341" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="W341" s="7">
+        <f>V341-H341</f>
+        <v>34</v>
+      </c>
+      <c r="X341" s="4" t="s">
+        <v>1747</v>
+      </c>
+      <c r="Y341" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z341" s="4">
+        <v>21</v>
+      </c>
+      <c r="AA341" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC341" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD341" s="53">
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="342" spans="1:30">
       <c r="A342">
         <v>52</v>
       </c>
@@ -29711,7 +29810,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="343" spans="1:21">
+    <row r="343" spans="1:30">
       <c r="A343">
         <v>53</v>
       </c>
@@ -29761,7 +29860,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="344" spans="1:21">
+    <row r="344" spans="1:30">
       <c r="A344">
         <v>54</v>
       </c>
@@ -29811,7 +29910,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="345" spans="1:21">
+    <row r="345" spans="1:30">
       <c r="A345">
         <v>55</v>
       </c>
@@ -29861,7 +29960,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="346" spans="1:21">
+    <row r="346" spans="1:30">
       <c r="A346">
         <v>56</v>
       </c>
@@ -29911,7 +30010,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="347" spans="1:21">
+    <row r="347" spans="1:30">
       <c r="A347">
         <v>57</v>
       </c>
@@ -29961,7 +30060,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="348" spans="1:21">
+    <row r="348" spans="1:30">
       <c r="A348">
         <v>58</v>
       </c>
@@ -30011,7 +30110,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="349" spans="1:21">
+    <row r="349" spans="1:30">
       <c r="A349">
         <v>59</v>
       </c>
@@ -30061,7 +30160,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="350" spans="1:21">
+    <row r="350" spans="1:30">
       <c r="A350">
         <v>60</v>
       </c>
@@ -30111,7 +30210,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="351" spans="1:21">
+    <row r="351" spans="1:30">
       <c r="A351">
         <v>61</v>
       </c>
@@ -30161,7 +30260,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="352" spans="1:21">
+    <row r="352" spans="1:30">
       <c r="A352">
         <v>62</v>
       </c>
@@ -47023,7 +47122,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="753" spans="1:21">
+    <row r="753" spans="1:28">
       <c r="A753">
         <v>6</v>
       </c>
@@ -47067,7 +47166,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="754" spans="1:21">
+    <row r="754" spans="1:28">
       <c r="A754">
         <v>7</v>
       </c>
@@ -47111,7 +47210,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="755" spans="1:21">
+    <row r="755" spans="1:28">
       <c r="A755">
         <v>8</v>
       </c>
@@ -47155,7 +47254,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="756" spans="1:21">
+    <row r="756" spans="1:28">
       <c r="A756">
         <v>9</v>
       </c>
@@ -47199,7 +47298,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="757" spans="1:21">
+    <row r="757" spans="1:28">
       <c r="A757">
         <v>10</v>
       </c>
@@ -47243,7 +47342,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="758" spans="1:21">
+    <row r="758" spans="1:28">
       <c r="A758">
         <v>11</v>
       </c>
@@ -47287,7 +47386,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="759" spans="1:21">
+    <row r="759" spans="1:28">
       <c r="A759">
         <v>12</v>
       </c>
@@ -47331,7 +47430,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="760" spans="1:21">
+    <row r="760" spans="1:28">
       <c r="A760">
         <v>13</v>
       </c>
@@ -47375,7 +47474,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="761" spans="1:21">
+    <row r="761" spans="1:28">
       <c r="A761">
         <v>14</v>
       </c>
@@ -47419,7 +47518,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="762" spans="1:21">
+    <row r="762" spans="1:28">
       <c r="A762">
         <v>15</v>
       </c>
@@ -47463,7 +47562,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="763" spans="1:21">
+    <row r="763" spans="1:28">
       <c r="A763">
         <v>16</v>
       </c>
@@ -47507,7 +47606,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="764" spans="1:21">
+    <row r="764" spans="1:28">
       <c r="A764">
         <v>17</v>
       </c>
@@ -47551,7 +47650,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="765" spans="1:21">
+    <row r="765" spans="1:28">
       <c r="A765">
         <v>18</v>
       </c>
@@ -47595,7 +47694,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="766" spans="1:21">
+    <row r="766" spans="1:28">
       <c r="A766">
         <v>19</v>
       </c>
@@ -47635,11 +47734,36 @@
       <c r="N766">
         <v>7.375</v>
       </c>
+      <c r="T766" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="U766" s="4" t="s">
         <v>985</v>
       </c>
-    </row>
-    <row r="767" spans="1:21">
+      <c r="V766" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W766" s="7">
+        <f>V766-H766</f>
+        <v>32</v>
+      </c>
+      <c r="X766" s="4" t="s">
+        <v>1746</v>
+      </c>
+      <c r="Y766" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z766" s="4">
+        <v>12</v>
+      </c>
+      <c r="AA766" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB766" s="53">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="767" spans="1:28">
       <c r="A767">
         <v>20</v>
       </c>
@@ -47683,7 +47807,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="768" spans="1:21">
+    <row r="768" spans="1:28">
       <c r="A768">
         <v>21</v>
       </c>
@@ -47727,7 +47851,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="769" spans="1:21">
+    <row r="769" spans="1:28">
       <c r="A769">
         <v>22</v>
       </c>
@@ -47771,7 +47895,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="770" spans="1:21">
+    <row r="770" spans="1:28">
       <c r="A770">
         <v>23</v>
       </c>
@@ -47815,7 +47939,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="771" spans="1:21">
+    <row r="771" spans="1:28">
       <c r="A771">
         <v>24</v>
       </c>
@@ -47859,7 +47983,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="772" spans="1:21">
+    <row r="772" spans="1:28">
       <c r="A772">
         <v>25</v>
       </c>
@@ -47903,7 +48027,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="773" spans="1:21">
+    <row r="773" spans="1:28">
       <c r="A773">
         <v>26</v>
       </c>
@@ -47947,7 +48071,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="774" spans="1:21">
+    <row r="774" spans="1:28">
       <c r="A774">
         <v>27</v>
       </c>
@@ -47991,7 +48115,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="775" spans="1:21">
+    <row r="775" spans="1:28">
       <c r="A775">
         <v>28</v>
       </c>
@@ -48035,7 +48159,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="776" spans="1:21">
+    <row r="776" spans="1:28">
       <c r="A776">
         <v>29</v>
       </c>
@@ -48079,7 +48203,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="777" spans="1:21">
+    <row r="777" spans="1:28">
       <c r="A777">
         <v>30</v>
       </c>
@@ -48119,11 +48243,36 @@
       <c r="N777">
         <v>9.0670000000000002</v>
       </c>
+      <c r="T777" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="U777" s="4" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="778" spans="1:21">
+      <c r="V777" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W777" s="7">
+        <f>V777-H777</f>
+        <v>32</v>
+      </c>
+      <c r="X777" s="4" t="s">
+        <v>1745</v>
+      </c>
+      <c r="Y777" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z777" s="4">
+        <v>27</v>
+      </c>
+      <c r="AA777" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB777" s="53">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="778" spans="1:28">
       <c r="A778">
         <v>31</v>
       </c>
@@ -48167,7 +48316,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="779" spans="1:21">
+    <row r="779" spans="1:28">
       <c r="A779">
         <v>32</v>
       </c>
@@ -48211,7 +48360,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="780" spans="1:21">
+    <row r="780" spans="1:28">
       <c r="A780">
         <v>33</v>
       </c>
@@ -48255,7 +48404,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="781" spans="1:21">
+    <row r="781" spans="1:28">
       <c r="A781">
         <v>34</v>
       </c>
@@ -48299,7 +48448,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="782" spans="1:21">
+    <row r="782" spans="1:28">
       <c r="A782">
         <v>35</v>
       </c>
@@ -48343,7 +48492,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="783" spans="1:21">
+    <row r="783" spans="1:28">
       <c r="A783">
         <v>36</v>
       </c>
@@ -48387,7 +48536,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="784" spans="1:21">
+    <row r="784" spans="1:28">
       <c r="A784">
         <v>37</v>
       </c>
@@ -49945,7 +50094,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="819" spans="1:31" s="33" customFormat="1" ht="17" thickBot="1">
+    <row r="819" spans="1:31" s="33" customFormat="1" ht="16" thickBot="1">
       <c r="A819" s="33">
         <v>75</v>
       </c>
@@ -51291,7 +51440,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="849" spans="1:21">
+    <row r="849" spans="1:28">
       <c r="A849">
         <v>30</v>
       </c>
@@ -51335,7 +51484,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="850" spans="1:21">
+    <row r="850" spans="1:28">
       <c r="A850">
         <v>31</v>
       </c>
@@ -51379,7 +51528,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="851" spans="1:21">
+    <row r="851" spans="1:28">
       <c r="A851">
         <v>32</v>
       </c>
@@ -51423,7 +51572,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="852" spans="1:21">
+    <row r="852" spans="1:28">
       <c r="A852">
         <v>33</v>
       </c>
@@ -51467,7 +51616,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="853" spans="1:21">
+    <row r="853" spans="1:28">
       <c r="A853">
         <v>34</v>
       </c>
@@ -51511,7 +51660,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="854" spans="1:21">
+    <row r="854" spans="1:28">
       <c r="A854">
         <v>35</v>
       </c>
@@ -51555,7 +51704,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="855" spans="1:21">
+    <row r="855" spans="1:28">
       <c r="A855">
         <v>36</v>
       </c>
@@ -51599,7 +51748,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="856" spans="1:21">
+    <row r="856" spans="1:28">
       <c r="A856">
         <v>37</v>
       </c>
@@ -51643,7 +51792,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="857" spans="1:21">
+    <row r="857" spans="1:28">
       <c r="A857">
         <v>38</v>
       </c>
@@ -51687,7 +51836,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="858" spans="1:21">
+    <row r="858" spans="1:28">
       <c r="A858">
         <v>39</v>
       </c>
@@ -51731,7 +51880,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="859" spans="1:21">
+    <row r="859" spans="1:28">
       <c r="A859">
         <v>40</v>
       </c>
@@ -51771,11 +51920,36 @@
       <c r="N859" s="31">
         <v>6.4909999999999997</v>
       </c>
+      <c r="T859" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="U859" s="4" t="s">
         <v>1078</v>
       </c>
-    </row>
-    <row r="860" spans="1:21">
+      <c r="V859" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W859" s="7">
+        <f>V859-H859</f>
+        <v>31</v>
+      </c>
+      <c r="X859" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y859" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z859" s="4">
+        <v>8</v>
+      </c>
+      <c r="AA859" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB859" s="53">
+        <v>0.10486111111111111</v>
+      </c>
+    </row>
+    <row r="860" spans="1:28">
       <c r="A860">
         <v>41</v>
       </c>
@@ -51819,7 +51993,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="861" spans="1:21">
+    <row r="861" spans="1:28">
       <c r="A861">
         <v>42</v>
       </c>
@@ -51863,7 +52037,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="862" spans="1:21">
+    <row r="862" spans="1:28">
       <c r="A862">
         <v>43</v>
       </c>
@@ -51907,7 +52081,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="863" spans="1:21">
+    <row r="863" spans="1:28">
       <c r="A863">
         <v>44</v>
       </c>
@@ -51951,7 +52125,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="864" spans="1:21">
+    <row r="864" spans="1:28">
       <c r="A864">
         <v>45</v>
       </c>
@@ -52699,7 +52873,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="881" spans="1:21">
+    <row r="881" spans="1:28">
       <c r="A881">
         <v>62</v>
       </c>
@@ -52743,7 +52917,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="882" spans="1:21">
+    <row r="882" spans="1:28">
       <c r="A882">
         <v>63</v>
       </c>
@@ -52787,7 +52961,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="883" spans="1:21">
+    <row r="883" spans="1:28">
       <c r="A883">
         <v>64</v>
       </c>
@@ -52831,7 +53005,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="884" spans="1:21">
+    <row r="884" spans="1:28">
       <c r="A884">
         <v>65</v>
       </c>
@@ -52875,7 +53049,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="885" spans="1:21">
+    <row r="885" spans="1:28">
       <c r="A885">
         <v>66</v>
       </c>
@@ -52919,7 +53093,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="886" spans="1:21">
+    <row r="886" spans="1:28">
       <c r="A886">
         <v>67</v>
       </c>
@@ -52963,7 +53137,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="887" spans="1:21">
+    <row r="887" spans="1:28">
       <c r="A887">
         <v>68</v>
       </c>
@@ -53007,7 +53181,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="888" spans="1:21">
+    <row r="888" spans="1:28">
       <c r="A888">
         <v>69</v>
       </c>
@@ -53051,7 +53225,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="889" spans="1:21">
+    <row r="889" spans="1:28">
       <c r="A889">
         <v>70</v>
       </c>
@@ -53095,7 +53269,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="890" spans="1:21">
+    <row r="890" spans="1:28">
       <c r="A890">
         <v>71</v>
       </c>
@@ -53139,7 +53313,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="891" spans="1:21">
+    <row r="891" spans="1:28">
       <c r="A891">
         <v>72</v>
       </c>
@@ -53183,7 +53357,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="892" spans="1:21">
+    <row r="892" spans="1:28">
       <c r="A892">
         <v>73</v>
       </c>
@@ -53227,7 +53401,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="893" spans="1:21">
+    <row r="893" spans="1:28">
       <c r="A893">
         <v>74</v>
       </c>
@@ -53271,7 +53445,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="894" spans="1:21">
+    <row r="894" spans="1:28">
       <c r="A894">
         <v>75</v>
       </c>
@@ -53311,11 +53485,36 @@
       <c r="N894" s="31">
         <v>5.7439999999999998</v>
       </c>
+      <c r="T894" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="U894" s="4" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="895" spans="1:21">
+      <c r="V894" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W894" s="7">
+        <f>V894-H894</f>
+        <v>31</v>
+      </c>
+      <c r="X894" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y894" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z894" s="4">
+        <v>31</v>
+      </c>
+      <c r="AA894" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB894" s="53">
+        <v>0.10486111111111111</v>
+      </c>
+    </row>
+    <row r="895" spans="1:28">
       <c r="A895">
         <v>76</v>
       </c>
@@ -53353,7 +53552,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="896" spans="1:21">
+    <row r="896" spans="1:28">
       <c r="A896">
         <v>77</v>
       </c>
@@ -54817,7 +55016,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="929" spans="1:21">
+    <row r="929" spans="1:28">
       <c r="A929">
         <v>33</v>
       </c>
@@ -54861,7 +55060,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="930" spans="1:21">
+    <row r="930" spans="1:28">
       <c r="A930">
         <v>34</v>
       </c>
@@ -54905,7 +55104,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="931" spans="1:21">
+    <row r="931" spans="1:28">
       <c r="A931">
         <v>35</v>
       </c>
@@ -54949,7 +55148,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="932" spans="1:21">
+    <row r="932" spans="1:28">
       <c r="A932">
         <v>36</v>
       </c>
@@ -54993,7 +55192,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="933" spans="1:21">
+    <row r="933" spans="1:28">
       <c r="A933">
         <v>37</v>
       </c>
@@ -55037,7 +55236,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="934" spans="1:21">
+    <row r="934" spans="1:28">
       <c r="A934">
         <v>38</v>
       </c>
@@ -55081,7 +55280,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="935" spans="1:21">
+    <row r="935" spans="1:28">
       <c r="A935">
         <v>39</v>
       </c>
@@ -55125,7 +55324,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="936" spans="1:21">
+    <row r="936" spans="1:28">
       <c r="A936">
         <v>40</v>
       </c>
@@ -55169,7 +55368,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="937" spans="1:21">
+    <row r="937" spans="1:28">
       <c r="A937">
         <v>41</v>
       </c>
@@ -55213,7 +55412,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="938" spans="1:21">
+    <row r="938" spans="1:28">
       <c r="A938">
         <v>42</v>
       </c>
@@ -55257,7 +55456,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="939" spans="1:21">
+    <row r="939" spans="1:28">
       <c r="A939">
         <v>43</v>
       </c>
@@ -55297,11 +55496,36 @@
       <c r="N939">
         <v>6.3710000000000004</v>
       </c>
+      <c r="T939" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="U939" s="4" t="s">
         <v>1158</v>
       </c>
-    </row>
-    <row r="940" spans="1:21">
+      <c r="V939" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W939" s="7">
+        <f>V939-H939</f>
+        <v>31</v>
+      </c>
+      <c r="X939" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="Y939" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z939" s="4">
+        <v>15</v>
+      </c>
+      <c r="AA939" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB939" s="53">
+        <v>0.10486111111111111</v>
+      </c>
+    </row>
+    <row r="940" spans="1:28">
       <c r="A940">
         <v>44</v>
       </c>
@@ -55345,7 +55569,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="941" spans="1:21">
+    <row r="941" spans="1:28">
       <c r="A941">
         <v>45</v>
       </c>
@@ -55389,7 +55613,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="942" spans="1:21">
+    <row r="942" spans="1:28">
       <c r="A942">
         <v>46</v>
       </c>
@@ -55433,7 +55657,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="943" spans="1:21">
+    <row r="943" spans="1:28">
       <c r="A943">
         <v>47</v>
       </c>
@@ -55477,7 +55701,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="944" spans="1:21">
+    <row r="944" spans="1:28">
       <c r="A944">
         <v>48</v>
       </c>
@@ -61866,7 +62090,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="1089" spans="1:21">
+    <row r="1089" spans="1:28">
       <c r="A1089">
         <v>42</v>
       </c>
@@ -61910,7 +62134,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="1090" spans="1:21">
+    <row r="1090" spans="1:28">
       <c r="A1090">
         <v>43</v>
       </c>
@@ -61954,7 +62178,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="1091" spans="1:21">
+    <row r="1091" spans="1:28">
       <c r="A1091">
         <v>44</v>
       </c>
@@ -61998,7 +62222,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="1092" spans="1:21">
+    <row r="1092" spans="1:28">
       <c r="A1092">
         <v>45</v>
       </c>
@@ -62042,7 +62266,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="1093" spans="1:21">
+    <row r="1093" spans="1:28">
       <c r="A1093">
         <v>46</v>
       </c>
@@ -62086,7 +62310,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="1094" spans="1:21">
+    <row r="1094" spans="1:28">
       <c r="A1094">
         <v>47</v>
       </c>
@@ -62130,7 +62354,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="1095" spans="1:21">
+    <row r="1095" spans="1:28">
       <c r="A1095">
         <v>48</v>
       </c>
@@ -62174,7 +62398,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="1096" spans="1:21">
+    <row r="1096" spans="1:28">
       <c r="A1096">
         <v>49</v>
       </c>
@@ -62218,7 +62442,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="1097" spans="1:21">
+    <row r="1097" spans="1:28">
       <c r="A1097">
         <v>50</v>
       </c>
@@ -62258,11 +62482,36 @@
       <c r="N1097">
         <v>7.5339999999999998</v>
       </c>
+      <c r="T1097" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="U1097" s="4" t="s">
         <v>1316</v>
       </c>
-    </row>
-    <row r="1098" spans="1:21">
+      <c r="V1097" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W1097" s="7">
+        <f>V1097-H1097</f>
+        <v>30</v>
+      </c>
+      <c r="X1097" s="4" t="s">
+        <v>1747</v>
+      </c>
+      <c r="Y1097" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z1097" s="4">
+        <v>29</v>
+      </c>
+      <c r="AA1097" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB1097" s="53">
+        <v>0.10555555555555556</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:28">
       <c r="A1098">
         <v>51</v>
       </c>
@@ -62309,7 +62558,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="1099" spans="1:21">
+    <row r="1099" spans="1:28">
       <c r="A1099">
         <v>52</v>
       </c>
@@ -62356,7 +62605,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="1100" spans="1:21">
+    <row r="1100" spans="1:28">
       <c r="A1100">
         <v>53</v>
       </c>
@@ -62400,7 +62649,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="1101" spans="1:21">
+    <row r="1101" spans="1:28">
       <c r="A1101">
         <v>54</v>
       </c>
@@ -62444,7 +62693,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="1102" spans="1:21">
+    <row r="1102" spans="1:28">
       <c r="A1102">
         <v>55</v>
       </c>
@@ -62488,7 +62737,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="1103" spans="1:21">
+    <row r="1103" spans="1:28">
       <c r="A1103">
         <v>56</v>
       </c>
@@ -62532,7 +62781,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="1104" spans="1:21">
+    <row r="1104" spans="1:28">
       <c r="A1104">
         <v>57</v>
       </c>
@@ -83746,6 +83995,1387 @@
         <v>35</v>
       </c>
       <c r="J1631" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:10">
+      <c r="A1632">
+        <v>1</v>
+      </c>
+      <c r="B1632" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1632" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1632">
+        <v>8.7859999999999996</v>
+      </c>
+      <c r="E1632" s="8">
+        <v>0.61249999999999993</v>
+      </c>
+      <c r="G1632" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1632" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1632" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1632" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:19">
+      <c r="A1633">
+        <v>2</v>
+      </c>
+      <c r="B1633" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1633" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1633">
+        <v>7.6639999999999997</v>
+      </c>
+      <c r="G1633" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1633" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1633" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1633" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:19">
+      <c r="A1634">
+        <v>3</v>
+      </c>
+      <c r="B1634" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1634" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1634">
+        <v>10.573</v>
+      </c>
+      <c r="G1634" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1634" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1634" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1634" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:19">
+      <c r="A1635">
+        <v>4</v>
+      </c>
+      <c r="B1635" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1635" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1635">
+        <v>8.2769999999999992</v>
+      </c>
+      <c r="G1635" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1635" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1635" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1635" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:19">
+      <c r="A1636">
+        <v>5</v>
+      </c>
+      <c r="B1636" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1636" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1636">
+        <v>5.2080000000000002</v>
+      </c>
+      <c r="G1636" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1636" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1636" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1636" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:19">
+      <c r="A1637">
+        <v>6</v>
+      </c>
+      <c r="B1637" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1637" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1637">
+        <v>5.1760000000000002</v>
+      </c>
+      <c r="G1637" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1637" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1637" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1637" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:19">
+      <c r="A1638">
+        <v>7</v>
+      </c>
+      <c r="B1638" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1638" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1638">
+        <v>9.3460000000000001</v>
+      </c>
+      <c r="G1638" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1638" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1638" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1638" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:19">
+      <c r="A1639">
+        <v>8</v>
+      </c>
+      <c r="B1639" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1639" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1639">
+        <v>4.1879999999999997</v>
+      </c>
+      <c r="G1639" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1639" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1639" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1639" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:19">
+      <c r="A1640">
+        <v>9</v>
+      </c>
+      <c r="B1640" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1640" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1640">
+        <v>10.725</v>
+      </c>
+      <c r="G1640" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1640" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1640" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1640" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:19">
+      <c r="A1641">
+        <v>10</v>
+      </c>
+      <c r="B1641" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1641" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1641">
+        <v>8.8460000000000001</v>
+      </c>
+      <c r="G1641" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1641" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1641" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1641" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1641" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:19">
+      <c r="A1642">
+        <v>11</v>
+      </c>
+      <c r="B1642" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1642" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1642">
+        <v>5.6630000000000003</v>
+      </c>
+      <c r="G1642" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1642" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1642" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1642" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:19">
+      <c r="A1643">
+        <v>12</v>
+      </c>
+      <c r="B1643" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1643" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1643">
+        <v>8.3569999999999993</v>
+      </c>
+      <c r="G1643" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1643" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1643" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1643" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:19">
+      <c r="A1644">
+        <v>13</v>
+      </c>
+      <c r="B1644" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1644" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1644">
+        <v>9.1029999999999998</v>
+      </c>
+      <c r="G1644" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1644" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1644" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1644" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:19">
+      <c r="A1645">
+        <v>14</v>
+      </c>
+      <c r="B1645" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1645" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1645">
+        <v>7.367</v>
+      </c>
+      <c r="G1645" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1645" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1645" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1645" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:19">
+      <c r="A1646">
+        <v>15</v>
+      </c>
+      <c r="B1646" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1646" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1646">
+        <v>10.986000000000001</v>
+      </c>
+      <c r="G1646" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1646" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1646" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1646" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:19">
+      <c r="A1647">
+        <v>16</v>
+      </c>
+      <c r="B1647" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1647" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1647">
+        <v>7.9169999999999998</v>
+      </c>
+      <c r="G1647" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1647" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1647" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1647" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:19">
+      <c r="A1648">
+        <v>17</v>
+      </c>
+      <c r="B1648" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1648" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1648">
+        <v>5.87</v>
+      </c>
+      <c r="G1648" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1648" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1648" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1648" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:10">
+      <c r="A1649">
+        <v>18</v>
+      </c>
+      <c r="B1649" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1649" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1649">
+        <v>8.766</v>
+      </c>
+      <c r="G1649" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1649" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1649" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1649" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:10">
+      <c r="A1650">
+        <v>19</v>
+      </c>
+      <c r="B1650" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1650" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1650">
+        <v>10.250999999999999</v>
+      </c>
+      <c r="G1650" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1650" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1650" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1650" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:10">
+      <c r="A1651">
+        <v>20</v>
+      </c>
+      <c r="B1651" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1651" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1651">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="G1651" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1651" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1651" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1651" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:10">
+      <c r="A1652">
+        <v>21</v>
+      </c>
+      <c r="B1652" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1652" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1652">
+        <v>12.022</v>
+      </c>
+      <c r="G1652" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1652" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1652" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1652" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:10">
+      <c r="A1653">
+        <v>22</v>
+      </c>
+      <c r="B1653" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1653" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1653">
+        <v>5.3120000000000003</v>
+      </c>
+      <c r="G1653" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1653" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1653" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1653" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:10">
+      <c r="A1654">
+        <v>23</v>
+      </c>
+      <c r="B1654" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1654" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1654">
+        <v>4.3470000000000004</v>
+      </c>
+      <c r="G1654" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1654" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1654" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1654" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:10">
+      <c r="A1655">
+        <v>24</v>
+      </c>
+      <c r="B1655" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1655" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1655">
+        <v>7.4379999999999997</v>
+      </c>
+      <c r="G1655" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1655" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1655" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1655" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:10">
+      <c r="A1656">
+        <v>25</v>
+      </c>
+      <c r="B1656" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1656" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1656" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1656" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1656" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1656" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:10">
+      <c r="A1657">
+        <v>26</v>
+      </c>
+      <c r="B1657" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1657" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1657" s="8">
+        <v>0.62013888888888891</v>
+      </c>
+      <c r="G1657" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1657" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1657" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1657" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:10">
+      <c r="A1658">
+        <v>1</v>
+      </c>
+      <c r="B1658" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1658" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1658">
+        <v>5.7720000000000002</v>
+      </c>
+      <c r="E1658" s="8">
+        <v>0.62013888888888891</v>
+      </c>
+      <c r="G1658" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1658" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1658" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1658" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:10">
+      <c r="A1659">
+        <v>2</v>
+      </c>
+      <c r="B1659" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1659" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1659">
+        <v>11.734</v>
+      </c>
+      <c r="G1659" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1659" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1659" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1659" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:10">
+      <c r="A1660">
+        <v>3</v>
+      </c>
+      <c r="B1660" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1660" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1660">
+        <v>7.2850000000000001</v>
+      </c>
+      <c r="G1660" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1660" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1660" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1660" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:10">
+      <c r="A1661">
+        <v>4</v>
+      </c>
+      <c r="B1661" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1661" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1661">
+        <v>4.7910000000000004</v>
+      </c>
+      <c r="G1661" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1661" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1661" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1661" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:10">
+      <c r="A1662">
+        <v>5</v>
+      </c>
+      <c r="B1662" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1662" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1662">
+        <v>12.79</v>
+      </c>
+      <c r="G1662" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1662" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1662" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1662" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:10">
+      <c r="A1663">
+        <v>6</v>
+      </c>
+      <c r="B1663" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1663" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1663">
+        <v>7.7050000000000001</v>
+      </c>
+      <c r="G1663" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1663" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1663" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1663" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:10">
+      <c r="A1664">
+        <v>7</v>
+      </c>
+      <c r="B1664" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1664" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1664">
+        <v>11.984</v>
+      </c>
+      <c r="G1664" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1664" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1664" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1664" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:10">
+      <c r="A1665">
+        <v>8</v>
+      </c>
+      <c r="B1665" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1665" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1665">
+        <v>7.7649999999999997</v>
+      </c>
+      <c r="G1665" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1665" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1665" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1665" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:10">
+      <c r="A1666">
+        <v>9</v>
+      </c>
+      <c r="B1666" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1666" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1666">
+        <v>8.6370000000000005</v>
+      </c>
+      <c r="G1666" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1666" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1666" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1666" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:10">
+      <c r="A1667">
+        <v>10</v>
+      </c>
+      <c r="B1667" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1667" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1667">
+        <v>6.4</v>
+      </c>
+      <c r="G1667" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1667" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1667" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1667" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:10">
+      <c r="A1668">
+        <v>11</v>
+      </c>
+      <c r="B1668" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1668" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1668">
+        <v>8.8650000000000002</v>
+      </c>
+      <c r="G1668" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1668" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1668" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1668" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:10">
+      <c r="A1669">
+        <v>12</v>
+      </c>
+      <c r="B1669" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1669" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1669">
+        <v>10.105</v>
+      </c>
+      <c r="G1669" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1669" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1669" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1669" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:10">
+      <c r="A1670">
+        <v>13</v>
+      </c>
+      <c r="B1670" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1670" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1670">
+        <v>9.0150000000000006</v>
+      </c>
+      <c r="G1670" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1670" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1670" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1670" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:10">
+      <c r="A1671">
+        <v>14</v>
+      </c>
+      <c r="B1671" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1671" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1671">
+        <v>12.52</v>
+      </c>
+      <c r="G1671" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1671" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1671" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1671" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:10">
+      <c r="A1672">
+        <v>15</v>
+      </c>
+      <c r="B1672" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1672" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1672">
+        <v>6.8410000000000002</v>
+      </c>
+      <c r="G1672" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1672" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1672" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1672" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:10">
+      <c r="A1673">
+        <v>16</v>
+      </c>
+      <c r="B1673" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1673" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1673">
+        <v>7.0670000000000002</v>
+      </c>
+      <c r="G1673" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1673" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1673" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1673" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:10">
+      <c r="A1674">
+        <v>17</v>
+      </c>
+      <c r="B1674" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1674" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1674">
+        <v>8.0530000000000008</v>
+      </c>
+      <c r="G1674" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1674" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1674" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1674" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:10">
+      <c r="A1675">
+        <v>18</v>
+      </c>
+      <c r="B1675" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1675" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1675">
+        <v>10.236000000000001</v>
+      </c>
+      <c r="G1675" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1675" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1675" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1675" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:10">
+      <c r="A1676">
+        <v>19</v>
+      </c>
+      <c r="B1676" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1676" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1676">
+        <v>7.1470000000000002</v>
+      </c>
+      <c r="G1676" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1676" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1676" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1676" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:10">
+      <c r="A1677">
+        <v>20</v>
+      </c>
+      <c r="B1677" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1677" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1677">
+        <v>11.042</v>
+      </c>
+      <c r="G1677" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1677" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1677" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1677" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:10">
+      <c r="A1678">
+        <v>21</v>
+      </c>
+      <c r="B1678" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1678" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1678">
+        <v>8.6890000000000001</v>
+      </c>
+      <c r="G1678" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1678" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1678" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1678" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:10">
+      <c r="A1679">
+        <v>22</v>
+      </c>
+      <c r="B1679" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1679" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1679">
+        <v>11.76</v>
+      </c>
+      <c r="G1679" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1679" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1679" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1679" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:10">
+      <c r="A1680">
+        <v>23</v>
+      </c>
+      <c r="B1680" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1680" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1680">
+        <v>5.3710000000000004</v>
+      </c>
+      <c r="G1680" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1680" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1680" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1680" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:10">
+      <c r="A1681">
+        <v>24</v>
+      </c>
+      <c r="B1681" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1681" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1681">
+        <v>7.4809999999999999</v>
+      </c>
+      <c r="G1681" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1681" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1681" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1681" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:10">
+      <c r="A1682">
+        <v>25</v>
+      </c>
+      <c r="B1682" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1682" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1682">
+        <v>10.121</v>
+      </c>
+      <c r="G1682" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1682" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1682" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1682" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:10">
+      <c r="A1683">
+        <v>26</v>
+      </c>
+      <c r="B1683" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1683" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1683" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1683" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1683" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1683" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:10">
+      <c r="A1684">
+        <v>27</v>
+      </c>
+      <c r="B1684" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1684" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1684" s="8">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G1684" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1684" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1684" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1684" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
getting data slice for trikinetics cohorts
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="53900" yWindow="260" windowWidth="34880" windowHeight="18820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2240" yWindow="820" windowWidth="34880" windowHeight="18820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_collections" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14428" uniqueCount="1748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14520" uniqueCount="1760">
   <si>
     <t>Site</t>
   </si>
@@ -5279,6 +5279,42 @@
   </si>
   <si>
     <t>dirty syringe</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>escaped</t>
+  </si>
+  <si>
+    <t>Almost dead, but left in; dead</t>
+  </si>
+  <si>
+    <t>34</t>
   </si>
 </sst>
 </file>
@@ -5383,8 +5419,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="447">
+  <cellStyleXfs count="451">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5977,7 +6017,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="447">
+  <cellStyles count="451">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6201,6 +6241,8 @@
     <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6424,6 +6466,8 @@
     <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11819,9 +11863,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE1874"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1775" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1803" sqref="F1803"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T220" sqref="T220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13142,8 +13186,32 @@
       <c r="Q23" s="17">
         <v>9.8500000000000004E-2</v>
       </c>
+      <c r="T23" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U23" s="4" t="s">
         <v>222</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="W23" s="4">
+        <v>45</v>
+      </c>
+      <c r="X23" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y23" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z23" s="4">
+        <v>14</v>
+      </c>
+      <c r="AA23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="53">
+        <v>0.4916666666666667</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
@@ -13603,7 +13671,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
@@ -13654,7 +13722,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -13705,7 +13773,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
@@ -13752,11 +13820,35 @@
       <c r="Q35" s="17">
         <v>7.8299999999999995E-2</v>
       </c>
+      <c r="T35" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U35" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="V35" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W35" s="4">
+        <v>43</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>1742</v>
+      </c>
+      <c r="Y35" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z35" s="4">
+        <v>28</v>
+      </c>
+      <c r="AA35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="53">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
@@ -13828,10 +13920,19 @@
         <v>1</v>
       </c>
       <c r="AB36" s="53">
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="AC36" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD36" s="53">
+        <v>0.49374999999999997</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
@@ -13882,7 +13983,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
@@ -13933,7 +14034,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
@@ -14005,7 +14106,7 @@
         <v>0.67222222222222217</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -14056,7 +14157,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>41</v>
       </c>
@@ -14107,7 +14208,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>42</v>
       </c>
@@ -14158,7 +14259,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>43</v>
       </c>
@@ -14209,7 +14310,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>44</v>
       </c>
@@ -14261,7 +14362,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>45</v>
       </c>
@@ -14306,7 +14407,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>46</v>
       </c>
@@ -14357,7 +14458,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>47</v>
       </c>
@@ -14408,7 +14509,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>48</v>
       </c>
@@ -16970,7 +17071,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>4</v>
       </c>
@@ -17024,7 +17125,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>5</v>
       </c>
@@ -17075,7 +17176,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>6</v>
       </c>
@@ -17152,8 +17253,17 @@
       <c r="AB99" s="53">
         <v>0.67222222222222217</v>
       </c>
-    </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC99" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD99" s="53">
+        <v>0.61527777777777781</v>
+      </c>
+      <c r="AE99" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="100" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>7</v>
       </c>
@@ -17204,7 +17314,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>8</v>
       </c>
@@ -17255,7 +17365,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>9</v>
       </c>
@@ -17309,7 +17419,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>10</v>
       </c>
@@ -17360,7 +17470,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>11</v>
       </c>
@@ -17411,7 +17521,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>12</v>
       </c>
@@ -17462,7 +17572,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>13</v>
       </c>
@@ -17513,7 +17623,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>14</v>
       </c>
@@ -17564,7 +17674,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>15</v>
       </c>
@@ -17615,7 +17725,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>16</v>
       </c>
@@ -17666,7 +17776,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>17</v>
       </c>
@@ -17717,7 +17827,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>18</v>
       </c>
@@ -17768,7 +17878,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>19</v>
       </c>
@@ -21262,6 +21372,27 @@
       </c>
       <c r="U179" s="4" t="s">
         <v>380</v>
+      </c>
+      <c r="V179" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="W179" s="4">
+        <v>42</v>
+      </c>
+      <c r="X179" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y179" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z179" s="4">
+        <v>26</v>
+      </c>
+      <c r="AA179" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB179" s="53">
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="180" spans="1:31" x14ac:dyDescent="0.2">
@@ -23423,6 +23554,9 @@
       <c r="Q219">
         <v>0.96996369999999998</v>
       </c>
+      <c r="T219" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U219" s="4" t="s">
         <v>422</v>
       </c>
@@ -26294,6 +26428,15 @@
       <c r="AB272" s="53">
         <v>0.67222222222222217</v>
       </c>
+      <c r="AC272" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD272" s="53">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="AE272" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="273" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A273">
@@ -29758,9 +29901,8 @@
       <c r="V341" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="W341" s="7">
-        <f>V341-H341</f>
-        <v>34</v>
+      <c r="W341" s="7" t="s">
+        <v>1759</v>
       </c>
       <c r="X341" s="4" t="s">
         <v>1746</v>
@@ -29773,6 +29915,9 @@
       </c>
       <c r="AA341" s="4">
         <v>2</v>
+      </c>
+      <c r="AB341" s="53">
+        <v>0.4069444444444445</v>
       </c>
       <c r="AC341" s="7" t="s">
         <v>134</v>
@@ -39930,7 +40075,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="593" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A593">
         <v>73</v>
       </c>
@@ -39998,7 +40143,7 @@
         <v>0.47430555555555554</v>
       </c>
     </row>
-    <row r="594" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A594">
         <v>74</v>
       </c>
@@ -40042,7 +40187,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="595" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A595">
         <v>75</v>
       </c>
@@ -40086,7 +40231,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="596" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A596">
         <v>76</v>
       </c>
@@ -40130,7 +40275,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="597" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A597">
         <v>77</v>
       </c>
@@ -40168,7 +40313,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="598" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A598">
         <v>78</v>
       </c>
@@ -40212,7 +40357,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="599" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A599">
         <v>1</v>
       </c>
@@ -40262,7 +40407,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="600" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A600">
         <v>2</v>
       </c>
@@ -40306,7 +40451,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="601" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A601">
         <v>3</v>
       </c>
@@ -40346,11 +40491,41 @@
       <c r="N601">
         <v>6.8860000000000001</v>
       </c>
+      <c r="T601" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U601" s="4" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="602" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="V601" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W601" s="4">
+        <v>34</v>
+      </c>
+      <c r="X601" s="4" t="s">
+        <v>1727</v>
+      </c>
+      <c r="Y601" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z601" s="4">
+        <v>16</v>
+      </c>
+      <c r="AA601" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB601" s="53">
+        <v>0.66736111111111107</v>
+      </c>
+      <c r="AC601" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD601" s="53">
+        <v>0.39930555555555558</v>
+      </c>
+    </row>
+    <row r="602" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A602">
         <v>4</v>
       </c>
@@ -40394,7 +40569,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="603" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A603">
         <v>5</v>
       </c>
@@ -40438,7 +40613,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="604" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A604">
         <v>6</v>
       </c>
@@ -40482,7 +40657,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="605" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A605">
         <v>7</v>
       </c>
@@ -40526,7 +40701,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="606" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A606">
         <v>8</v>
       </c>
@@ -40570,7 +40745,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="607" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A607">
         <v>9</v>
       </c>
@@ -40614,7 +40789,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="608" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A608">
         <v>10</v>
       </c>
@@ -41097,8 +41272,32 @@
       <c r="N618">
         <v>8.0150000000000006</v>
       </c>
+      <c r="T618" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U618" s="4" t="s">
         <v>836</v>
+      </c>
+      <c r="V618" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W618" s="4">
+        <v>34</v>
+      </c>
+      <c r="X618" s="4" t="s">
+        <v>1748</v>
+      </c>
+      <c r="Y618" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z618" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA618" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB618" s="53">
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="619" spans="1:28" x14ac:dyDescent="0.2">
@@ -49216,8 +49415,32 @@
       <c r="N798">
         <v>4.351</v>
       </c>
+      <c r="T798" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U798" s="4" t="s">
         <v>1016</v>
+      </c>
+      <c r="V798" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W798" s="4">
+        <v>35</v>
+      </c>
+      <c r="X798" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="Y798" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z798" s="4">
+        <v>25</v>
+      </c>
+      <c r="AA798" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB798" s="53">
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="799" spans="1:28" x14ac:dyDescent="0.2">
@@ -49260,8 +49483,32 @@
       <c r="N799">
         <v>7.1050000000000004</v>
       </c>
+      <c r="T799" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U799" s="4" t="s">
         <v>1017</v>
+      </c>
+      <c r="V799" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W799" s="4">
+        <v>35</v>
+      </c>
+      <c r="X799" s="4" t="s">
+        <v>1749</v>
+      </c>
+      <c r="Y799" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z799" s="4">
+        <v>24</v>
+      </c>
+      <c r="AA799" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB799" s="53">
+        <v>0.66736111111111107</v>
       </c>
     </row>
     <row r="800" spans="1:28" x14ac:dyDescent="0.2">
@@ -50757,7 +51004,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="833" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="833" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A833">
         <v>14</v>
       </c>
@@ -50801,7 +51048,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="834" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="834" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A834">
         <v>15</v>
       </c>
@@ -50845,7 +51092,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="835" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="835" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A835">
         <v>16</v>
       </c>
@@ -50889,7 +51136,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="836" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="836" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A836">
         <v>17</v>
       </c>
@@ -50933,7 +51180,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="837" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A837">
         <v>18</v>
       </c>
@@ -50977,7 +51224,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="838" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="838" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A838">
         <v>19</v>
       </c>
@@ -51021,7 +51268,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="839" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="839" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A839">
         <v>20</v>
       </c>
@@ -51065,7 +51312,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="840" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="840" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A840">
         <v>21</v>
       </c>
@@ -51105,11 +51352,35 @@
       <c r="N840" s="31">
         <v>3.4630000000000001</v>
       </c>
+      <c r="T840" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U840" s="4" t="s">
         <v>1058</v>
       </c>
-    </row>
-    <row r="841" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V840" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W840" s="4">
+        <v>36</v>
+      </c>
+      <c r="X840" s="4" t="s">
+        <v>1750</v>
+      </c>
+      <c r="Y840" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z840" s="4">
+        <v>9</v>
+      </c>
+      <c r="AA840" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB840" s="53">
+        <v>0.66805555555555562</v>
+      </c>
+    </row>
+    <row r="841" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A841">
         <v>22</v>
       </c>
@@ -51153,7 +51424,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="842" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="842" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A842">
         <v>23</v>
       </c>
@@ -51197,7 +51468,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="843" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="843" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A843">
         <v>24</v>
       </c>
@@ -51241,7 +51512,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="844" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="844" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A844">
         <v>25</v>
       </c>
@@ -51285,7 +51556,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="845" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="845" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A845">
         <v>26</v>
       </c>
@@ -51329,7 +51600,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="846" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="846" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A846">
         <v>27</v>
       </c>
@@ -51373,7 +51644,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="847" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="847" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A847">
         <v>28</v>
       </c>
@@ -51417,7 +51688,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="848" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="848" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A848">
         <v>29</v>
       </c>
@@ -53532,7 +53803,7 @@
         <v>1</v>
       </c>
       <c r="AB894" s="53">
-        <v>0.10486111111111111</v>
+        <v>0.60486111111111118</v>
       </c>
     </row>
     <row r="895" spans="1:28" x14ac:dyDescent="0.2">
@@ -53617,7 +53888,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="897" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="897" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A897">
         <v>1</v>
       </c>
@@ -53667,7 +53938,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="898" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="898" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A898">
         <v>2</v>
       </c>
@@ -53711,7 +53982,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="899" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="899" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A899">
         <v>3</v>
       </c>
@@ -53751,11 +54022,35 @@
       <c r="N899">
         <v>5.45</v>
       </c>
+      <c r="T899" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U899" s="4" t="s">
         <v>1117</v>
       </c>
-    </row>
-    <row r="900" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V899" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="W899" s="4">
+        <v>33</v>
+      </c>
+      <c r="X899" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="Y899" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z899" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA899" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB899" s="53">
+        <v>0.72569444444444453</v>
+      </c>
+    </row>
+    <row r="900" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A900">
         <v>4</v>
       </c>
@@ -53799,7 +54094,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="901" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="901" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A901">
         <v>5</v>
       </c>
@@ -53843,7 +54138,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="902" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="902" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A902">
         <v>6</v>
       </c>
@@ -53883,11 +54178,35 @@
       <c r="N902">
         <v>7.524</v>
       </c>
+      <c r="T902" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U902" s="4" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="903" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V902" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="W902" s="4">
+        <v>35</v>
+      </c>
+      <c r="X902" s="4" t="s">
+        <v>1756</v>
+      </c>
+      <c r="Y902" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z902" s="4">
+        <v>17</v>
+      </c>
+      <c r="AA902" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB902" s="53">
+        <v>0.4291666666666667</v>
+      </c>
+    </row>
+    <row r="903" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A903">
         <v>7</v>
       </c>
@@ -53931,7 +54250,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="904" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="904" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A904">
         <v>8</v>
       </c>
@@ -53975,7 +54294,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="905" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="905" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A905">
         <v>9</v>
       </c>
@@ -54019,7 +54338,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="906" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="906" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A906">
         <v>10</v>
       </c>
@@ -54066,7 +54385,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="907" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="907" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A907">
         <v>11</v>
       </c>
@@ -54110,7 +54429,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="908" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="908" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A908">
         <v>12</v>
       </c>
@@ -54154,7 +54473,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="909" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="909" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A909">
         <v>13</v>
       </c>
@@ -54198,7 +54517,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="910" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="910" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A910">
         <v>14</v>
       </c>
@@ -54245,7 +54564,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="911" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="911" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A911">
         <v>15</v>
       </c>
@@ -54289,7 +54608,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="912" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="912" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A912">
         <v>16</v>
       </c>
@@ -57093,8 +57412,41 @@
       <c r="O974" s="8">
         <v>0.51944444444444449</v>
       </c>
+      <c r="T974" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U974" s="4" t="s">
         <v>1192</v>
+      </c>
+      <c r="V974" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="W974" s="4">
+        <v>33</v>
+      </c>
+      <c r="X974" s="4" t="s">
+        <v>1755</v>
+      </c>
+      <c r="Y974" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z974" s="4">
+        <v>20</v>
+      </c>
+      <c r="AA974" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB974" s="53">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="AC974" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD974" s="53">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="AE974" t="s">
+        <v>1757</v>
       </c>
     </row>
     <row r="975" spans="1:31" x14ac:dyDescent="0.2">
@@ -57185,7 +57537,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="977" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="977" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A977">
         <v>4</v>
       </c>
@@ -57229,7 +57581,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="978" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="978" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A978">
         <v>5</v>
       </c>
@@ -57273,7 +57625,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="979" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="979" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A979">
         <v>6</v>
       </c>
@@ -57317,7 +57669,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="980" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="980" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A980">
         <v>7</v>
       </c>
@@ -57361,7 +57713,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="981" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="981" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A981">
         <v>8</v>
       </c>
@@ -57401,11 +57753,35 @@
       <c r="N981" s="31">
         <v>5.89</v>
       </c>
+      <c r="T981" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U981" s="4" t="s">
         <v>1199</v>
       </c>
-    </row>
-    <row r="982" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V981" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W981" s="4">
+        <v>33</v>
+      </c>
+      <c r="X981" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="Y981" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z981" s="4">
+        <v>13</v>
+      </c>
+      <c r="AA981" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB981" s="53">
+        <v>0.66805555555555562</v>
+      </c>
+    </row>
+    <row r="982" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A982">
         <v>9</v>
       </c>
@@ -57449,7 +57825,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="983" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="983" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A983">
         <v>10</v>
       </c>
@@ -57493,7 +57869,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="984" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="984" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A984">
         <v>11</v>
       </c>
@@ -57537,7 +57913,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="985" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="985" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A985">
         <v>12</v>
       </c>
@@ -57581,7 +57957,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="986" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="986" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A986">
         <v>13</v>
       </c>
@@ -57621,11 +57997,35 @@
       <c r="N986" s="31">
         <v>5.0650000000000004</v>
       </c>
+      <c r="T986" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U986" s="4" t="s">
         <v>1204</v>
       </c>
-    </row>
-    <row r="987" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V986" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W986" s="4">
+        <v>33</v>
+      </c>
+      <c r="X986" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="Y986" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z986" s="4">
+        <v>16</v>
+      </c>
+      <c r="AA986" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB986" s="53">
+        <v>0.66875000000000007</v>
+      </c>
+    </row>
+    <row r="987" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A987">
         <v>14</v>
       </c>
@@ -57669,7 +58069,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="988" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="988" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A988">
         <v>15</v>
       </c>
@@ -57713,7 +58113,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="989" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="989" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A989">
         <v>16</v>
       </c>
@@ -57757,7 +58157,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="990" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="990" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A990">
         <v>17</v>
       </c>
@@ -57797,11 +58197,35 @@
       <c r="N990" s="31">
         <v>8.3689999999999998</v>
       </c>
+      <c r="T990" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U990" s="4" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="991" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V990" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W990" s="4">
+        <v>33</v>
+      </c>
+      <c r="X990" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="Y990" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z990" s="4">
+        <v>17</v>
+      </c>
+      <c r="AA990" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB990" s="53">
+        <v>0.66805555555555562</v>
+      </c>
+    </row>
+    <row r="991" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A991">
         <v>18</v>
       </c>
@@ -57845,7 +58269,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="992" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="992" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A992">
         <v>19</v>
       </c>
@@ -61407,7 +61831,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="1073" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1073" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1073">
         <v>25</v>
       </c>
@@ -61451,7 +61875,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="1074" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1074" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1074">
         <v>26</v>
       </c>
@@ -61495,7 +61919,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="1075" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1075" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1075">
         <v>27</v>
       </c>
@@ -61539,7 +61963,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="1076" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1076" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1076">
         <v>28</v>
       </c>
@@ -61579,11 +62003,35 @@
       <c r="N1076">
         <v>9.7810000000000006</v>
       </c>
+      <c r="T1076" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U1076" s="4" t="s">
         <v>1294</v>
       </c>
-    </row>
-    <row r="1077" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1076" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W1076" s="4">
+        <v>31</v>
+      </c>
+      <c r="X1076" s="4" t="s">
+        <v>1751</v>
+      </c>
+      <c r="Y1076" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1076" s="4">
+        <v>7</v>
+      </c>
+      <c r="AA1076" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB1076" s="53">
+        <v>0.66805555555555562</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1077">
         <v>29</v>
       </c>
@@ -61623,11 +62071,35 @@
       <c r="N1077">
         <v>10.204000000000001</v>
       </c>
+      <c r="T1077" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U1077" s="4" t="s">
         <v>1295</v>
       </c>
-    </row>
-    <row r="1078" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1077" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="W1077" s="4">
+        <v>32</v>
+      </c>
+      <c r="X1077" s="4" t="s">
+        <v>1752</v>
+      </c>
+      <c r="Y1077" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1077" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA1077" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB1077" s="53">
+        <v>0.72569444444444453</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1078">
         <v>30</v>
       </c>
@@ -61671,7 +62143,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="1079" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1079" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1079">
         <v>31</v>
       </c>
@@ -61715,7 +62187,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="1080" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1080" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1080">
         <v>33</v>
       </c>
@@ -61759,7 +62231,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="1081" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1081" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1081">
         <v>34</v>
       </c>
@@ -61803,7 +62275,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="1082" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1082" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1082">
         <v>35</v>
       </c>
@@ -61847,7 +62319,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="1083" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1083" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1083">
         <v>36</v>
       </c>
@@ -61891,7 +62363,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="1084" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1084" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1084">
         <v>37</v>
       </c>
@@ -61935,7 +62407,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="1085" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1085" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1085">
         <v>38</v>
       </c>
@@ -61979,7 +62451,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="1086" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1086" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1086">
         <v>39</v>
       </c>
@@ -62023,7 +62495,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="1087" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1087" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1087">
         <v>40</v>
       </c>
@@ -62067,7 +62539,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="1088" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1088" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1088">
         <v>41</v>
       </c>
@@ -62283,8 +62755,32 @@
       <c r="N1092">
         <v>6.5449999999999999</v>
       </c>
+      <c r="T1092" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U1092" s="4" t="s">
         <v>1310</v>
+      </c>
+      <c r="V1092" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="W1092" s="4">
+        <v>32</v>
+      </c>
+      <c r="X1092" s="4" t="s">
+        <v>1753</v>
+      </c>
+      <c r="Y1092" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1092" s="4">
+        <v>13</v>
+      </c>
+      <c r="AA1092" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB1092" s="53">
+        <v>0.72638888888888886</v>
       </c>
     </row>
     <row r="1093" spans="1:28" x14ac:dyDescent="0.2">
@@ -62846,7 +63342,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="1105" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1105">
         <v>58</v>
       </c>
@@ -62890,7 +63386,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="1106" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1106" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1106">
         <v>59</v>
       </c>
@@ -62934,7 +63430,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="1107" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1107">
         <v>60</v>
       </c>
@@ -62974,11 +63470,35 @@
       <c r="N1107">
         <v>5.0449999999999999</v>
       </c>
+      <c r="T1107" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U1107" s="4" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="1108" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1107" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W1107" s="4">
+        <v>31</v>
+      </c>
+      <c r="X1107" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="Y1107" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1107" s="4">
+        <v>30</v>
+      </c>
+      <c r="AA1107" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB1107" s="53">
+        <v>0.66736111111111107</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1108">
         <v>61</v>
       </c>
@@ -63016,7 +63536,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="1109" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1109" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1109">
         <v>62</v>
       </c>
@@ -63060,7 +63580,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="1110" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1110" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1110">
         <v>63</v>
       </c>
@@ -63104,7 +63624,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="1111" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1111" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1111">
         <v>64</v>
       </c>
@@ -63142,7 +63662,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="1112" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1112" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1112">
         <v>65</v>
       </c>
@@ -63186,7 +63706,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="1113" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1113" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1113">
         <v>66</v>
       </c>
@@ -63230,7 +63750,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="1114" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1114" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1114">
         <v>67</v>
       </c>
@@ -63274,7 +63794,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="1115" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1115" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1115">
         <v>68</v>
       </c>
@@ -63318,7 +63838,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="1116" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1116" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1116">
         <v>69</v>
       </c>
@@ -63362,7 +63882,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="1117" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1117" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1117">
         <v>70</v>
       </c>
@@ -63406,7 +63926,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="1118" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1118" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1118">
         <v>71</v>
       </c>
@@ -63450,7 +63970,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="1119" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1119" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1119">
         <v>72</v>
       </c>
@@ -63494,7 +64014,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="1120" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1120" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1120">
         <v>73</v>
       </c>
@@ -64960,7 +65480,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="1153" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1153" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1153">
         <v>29</v>
       </c>
@@ -65004,7 +65524,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="1154" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1154" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1154">
         <v>30</v>
       </c>
@@ -65048,7 +65568,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="1155" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1155" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1155">
         <v>31</v>
       </c>
@@ -65092,7 +65612,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="1156" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1156" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1156">
         <v>32</v>
       </c>
@@ -65136,7 +65656,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="1157" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1157" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1157">
         <v>33</v>
       </c>
@@ -65180,7 +65700,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="1158" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1158" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1158">
         <v>34</v>
       </c>
@@ -65224,7 +65744,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="1159" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1159" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1159">
         <v>35</v>
       </c>
@@ -65264,11 +65784,35 @@
       <c r="N1159">
         <v>6.3579999999999997</v>
       </c>
+      <c r="T1159" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U1159" s="4" t="s">
         <v>1377</v>
       </c>
-    </row>
-    <row r="1160" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1159" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="W1159" s="4">
+        <v>33</v>
+      </c>
+      <c r="X1159" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="Y1159" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1159" s="4">
+        <v>16</v>
+      </c>
+      <c r="AA1159" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB1159" s="53">
+        <v>0.4291666666666667</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1160">
         <v>36</v>
       </c>
@@ -65312,7 +65856,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="1161" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1161" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1161">
         <v>37</v>
       </c>
@@ -65356,7 +65900,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="1162" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1162" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1162">
         <v>38</v>
       </c>
@@ -65400,7 +65944,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="1163" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1163" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1163">
         <v>39</v>
       </c>
@@ -65444,7 +65988,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="1164" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1164" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1164">
         <v>40</v>
       </c>
@@ -65488,7 +66032,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="1165" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1165" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1165">
         <v>41</v>
       </c>
@@ -65535,7 +66079,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="1166" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1166" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1166">
         <v>42</v>
       </c>
@@ -65579,7 +66123,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="1167" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1167" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1167">
         <v>43</v>
       </c>
@@ -65623,7 +66167,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="1168" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1168" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1168">
         <v>44</v>
       </c>
@@ -65663,8 +66207,32 @@
       <c r="N1168">
         <v>5.6740000000000004</v>
       </c>
+      <c r="T1168" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U1168" s="4" t="s">
         <v>1386</v>
+      </c>
+      <c r="V1168" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="W1168" s="4">
+        <v>31</v>
+      </c>
+      <c r="X1168" s="4" t="s">
+        <v>1754</v>
+      </c>
+      <c r="Y1168" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1168" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA1168" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB1168" s="53">
+        <v>0.72638888888888886</v>
       </c>
     </row>
     <row r="1169" spans="1:21" x14ac:dyDescent="0.2">
@@ -67078,7 +67646,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="1201" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1201" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1201">
         <v>10</v>
       </c>
@@ -67122,7 +67690,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="1202" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1202" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1202">
         <v>11</v>
       </c>
@@ -67166,7 +67734,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="1203" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1203" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1203">
         <v>12</v>
       </c>
@@ -67210,7 +67778,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="1204" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1204" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1204">
         <v>13</v>
       </c>
@@ -67250,11 +67818,35 @@
       <c r="N1204">
         <v>3.9159999999999999</v>
       </c>
+      <c r="T1204" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U1204" s="4" t="s">
         <v>1422</v>
       </c>
-    </row>
-    <row r="1205" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1204" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W1204" s="4">
+        <v>30</v>
+      </c>
+      <c r="X1204" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y1204" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1204" s="4">
+        <v>30</v>
+      </c>
+      <c r="AA1204" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB1204" s="53">
+        <v>0.66805555555555562</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1205">
         <v>14</v>
       </c>
@@ -67298,7 +67890,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="1206" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1206" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1206">
         <v>15</v>
       </c>
@@ -67342,7 +67934,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="1207" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1207" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1207">
         <v>16</v>
       </c>
@@ -67386,7 +67978,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="1208" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1208" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1208">
         <v>17</v>
       </c>
@@ -67430,7 +68022,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="1209" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1209" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1209">
         <v>18</v>
       </c>
@@ -67474,7 +68066,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="1210" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1210" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1210">
         <v>19</v>
       </c>
@@ -67518,7 +68110,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="1211" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1211" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1211">
         <v>20</v>
       </c>
@@ -67562,7 +68154,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="1212" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1212" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1212">
         <v>21</v>
       </c>
@@ -67606,7 +68198,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="1213" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1213" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1213">
         <v>22</v>
       </c>
@@ -67650,7 +68242,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="1214" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1214" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1214">
         <v>23</v>
       </c>
@@ -67694,7 +68286,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="1215" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1215" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1215">
         <v>24</v>
       </c>
@@ -67738,7 +68330,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="1216" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1216" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1216">
         <v>25</v>
       </c>
@@ -71319,7 +71911,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="1297" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1297" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1297">
         <v>3</v>
       </c>
@@ -71359,11 +71951,35 @@
       <c r="N1297">
         <v>9.5660000000000007</v>
       </c>
+      <c r="T1297" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="U1297" s="4" t="s">
         <v>1515</v>
       </c>
-    </row>
-    <row r="1298" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1297" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="W1297" s="4">
+        <v>31</v>
+      </c>
+      <c r="X1297" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y1297" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1297" s="4">
+        <v>23</v>
+      </c>
+      <c r="AA1297" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB1297" s="53">
+        <v>0.4291666666666667</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1298">
         <v>4</v>
       </c>
@@ -71407,7 +72023,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="1299" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1299" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1299">
         <v>5</v>
       </c>
@@ -71451,7 +72067,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="1300" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1300" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1300">
         <v>6</v>
       </c>
@@ -71495,7 +72111,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="1301" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1301" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1301">
         <v>7</v>
       </c>
@@ -71539,7 +72155,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="1302" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1302" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1302">
         <v>8</v>
       </c>
@@ -71583,7 +72199,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="1303" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1303" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1303">
         <v>9</v>
       </c>
@@ -71627,7 +72243,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="1304" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1304" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1304">
         <v>10</v>
       </c>
@@ -71671,7 +72287,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="1305" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1305" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1305">
         <v>11</v>
       </c>
@@ -71715,7 +72331,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="1306" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1306" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1306">
         <v>12</v>
       </c>
@@ -71759,7 +72375,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="1307" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1307" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1307">
         <v>13</v>
       </c>
@@ -71803,7 +72419,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="1308" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1308" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1308">
         <v>14</v>
       </c>
@@ -71847,7 +72463,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="1309" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1309" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1309">
         <v>15</v>
       </c>
@@ -71891,7 +72507,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="1310" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1310" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1310">
         <v>16</v>
       </c>
@@ -71935,7 +72551,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="1311" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1311" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1311">
         <v>17</v>
       </c>
@@ -71979,7 +72595,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="1312" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1312" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1312">
         <v>18</v>
       </c>
@@ -90108,6 +90724,12 @@
       <c r="C1834" t="s">
         <v>5</v>
       </c>
+      <c r="D1834">
+        <v>8.5670000000000002</v>
+      </c>
+      <c r="E1834" s="8">
+        <v>0.50138888888888888</v>
+      </c>
       <c r="G1834" s="1" t="s">
         <v>138</v>
       </c>
@@ -90119,6 +90741,9 @@
       </c>
       <c r="J1834" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="K1834" s="31">
+        <v>7000</v>
       </c>
     </row>
     <row r="1835" spans="1:11" x14ac:dyDescent="0.2">
@@ -90131,6 +90756,9 @@
       <c r="C1835" t="s">
         <v>5</v>
       </c>
+      <c r="D1835">
+        <v>8.4610000000000003</v>
+      </c>
       <c r="G1835" s="1" t="s">
         <v>138</v>
       </c>
@@ -90142,6 +90770,9 @@
       </c>
       <c r="J1835" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="K1835" s="31">
+        <v>7000</v>
       </c>
     </row>
     <row r="1836" spans="1:11" x14ac:dyDescent="0.2">
@@ -90154,6 +90785,9 @@
       <c r="C1836" t="s">
         <v>5</v>
       </c>
+      <c r="D1836">
+        <v>11.715999999999999</v>
+      </c>
       <c r="G1836" s="1" t="s">
         <v>138</v>
       </c>
@@ -90166,6 +90800,9 @@
       <c r="J1836" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K1836" s="31">
+        <v>7000</v>
+      </c>
     </row>
     <row r="1837" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1837">
@@ -90177,6 +90814,9 @@
       <c r="C1837" t="s">
         <v>5</v>
       </c>
+      <c r="D1837">
+        <v>4.6959999999999997</v>
+      </c>
       <c r="G1837" s="1" t="s">
         <v>138</v>
       </c>
@@ -90188,6 +90828,9 @@
       </c>
       <c r="J1837" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="K1837" s="31">
+        <v>7000</v>
       </c>
     </row>
     <row r="1838" spans="1:11" x14ac:dyDescent="0.2">
@@ -90200,6 +90843,9 @@
       <c r="C1838" t="s">
         <v>5</v>
       </c>
+      <c r="D1838">
+        <v>4.8170000000000002</v>
+      </c>
       <c r="G1838" s="1" t="s">
         <v>138</v>
       </c>
@@ -90212,6 +90858,9 @@
       <c r="J1838" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K1838" s="31">
+        <v>7000</v>
+      </c>
     </row>
     <row r="1839" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1839">
@@ -90223,6 +90872,9 @@
       <c r="C1839" t="s">
         <v>5</v>
       </c>
+      <c r="D1839">
+        <v>11.222</v>
+      </c>
       <c r="G1839" s="1" t="s">
         <v>138</v>
       </c>
@@ -90234,6 +90886,9 @@
       </c>
       <c r="J1839" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="K1839" s="31">
+        <v>7000</v>
       </c>
     </row>
     <row r="1840" spans="1:11" x14ac:dyDescent="0.2">
@@ -90246,6 +90901,9 @@
       <c r="C1840" t="s">
         <v>5</v>
       </c>
+      <c r="D1840">
+        <v>7.6050000000000004</v>
+      </c>
       <c r="G1840" s="1" t="s">
         <v>138</v>
       </c>
@@ -90258,8 +90916,11 @@
       <c r="J1840" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1841" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1840" s="31">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1841">
         <v>8</v>
       </c>
@@ -90269,6 +90930,9 @@
       <c r="C1841" t="s">
         <v>5</v>
       </c>
+      <c r="D1841">
+        <v>12.481999999999999</v>
+      </c>
       <c r="G1841" s="1" t="s">
         <v>138</v>
       </c>
@@ -90281,8 +90945,11 @@
       <c r="J1841" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1842" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1841" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1842">
         <v>9</v>
       </c>
@@ -90292,6 +90959,9 @@
       <c r="C1842" t="s">
         <v>5</v>
       </c>
+      <c r="D1842">
+        <v>7.0439999999999996</v>
+      </c>
       <c r="G1842" s="1" t="s">
         <v>138</v>
       </c>
@@ -90304,8 +90974,11 @@
       <c r="J1842" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1843" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1842" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1843">
         <v>10</v>
       </c>
@@ -90315,6 +90988,9 @@
       <c r="C1843" t="s">
         <v>5</v>
       </c>
+      <c r="D1843">
+        <v>5.6660000000000004</v>
+      </c>
       <c r="G1843" s="1" t="s">
         <v>138</v>
       </c>
@@ -90327,8 +91003,11 @@
       <c r="J1843" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1844" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1843" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1844">
         <v>11</v>
       </c>
@@ -90338,6 +91017,9 @@
       <c r="C1844" t="s">
         <v>5</v>
       </c>
+      <c r="D1844">
+        <v>8.8840000000000003</v>
+      </c>
       <c r="G1844" s="1" t="s">
         <v>138</v>
       </c>
@@ -90350,8 +91032,11 @@
       <c r="J1844" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1845" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1844" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1845">
         <v>12</v>
       </c>
@@ -90361,6 +91046,9 @@
       <c r="C1845" t="s">
         <v>5</v>
       </c>
+      <c r="D1845">
+        <v>4.9989999999999997</v>
+      </c>
       <c r="G1845" s="1" t="s">
         <v>138</v>
       </c>
@@ -90373,8 +91061,11 @@
       <c r="J1845" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1846" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1845" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1846">
         <v>13</v>
       </c>
@@ -90384,6 +91075,9 @@
       <c r="C1846" t="s">
         <v>5</v>
       </c>
+      <c r="D1846">
+        <v>11.090999999999999</v>
+      </c>
       <c r="G1846" s="1" t="s">
         <v>138</v>
       </c>
@@ -90396,8 +91090,11 @@
       <c r="J1846" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1847" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1846" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1847">
         <v>14</v>
       </c>
@@ -90407,6 +91104,9 @@
       <c r="C1847" t="s">
         <v>5</v>
       </c>
+      <c r="D1847">
+        <v>9.3870000000000005</v>
+      </c>
       <c r="G1847" s="1" t="s">
         <v>138</v>
       </c>
@@ -90419,8 +91119,11 @@
       <c r="J1847" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1848" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1847" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1848">
         <v>15</v>
       </c>
@@ -90430,6 +91133,9 @@
       <c r="C1848" t="s">
         <v>5</v>
       </c>
+      <c r="D1848">
+        <v>12.439</v>
+      </c>
       <c r="G1848" s="1" t="s">
         <v>138</v>
       </c>
@@ -90442,8 +91148,11 @@
       <c r="J1848" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1849" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1848" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1849">
         <v>16</v>
       </c>
@@ -90453,6 +91162,9 @@
       <c r="C1849" t="s">
         <v>5</v>
       </c>
+      <c r="D1849">
+        <v>7.6879999999999997</v>
+      </c>
       <c r="G1849" s="1" t="s">
         <v>138</v>
       </c>
@@ -90465,8 +91177,11 @@
       <c r="J1849" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1850" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1849" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1850">
         <v>17</v>
       </c>
@@ -90476,6 +91191,9 @@
       <c r="C1850" t="s">
         <v>5</v>
       </c>
+      <c r="D1850">
+        <v>11.819000000000001</v>
+      </c>
       <c r="G1850" s="1" t="s">
         <v>138</v>
       </c>
@@ -90488,8 +91206,11 @@
       <c r="J1850" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1851" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1850" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1851">
         <v>18</v>
       </c>
@@ -90499,6 +91220,9 @@
       <c r="C1851" t="s">
         <v>5</v>
       </c>
+      <c r="D1851">
+        <v>8.0020000000000007</v>
+      </c>
       <c r="G1851" s="1" t="s">
         <v>138</v>
       </c>
@@ -90511,8 +91235,11 @@
       <c r="J1851" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1852" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1851" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1852">
         <v>19</v>
       </c>
@@ -90534,8 +91261,11 @@
       <c r="J1852" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1853" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1852" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1853" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1853">
         <v>20</v>
       </c>
@@ -90545,6 +91275,9 @@
       <c r="C1853" t="s">
         <v>5</v>
       </c>
+      <c r="E1853" s="8">
+        <v>0.50555555555555554</v>
+      </c>
       <c r="G1853" s="1" t="s">
         <v>138</v>
       </c>
@@ -90557,8 +91290,11 @@
       <c r="J1853" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1854" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1853" s="9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="1854" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1854">
         <v>1</v>
       </c>
@@ -90568,6 +91304,12 @@
       <c r="C1854" t="s">
         <v>5</v>
       </c>
+      <c r="D1854">
+        <v>7.1980000000000004</v>
+      </c>
+      <c r="E1854" s="8">
+        <v>0.49722222222222223</v>
+      </c>
       <c r="G1854" s="1" t="s">
         <v>138</v>
       </c>
@@ -90580,8 +91322,11 @@
       <c r="J1854" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1855" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1854" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1855" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1855">
         <v>2</v>
       </c>
@@ -90591,6 +91336,9 @@
       <c r="C1855" t="s">
         <v>5</v>
       </c>
+      <c r="D1855">
+        <v>6.8959999999999999</v>
+      </c>
       <c r="G1855" s="1" t="s">
         <v>138</v>
       </c>
@@ -90603,8 +91351,11 @@
       <c r="J1855" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1856" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1855" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1856" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1856">
         <v>3</v>
       </c>
@@ -90614,6 +91365,9 @@
       <c r="C1856" t="s">
         <v>5</v>
       </c>
+      <c r="D1856">
+        <v>9.2780000000000005</v>
+      </c>
       <c r="G1856" s="1" t="s">
         <v>138</v>
       </c>
@@ -90626,8 +91380,11 @@
       <c r="J1856" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1857" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1856" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1857">
         <v>4</v>
       </c>
@@ -90637,6 +91394,9 @@
       <c r="C1857" t="s">
         <v>5</v>
       </c>
+      <c r="D1857">
+        <v>5.0069999999999997</v>
+      </c>
       <c r="G1857" s="1" t="s">
         <v>138</v>
       </c>
@@ -90649,8 +91409,11 @@
       <c r="J1857" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1858" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1857" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1858">
         <v>5</v>
       </c>
@@ -90660,6 +91423,9 @@
       <c r="C1858" t="s">
         <v>5</v>
       </c>
+      <c r="D1858">
+        <v>8.6809999999999992</v>
+      </c>
       <c r="G1858" s="1" t="s">
         <v>138</v>
       </c>
@@ -90672,8 +91438,11 @@
       <c r="J1858" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1859" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1858" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1859" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1859">
         <v>6</v>
       </c>
@@ -90683,6 +91452,9 @@
       <c r="C1859" t="s">
         <v>5</v>
       </c>
+      <c r="D1859">
+        <v>10.082000000000001</v>
+      </c>
       <c r="G1859" s="1" t="s">
         <v>138</v>
       </c>
@@ -90695,8 +91467,11 @@
       <c r="J1859" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1860" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1859" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1860" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1860">
         <v>7</v>
       </c>
@@ -90706,6 +91481,9 @@
       <c r="C1860" t="s">
         <v>5</v>
       </c>
+      <c r="D1860">
+        <v>10.522</v>
+      </c>
       <c r="G1860" s="1" t="s">
         <v>138</v>
       </c>
@@ -90718,8 +91496,11 @@
       <c r="J1860" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1861" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1860" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1861" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1861">
         <v>8</v>
       </c>
@@ -90729,6 +91510,9 @@
       <c r="C1861" t="s">
         <v>5</v>
       </c>
+      <c r="D1861">
+        <v>8.1110000000000007</v>
+      </c>
       <c r="G1861" s="1" t="s">
         <v>138</v>
       </c>
@@ -90741,8 +91525,11 @@
       <c r="J1861" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1862" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1861" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1862">
         <v>9</v>
       </c>
@@ -90752,6 +91539,9 @@
       <c r="C1862" t="s">
         <v>5</v>
       </c>
+      <c r="D1862">
+        <v>10.840999999999999</v>
+      </c>
       <c r="G1862" s="1" t="s">
         <v>138</v>
       </c>
@@ -90764,8 +91554,11 @@
       <c r="J1862" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1863" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1862" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1863">
         <v>10</v>
       </c>
@@ -90775,6 +91568,9 @@
       <c r="C1863" t="s">
         <v>5</v>
       </c>
+      <c r="D1863">
+        <v>9.6620000000000008</v>
+      </c>
       <c r="G1863" s="1" t="s">
         <v>138</v>
       </c>
@@ -90787,8 +91583,11 @@
       <c r="J1863" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1864" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1863" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1864">
         <v>11</v>
       </c>
@@ -90798,6 +91597,9 @@
       <c r="C1864" t="s">
         <v>5</v>
       </c>
+      <c r="D1864">
+        <v>10.042</v>
+      </c>
       <c r="G1864" s="1" t="s">
         <v>138</v>
       </c>
@@ -90810,8 +91612,11 @@
       <c r="J1864" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1865" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1864" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1865">
         <v>12</v>
       </c>
@@ -90821,6 +91626,9 @@
       <c r="C1865" t="s">
         <v>5</v>
       </c>
+      <c r="D1865">
+        <v>8.6349999999999998</v>
+      </c>
       <c r="G1865" s="1" t="s">
         <v>138</v>
       </c>
@@ -90833,8 +91641,11 @@
       <c r="J1865" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1866" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1865" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1866">
         <v>13</v>
       </c>
@@ -90844,6 +91655,9 @@
       <c r="C1866" t="s">
         <v>5</v>
       </c>
+      <c r="D1866">
+        <v>7.1769999999999996</v>
+      </c>
       <c r="G1866" s="1" t="s">
         <v>138</v>
       </c>
@@ -90856,8 +91670,11 @@
       <c r="J1866" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1867" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1866" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1867">
         <v>14</v>
       </c>
@@ -90867,6 +91684,9 @@
       <c r="C1867" t="s">
         <v>5</v>
       </c>
+      <c r="D1867">
+        <v>10.661</v>
+      </c>
       <c r="G1867" s="1" t="s">
         <v>138</v>
       </c>
@@ -90879,8 +91699,11 @@
       <c r="J1867" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1868" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1867" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1868">
         <v>15</v>
       </c>
@@ -90890,6 +91713,9 @@
       <c r="C1868" t="s">
         <v>5</v>
       </c>
+      <c r="D1868">
+        <v>10.757999999999999</v>
+      </c>
       <c r="G1868" s="1" t="s">
         <v>138</v>
       </c>
@@ -90902,8 +91728,11 @@
       <c r="J1868" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1869" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1868" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1869">
         <v>16</v>
       </c>
@@ -90913,6 +91742,9 @@
       <c r="C1869" t="s">
         <v>5</v>
       </c>
+      <c r="D1869">
+        <v>8.5150000000000006</v>
+      </c>
       <c r="G1869" s="1" t="s">
         <v>138</v>
       </c>
@@ -90925,8 +91757,11 @@
       <c r="J1869" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1870" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1869" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1870">
         <v>17</v>
       </c>
@@ -90936,6 +91771,9 @@
       <c r="C1870" t="s">
         <v>5</v>
       </c>
+      <c r="D1870">
+        <v>8.3610000000000007</v>
+      </c>
       <c r="G1870" s="1" t="s">
         <v>138</v>
       </c>
@@ -90948,8 +91786,11 @@
       <c r="J1870" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1871" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1870" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1871">
         <v>18</v>
       </c>
@@ -90971,8 +91812,11 @@
       <c r="J1871" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1872" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1871" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1872">
         <v>19</v>
       </c>
@@ -90982,6 +91826,9 @@
       <c r="C1872" t="s">
         <v>5</v>
       </c>
+      <c r="E1872" s="8">
+        <v>0.50138888888888888</v>
+      </c>
       <c r="G1872" s="1" t="s">
         <v>138</v>
       </c>
@@ -90994,31 +91841,15 @@
       <c r="J1872" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1873" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1873">
-        <v>20</v>
-      </c>
-      <c r="B1873" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1873" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1873" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1873" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1873" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1873" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1874" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1872" s="9">
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="1873" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J1873" s="1"/>
+      <c r="K1873" s="9"/>
+    </row>
+    <row r="1874" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J1874" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
entering in data and raw resp
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="920" windowWidth="44900" windowHeight="24180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3800" yWindow="1820" windowWidth="44900" windowHeight="24180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maggot_collections" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14551" uniqueCount="1768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14623" uniqueCount="1768">
   <si>
     <t>Site</t>
   </si>
@@ -11885,11 +11885,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE1874"/>
+  <dimension ref="A1:AE1884"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC29" sqref="AC29"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1765" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1765" sqref="K1765"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -94240,12 +94240,425 @@
         <v>2.582539E-2</v>
       </c>
     </row>
-    <row r="1873" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J1873" s="1"/>
-      <c r="K1873" s="9"/>
-    </row>
-    <row r="1874" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J1874" s="1"/>
+    <row r="1873" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1873">
+        <v>1</v>
+      </c>
+      <c r="B1873" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1873" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1873">
+        <v>9.8520000000000003</v>
+      </c>
+      <c r="E1873" s="8">
+        <v>0.63472222222222219</v>
+      </c>
+      <c r="G1873" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1873" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1873" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1873" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1873" s="9">
+        <v>7000</v>
+      </c>
+      <c r="L1873" s="16">
+        <v>0.44209490740740742</v>
+      </c>
+      <c r="M1873">
+        <v>0.1387167</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1874">
+        <v>2</v>
+      </c>
+      <c r="B1874" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1874" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1874">
+        <v>8.2520000000000007</v>
+      </c>
+      <c r="G1874" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1874" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1874" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1874" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1874" s="9">
+        <v>7000</v>
+      </c>
+      <c r="L1874" s="16">
+        <v>0.44337962962962968</v>
+      </c>
+      <c r="M1874">
+        <v>0.76856120000000006</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1875">
+        <v>3</v>
+      </c>
+      <c r="B1875" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1875" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1875">
+        <v>8.1240000000000006</v>
+      </c>
+      <c r="G1875" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1875" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1875" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1875" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1875" s="9">
+        <v>7000</v>
+      </c>
+      <c r="L1875" s="16">
+        <v>0.4442592592592593</v>
+      </c>
+      <c r="M1875" s="17">
+        <v>9.5305570000000006E-2</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1876">
+        <v>4</v>
+      </c>
+      <c r="B1876" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1876" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1876">
+        <v>9.6379999999999999</v>
+      </c>
+      <c r="G1876" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1876" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1876" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1876" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1876" s="9">
+        <v>7000</v>
+      </c>
+      <c r="L1876" s="16">
+        <v>0.44518518518518518</v>
+      </c>
+      <c r="M1876" s="17">
+        <v>8.9684710000000001E-2</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1877">
+        <v>5</v>
+      </c>
+      <c r="B1877" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1877" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1877" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1877" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1877" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1877" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1877" s="9">
+        <v>7000</v>
+      </c>
+      <c r="L1877" s="16">
+        <v>0.44607638888888884</v>
+      </c>
+      <c r="M1877" s="17">
+        <v>1.430969E-2</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1878">
+        <v>6</v>
+      </c>
+      <c r="B1878" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1878" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1878" s="8">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="G1878" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1878" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1878" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1878" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1878" s="9">
+        <v>7000</v>
+      </c>
+      <c r="L1878" s="16">
+        <v>0.44680555555555551</v>
+      </c>
+      <c r="M1878">
+        <v>1.05226E-2</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1879">
+        <v>1</v>
+      </c>
+      <c r="B1879" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1879" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1879">
+        <v>11.486000000000001</v>
+      </c>
+      <c r="E1879" s="8">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="G1879" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1879" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1879" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1879" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1879" s="9">
+        <v>6262</v>
+      </c>
+      <c r="L1879" s="16">
+        <v>0.44209490740740742</v>
+      </c>
+      <c r="M1879">
+        <v>0.33963080000000001</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1880">
+        <v>2</v>
+      </c>
+      <c r="B1880" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1880" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1880">
+        <v>7.8970000000000002</v>
+      </c>
+      <c r="G1880" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1880" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1880" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1880" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1880" s="9">
+        <v>6262</v>
+      </c>
+      <c r="L1880" s="16">
+        <v>0.44337962962962968</v>
+      </c>
+      <c r="M1880">
+        <v>0.15664649999999999</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1881">
+        <v>3</v>
+      </c>
+      <c r="B1881" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1881" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1881">
+        <v>11.602</v>
+      </c>
+      <c r="G1881" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1881" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1881" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1881" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1881" s="9">
+        <v>6262</v>
+      </c>
+      <c r="L1881" s="16">
+        <v>0.4442592592592593</v>
+      </c>
+      <c r="M1881">
+        <v>0.39685280000000001</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1882">
+        <v>4</v>
+      </c>
+      <c r="B1882" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1882" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1882">
+        <v>7.7939999999999996</v>
+      </c>
+      <c r="G1882" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1882" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1882" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1882" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1882" s="9">
+        <v>6262</v>
+      </c>
+      <c r="L1882" s="16">
+        <v>0.44518518518518518</v>
+      </c>
+      <c r="M1882">
+        <v>0.2163901</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1883">
+        <v>5</v>
+      </c>
+      <c r="B1883" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1883" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1883" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1883" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1883" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1883" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1883" s="9">
+        <v>6262</v>
+      </c>
+      <c r="L1883" s="16">
+        <v>0.44607638888888884</v>
+      </c>
+      <c r="M1883">
+        <v>2.2011099999999999E-2</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1884">
+        <v>6</v>
+      </c>
+      <c r="B1884" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1884" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1884" s="8">
+        <v>0.63472222222222219</v>
+      </c>
+      <c r="G1884" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1884" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1884" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1884" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1884" s="9">
+        <v>6262</v>
+      </c>
+      <c r="L1884" s="16">
+        <v>0.44680555555555551</v>
+      </c>
+      <c r="M1884">
+        <v>1.7909100000000001E-2</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S1467"/>

</xml_diff>

<commit_message>
updated eclosions and deaths
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14828" uniqueCount="1779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14843" uniqueCount="1782">
   <si>
     <t>Site</t>
   </si>
@@ -5367,6 +5367,15 @@
   </si>
   <si>
     <t>water tube dried up; died. FROZEN</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>not completely eclosed when put in trikinetics, stuck into pupae</t>
   </si>
 </sst>
 </file>
@@ -6799,7 +6808,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11932,9 +11941,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1910"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1409" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB1428" sqref="AB1428"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE1372" sqref="AE1372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -27095,8 +27104,32 @@
       <c r="Q282" s="17">
         <v>8.8200000000000001E-2</v>
       </c>
+      <c r="T282" s="4" t="s">
+        <v>1740</v>
+      </c>
       <c r="U282" s="4" t="s">
         <v>491</v>
+      </c>
+      <c r="V282" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="W282" s="4">
+        <v>47</v>
+      </c>
+      <c r="X282" s="4" t="s">
+        <v>1779</v>
+      </c>
+      <c r="Y282" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z282" s="4">
+        <v>25</v>
+      </c>
+      <c r="AA282" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB282" s="53">
+        <v>0.5854166666666667</v>
       </c>
     </row>
     <row r="283" spans="1:28">
@@ -75907,7 +75940,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="1377" spans="1:28">
+    <row r="1377" spans="1:31">
       <c r="A1377">
         <v>12</v>
       </c>
@@ -75945,7 +75978,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="1378" spans="1:28">
+    <row r="1378" spans="1:31">
       <c r="A1378">
         <v>13</v>
       </c>
@@ -75989,7 +76022,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="1379" spans="1:28">
+    <row r="1379" spans="1:31">
       <c r="A1379">
         <v>14</v>
       </c>
@@ -76033,7 +76066,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="1380" spans="1:28">
+    <row r="1380" spans="1:31">
       <c r="A1380">
         <v>15</v>
       </c>
@@ -76077,7 +76110,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="1381" spans="1:28">
+    <row r="1381" spans="1:31">
       <c r="A1381">
         <v>16</v>
       </c>
@@ -76138,8 +76171,17 @@
       <c r="AB1381" s="53">
         <v>0.66249999999999998</v>
       </c>
-    </row>
-    <row r="1382" spans="1:28">
+      <c r="AC1381" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD1381" s="53">
+        <v>0.56874999999999998</v>
+      </c>
+      <c r="AE1381" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:31">
       <c r="A1382">
         <v>17</v>
       </c>
@@ -76183,7 +76225,7 @@
         <v>1599</v>
       </c>
     </row>
-    <row r="1383" spans="1:28">
+    <row r="1383" spans="1:31">
       <c r="A1383">
         <v>18</v>
       </c>
@@ -76227,7 +76269,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="1384" spans="1:28">
+    <row r="1384" spans="1:31">
       <c r="A1384">
         <v>19</v>
       </c>
@@ -76271,7 +76313,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="1385" spans="1:28">
+    <row r="1385" spans="1:31">
       <c r="A1385">
         <v>20</v>
       </c>
@@ -76339,7 +76381,7 @@
         <v>0.84791666666666676</v>
       </c>
     </row>
-    <row r="1386" spans="1:28">
+    <row r="1386" spans="1:31">
       <c r="A1386">
         <v>21</v>
       </c>
@@ -76377,7 +76419,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="1387" spans="1:28">
+    <row r="1387" spans="1:31">
       <c r="A1387">
         <v>22</v>
       </c>
@@ -76421,7 +76463,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="1388" spans="1:28">
+    <row r="1388" spans="1:31">
       <c r="A1388">
         <v>23</v>
       </c>
@@ -76465,7 +76507,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="1389" spans="1:28">
+    <row r="1389" spans="1:31">
       <c r="A1389">
         <v>24</v>
       </c>
@@ -76509,7 +76551,7 @@
         <v>1606</v>
       </c>
     </row>
-    <row r="1390" spans="1:28">
+    <row r="1390" spans="1:31">
       <c r="A1390">
         <v>25</v>
       </c>
@@ -76553,7 +76595,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="1391" spans="1:28">
+    <row r="1391" spans="1:31">
       <c r="A1391">
         <v>26</v>
       </c>
@@ -76597,7 +76639,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="1392" spans="1:28">
+    <row r="1392" spans="1:31">
       <c r="A1392">
         <v>27</v>
       </c>
@@ -80150,8 +80192,35 @@
       <c r="N1471">
         <v>4.5410000000000004</v>
       </c>
+      <c r="T1471" s="4" t="s">
+        <v>1740</v>
+      </c>
       <c r="U1471" s="4" t="s">
         <v>1688</v>
+      </c>
+      <c r="V1471" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="W1471" s="4">
+        <v>31</v>
+      </c>
+      <c r="X1471" s="4" t="s">
+        <v>1780</v>
+      </c>
+      <c r="Y1471" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1471" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA1471" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB1471" s="53">
+        <v>0.73125000000000007</v>
+      </c>
+      <c r="AE1471" t="s">
+        <v>1781</v>
       </c>
     </row>
     <row r="1472" spans="1:31">
@@ -80902,7 +80971,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="1489" spans="1:21">
+    <row r="1489" spans="1:28">
       <c r="A1489">
         <v>3</v>
       </c>
@@ -80949,7 +81018,7 @@
         <v>1706</v>
       </c>
     </row>
-    <row r="1490" spans="1:21">
+    <row r="1490" spans="1:28">
       <c r="A1490">
         <v>4</v>
       </c>
@@ -80993,7 +81062,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="1491" spans="1:21">
+    <row r="1491" spans="1:28">
       <c r="A1491">
         <v>5</v>
       </c>
@@ -81037,7 +81106,7 @@
         <v>1708</v>
       </c>
     </row>
-    <row r="1492" spans="1:21">
+    <row r="1492" spans="1:28">
       <c r="A1492">
         <v>6</v>
       </c>
@@ -81081,7 +81150,7 @@
         <v>1709</v>
       </c>
     </row>
-    <row r="1493" spans="1:21">
+    <row r="1493" spans="1:28">
       <c r="A1493">
         <v>7</v>
       </c>
@@ -81125,7 +81194,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="1494" spans="1:21">
+    <row r="1494" spans="1:28">
       <c r="A1494">
         <v>8</v>
       </c>
@@ -81169,7 +81238,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="1495" spans="1:21">
+    <row r="1495" spans="1:28">
       <c r="A1495">
         <v>9</v>
       </c>
@@ -81213,7 +81282,7 @@
         <v>1712</v>
       </c>
     </row>
-    <row r="1496" spans="1:21">
+    <row r="1496" spans="1:28">
       <c r="A1496">
         <v>10</v>
       </c>
@@ -81257,7 +81326,7 @@
         <v>1713</v>
       </c>
     </row>
-    <row r="1497" spans="1:21">
+    <row r="1497" spans="1:28">
       <c r="A1497">
         <v>11</v>
       </c>
@@ -81301,7 +81370,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="1498" spans="1:21">
+    <row r="1498" spans="1:28">
       <c r="A1498">
         <v>12</v>
       </c>
@@ -81345,7 +81414,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="1499" spans="1:21">
+    <row r="1499" spans="1:28">
       <c r="A1499">
         <v>13</v>
       </c>
@@ -81389,7 +81458,7 @@
         <v>1716</v>
       </c>
     </row>
-    <row r="1500" spans="1:21">
+    <row r="1500" spans="1:28">
       <c r="A1500">
         <v>14</v>
       </c>
@@ -81433,7 +81502,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="1501" spans="1:21">
+    <row r="1501" spans="1:28">
       <c r="A1501">
         <v>15</v>
       </c>
@@ -81477,7 +81546,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="1502" spans="1:21">
+    <row r="1502" spans="1:28">
       <c r="A1502">
         <v>16</v>
       </c>
@@ -81517,11 +81586,35 @@
       <c r="N1502">
         <v>5.399</v>
       </c>
+      <c r="T1502" s="4" t="s">
+        <v>1740</v>
+      </c>
       <c r="U1502" s="4" t="s">
         <v>1719</v>
       </c>
-    </row>
-    <row r="1503" spans="1:21">
+      <c r="V1502" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="W1502" s="4">
+        <v>31</v>
+      </c>
+      <c r="X1502" s="4" t="s">
+        <v>1725</v>
+      </c>
+      <c r="Y1502" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1502" s="4">
+        <v>7</v>
+      </c>
+      <c r="AA1502" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB1502" s="53">
+        <v>0.5854166666666667</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:28">
       <c r="A1503">
         <v>17</v>
       </c>
@@ -81565,7 +81658,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="1504" spans="1:21">
+    <row r="1504" spans="1:28">
       <c r="A1504">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
updating data sheet with eclosion times
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14843" uniqueCount="1782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14854" uniqueCount="1784">
   <si>
     <t>Site</t>
   </si>
@@ -5376,6 +5376,12 @@
   </si>
   <si>
     <t>not completely eclosed when put in trikinetics, stuck into pupae</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>not put into trikinetics because it died</t>
   </si>
 </sst>
 </file>
@@ -6808,7 +6814,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11942,8 +11948,8 @@
   <dimension ref="A1:AJ1910"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE1372" sqref="AE1372"/>
+      <pane ySplit="1" topLeftCell="A1453" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC1472" sqref="AC1472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14207,10 +14213,10 @@
         <v>238</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="W39" s="4">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="X39" s="4" t="s">
         <v>184</v>
@@ -14218,11 +14224,14 @@
       <c r="Y39" s="4" t="s">
         <v>185</v>
       </c>
+      <c r="Z39" s="4">
+        <v>23</v>
+      </c>
       <c r="AA39" s="4">
         <v>2</v>
       </c>
       <c r="AB39" s="53">
-        <v>0.67222222222222217</v>
+        <v>0.47361111111111115</v>
       </c>
     </row>
     <row r="40" spans="1:31">
@@ -17789,8 +17798,32 @@
       <c r="Q107" s="17">
         <v>8.2500000000000004E-2</v>
       </c>
+      <c r="T107" s="4" t="s">
+        <v>1740</v>
+      </c>
       <c r="U107" s="4" t="s">
         <v>307</v>
+      </c>
+      <c r="V107" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="W107" s="4">
+        <v>33</v>
+      </c>
+      <c r="X107" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="Y107" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z107" s="4">
+        <v>11</v>
+      </c>
+      <c r="AA107" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB107" s="53">
+        <v>0.47291666666666665</v>
       </c>
     </row>
     <row r="108" spans="1:31">
@@ -77392,7 +77425,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="1409" spans="1:21">
+    <row r="1409" spans="1:31">
       <c r="A1409">
         <v>10</v>
       </c>
@@ -77436,7 +77469,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="1410" spans="1:21">
+    <row r="1410" spans="1:31">
       <c r="A1410">
         <v>11</v>
       </c>
@@ -77480,7 +77513,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="1411" spans="1:21">
+    <row r="1411" spans="1:31">
       <c r="A1411">
         <v>12</v>
       </c>
@@ -77524,7 +77557,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="1412" spans="1:21">
+    <row r="1412" spans="1:31">
       <c r="A1412">
         <v>13</v>
       </c>
@@ -77568,7 +77601,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="1413" spans="1:21">
+    <row r="1413" spans="1:31">
       <c r="A1413">
         <v>14</v>
       </c>
@@ -77612,7 +77645,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="1414" spans="1:21">
+    <row r="1414" spans="1:31">
       <c r="A1414">
         <v>15</v>
       </c>
@@ -77656,7 +77689,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="1415" spans="1:21">
+    <row r="1415" spans="1:31">
       <c r="A1415">
         <v>16</v>
       </c>
@@ -77700,7 +77733,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="1416" spans="1:21">
+    <row r="1416" spans="1:31">
       <c r="A1416">
         <v>17</v>
       </c>
@@ -77740,11 +77773,35 @@
       <c r="N1416">
         <v>5.9470000000000001</v>
       </c>
+      <c r="T1416" s="4" t="s">
+        <v>1740</v>
+      </c>
       <c r="U1416" s="4" t="s">
         <v>1633</v>
       </c>
-    </row>
-    <row r="1417" spans="1:21">
+      <c r="V1416" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="W1416" s="4">
+        <v>33</v>
+      </c>
+      <c r="X1416" s="4" t="s">
+        <v>1782</v>
+      </c>
+      <c r="Y1416" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC1416" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD1416" s="53">
+        <v>0.47291666666666665</v>
+      </c>
+      <c r="AE1416" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:31">
       <c r="A1417">
         <v>18</v>
       </c>
@@ -77788,7 +77845,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="1418" spans="1:21">
+    <row r="1418" spans="1:31">
       <c r="A1418">
         <v>19</v>
       </c>
@@ -77832,7 +77889,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="1419" spans="1:21">
+    <row r="1419" spans="1:31">
       <c r="A1419">
         <v>20</v>
       </c>
@@ -77876,7 +77933,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="1420" spans="1:21">
+    <row r="1420" spans="1:31">
       <c r="A1420">
         <v>21</v>
       </c>
@@ -77920,7 +77977,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="1421" spans="1:21">
+    <row r="1421" spans="1:31">
       <c r="A1421">
         <v>22</v>
       </c>
@@ -77964,7 +78021,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="1422" spans="1:21">
+    <row r="1422" spans="1:31">
       <c r="A1422">
         <v>23</v>
       </c>
@@ -78008,7 +78065,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="1423" spans="1:21">
+    <row r="1423" spans="1:31">
       <c r="A1423">
         <v>24</v>
       </c>
@@ -78052,7 +78109,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="1424" spans="1:21">
+    <row r="1424" spans="1:31">
       <c r="A1424">
         <v>25</v>
       </c>
@@ -80218,6 +80275,12 @@
       </c>
       <c r="AB1471" s="53">
         <v>0.73125000000000007</v>
+      </c>
+      <c r="AC1471" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD1471" s="53">
+        <v>0.4548611111111111</v>
       </c>
       <c r="AE1471" t="s">
         <v>1781</v>

</xml_diff>

<commit_message>
adding trikinetics data into master spreadsheet
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14854" uniqueCount="1784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14887" uniqueCount="1784">
   <si>
     <t>Site</t>
   </si>
@@ -5486,7 +5486,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="457">
+  <cellStyleXfs count="463">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5944,8 +5944,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -6089,8 +6095,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="457">
+  <cellStyles count="463">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6319,6 +6331,9 @@
     <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6547,6 +6562,9 @@
     <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6814,7 +6832,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11947,9 +11965,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1910"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1453" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC1472" sqref="AC1472"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF35" sqref="AF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11975,7 +11993,7 @@
     <col min="29" max="29" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -12886,7 +12904,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -12937,7 +12955,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -12988,7 +13006,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -13062,8 +13080,23 @@
       <c r="AB19" s="53">
         <v>0.43402777777777773</v>
       </c>
-    </row>
-    <row r="20" spans="1:28">
+      <c r="AC19" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD19" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF19">
+        <v>3</v>
+      </c>
+      <c r="AG19">
+        <v>26</v>
+      </c>
+      <c r="AH19" s="69">
+        <v>43020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -13114,7 +13147,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -13188,8 +13221,26 @@
       <c r="AB21" s="53">
         <v>0.67222222222222217</v>
       </c>
-    </row>
-    <row r="22" spans="1:28">
+      <c r="AC21" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD21" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF21">
+        <v>3</v>
+      </c>
+      <c r="AG21">
+        <v>6</v>
+      </c>
+      <c r="AH21" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI21" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -13240,7 +13291,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:35">
       <c r="A23">
         <v>23</v>
       </c>
@@ -13315,7 +13366,7 @@
         <v>0.4916666666666667</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:35">
       <c r="A24">
         <v>24</v>
       </c>
@@ -13366,7 +13417,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:35">
       <c r="A25">
         <v>25</v>
       </c>
@@ -13417,7 +13468,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:35">
       <c r="A26">
         <v>26</v>
       </c>
@@ -13468,7 +13519,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:35">
       <c r="A27">
         <v>27</v>
       </c>
@@ -13519,7 +13570,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:35">
       <c r="A28">
         <v>28</v>
       </c>
@@ -13570,7 +13621,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:35">
       <c r="A29">
         <v>29</v>
       </c>
@@ -13621,7 +13672,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:35">
       <c r="A30">
         <v>30</v>
       </c>
@@ -13696,7 +13747,7 @@
         <v>0.66111111111111109</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:35">
       <c r="A31">
         <v>31</v>
       </c>
@@ -13747,7 +13798,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:35">
       <c r="A32">
         <v>32</v>
       </c>
@@ -13972,6 +14023,12 @@
       <c r="AB35" s="53">
         <v>0.66666666666666663</v>
       </c>
+      <c r="AC35" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD35" s="53">
+        <v>0.84027777777777779</v>
+      </c>
     </row>
     <row r="36" spans="1:31">
       <c r="A36">
@@ -16327,7 +16384,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="81" spans="1:31">
+    <row r="81" spans="1:35">
       <c r="A81">
         <v>33</v>
       </c>
@@ -16401,8 +16458,26 @@
       <c r="AB81" s="53">
         <v>0.67222222222222217</v>
       </c>
-    </row>
-    <row r="82" spans="1:31">
+      <c r="AC81" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD81" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF81">
+        <v>3</v>
+      </c>
+      <c r="AG81">
+        <v>9</v>
+      </c>
+      <c r="AH81" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI81" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="82" spans="1:35">
       <c r="A82">
         <v>34</v>
       </c>
@@ -16453,7 +16528,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="83" spans="1:31">
+    <row r="83" spans="1:35">
       <c r="A83">
         <v>35</v>
       </c>
@@ -16505,7 +16580,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="84" spans="1:31">
+    <row r="84" spans="1:35">
       <c r="A84">
         <v>36</v>
       </c>
@@ -16557,7 +16632,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="1:31">
+    <row r="85" spans="1:35">
       <c r="A85">
         <v>37</v>
       </c>
@@ -16608,7 +16683,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:31">
+    <row r="86" spans="1:35">
       <c r="A86">
         <v>38</v>
       </c>
@@ -16682,8 +16757,26 @@
       <c r="AB86" s="53">
         <v>0.67222222222222217</v>
       </c>
-    </row>
-    <row r="87" spans="1:31">
+      <c r="AC86" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD86" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF86">
+        <v>3</v>
+      </c>
+      <c r="AG86">
+        <v>10</v>
+      </c>
+      <c r="AH86" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI86" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="87" spans="1:35">
       <c r="A87">
         <v>39</v>
       </c>
@@ -16734,7 +16827,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="88" spans="1:31">
+    <row r="88" spans="1:35">
       <c r="A88">
         <v>40</v>
       </c>
@@ -16785,7 +16878,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="1:31">
+    <row r="89" spans="1:35">
       <c r="A89">
         <v>41</v>
       </c>
@@ -16837,7 +16930,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="90" spans="1:31">
+    <row r="90" spans="1:35">
       <c r="A90">
         <v>45</v>
       </c>
@@ -16883,7 +16976,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="91" spans="1:31">
+    <row r="91" spans="1:35">
       <c r="A91">
         <v>47</v>
       </c>
@@ -16931,7 +17024,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="1:31">
+    <row r="92" spans="1:35">
       <c r="A92">
         <v>48</v>
       </c>
@@ -16983,7 +17076,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="1:31" s="37" customFormat="1">
+    <row r="93" spans="1:35" s="37" customFormat="1">
       <c r="A93" s="37">
         <v>50</v>
       </c>
@@ -17043,7 +17136,7 @@
       <c r="AD93" s="4"/>
       <c r="AE93"/>
     </row>
-    <row r="94" spans="1:31">
+    <row r="94" spans="1:35">
       <c r="A94">
         <v>1</v>
       </c>
@@ -17097,7 +17190,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="1:31">
+    <row r="95" spans="1:35">
       <c r="A95">
         <v>2</v>
       </c>
@@ -17148,7 +17241,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="1:31">
+    <row r="96" spans="1:35">
       <c r="A96">
         <v>3</v>
       </c>
@@ -22291,7 +22384,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="193" spans="1:31">
+    <row r="193" spans="1:35">
       <c r="A193">
         <v>40</v>
       </c>
@@ -22342,7 +22435,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="194" spans="1:31">
+    <row r="194" spans="1:35">
       <c r="A194">
         <v>41</v>
       </c>
@@ -22393,7 +22486,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="195" spans="1:31">
+    <row r="195" spans="1:35">
       <c r="A195">
         <v>42</v>
       </c>
@@ -22444,7 +22537,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="196" spans="1:31">
+    <row r="196" spans="1:35">
       <c r="A196">
         <v>43</v>
       </c>
@@ -22495,7 +22588,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="197" spans="1:31">
+    <row r="197" spans="1:35">
       <c r="A197">
         <v>44</v>
       </c>
@@ -22546,7 +22639,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="198" spans="1:31">
+    <row r="198" spans="1:35">
       <c r="A198">
         <v>45</v>
       </c>
@@ -22597,7 +22690,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="199" spans="1:31">
+    <row r="199" spans="1:35">
       <c r="A199">
         <v>46</v>
       </c>
@@ -22648,7 +22741,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="200" spans="1:31">
+    <row r="200" spans="1:35">
       <c r="A200">
         <v>47</v>
       </c>
@@ -22732,7 +22825,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="201" spans="1:31">
+    <row r="201" spans="1:35">
       <c r="A201">
         <v>48</v>
       </c>
@@ -22783,7 +22876,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="202" spans="1:31">
+    <row r="202" spans="1:35">
       <c r="A202">
         <v>49</v>
       </c>
@@ -22834,7 +22927,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="203" spans="1:31">
+    <row r="203" spans="1:35">
       <c r="A203">
         <v>50</v>
       </c>
@@ -22885,7 +22978,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="204" spans="1:31">
+    <row r="204" spans="1:35">
       <c r="A204">
         <v>51</v>
       </c>
@@ -22959,8 +23052,26 @@
       <c r="AB204" s="53">
         <v>0.70416666666666661</v>
       </c>
-    </row>
-    <row r="205" spans="1:31">
+      <c r="AC204" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD204" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF204">
+        <v>3</v>
+      </c>
+      <c r="AG204">
+        <v>5</v>
+      </c>
+      <c r="AH204" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI204" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="205" spans="1:35">
       <c r="A205">
         <v>52</v>
       </c>
@@ -23011,7 +23122,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="206" spans="1:31">
+    <row r="206" spans="1:35">
       <c r="A206">
         <v>53</v>
       </c>
@@ -23065,7 +23176,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="207" spans="1:31">
+    <row r="207" spans="1:35">
       <c r="A207">
         <v>54</v>
       </c>
@@ -23116,7 +23227,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="208" spans="1:31">
+    <row r="208" spans="1:35">
       <c r="A208">
         <v>55</v>
       </c>
@@ -23167,7 +23278,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="209" spans="1:31">
+    <row r="209" spans="1:35">
       <c r="A209">
         <v>56</v>
       </c>
@@ -23218,7 +23329,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="210" spans="1:31">
+    <row r="210" spans="1:35">
       <c r="A210">
         <v>57</v>
       </c>
@@ -23269,7 +23380,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="211" spans="1:31">
+    <row r="211" spans="1:35">
       <c r="A211">
         <v>58</v>
       </c>
@@ -23314,7 +23425,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="212" spans="1:31" s="37" customFormat="1">
+    <row r="212" spans="1:35" s="37" customFormat="1">
       <c r="A212" s="37">
         <v>59</v>
       </c>
@@ -23367,7 +23478,7 @@
       <c r="AD212" s="4"/>
       <c r="AE212"/>
     </row>
-    <row r="213" spans="1:31" s="18" customFormat="1">
+    <row r="213" spans="1:35" s="18" customFormat="1">
       <c r="A213" s="18">
         <v>1</v>
       </c>
@@ -23434,7 +23545,7 @@
       <c r="AD213" s="4"/>
       <c r="AE213"/>
     </row>
-    <row r="214" spans="1:31">
+    <row r="214" spans="1:35">
       <c r="A214">
         <v>2</v>
       </c>
@@ -23484,7 +23595,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="215" spans="1:31">
+    <row r="215" spans="1:35">
       <c r="A215">
         <v>3</v>
       </c>
@@ -23534,7 +23645,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="216" spans="1:31">
+    <row r="216" spans="1:35">
       <c r="A216">
         <v>4</v>
       </c>
@@ -23584,7 +23695,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="217" spans="1:31">
+    <row r="217" spans="1:35">
       <c r="A217">
         <v>5</v>
       </c>
@@ -23657,8 +23768,26 @@
       <c r="AB217" s="53">
         <v>0.51388888888888895</v>
       </c>
-    </row>
-    <row r="218" spans="1:31">
+      <c r="AC217" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD217" s="53">
+        <v>0.87777777777777777</v>
+      </c>
+      <c r="AF217">
+        <v>3</v>
+      </c>
+      <c r="AG217">
+        <v>25</v>
+      </c>
+      <c r="AH217" s="69">
+        <v>43021</v>
+      </c>
+      <c r="AI217" s="8">
+        <v>0.87777777777777777</v>
+      </c>
+    </row>
+    <row r="218" spans="1:35">
       <c r="A218">
         <v>6</v>
       </c>
@@ -23708,7 +23837,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="219" spans="1:31">
+    <row r="219" spans="1:35">
       <c r="A219">
         <v>7</v>
       </c>
@@ -23781,8 +23910,26 @@
       <c r="AB219" s="53">
         <v>0.42291666666666666</v>
       </c>
-    </row>
-    <row r="220" spans="1:31">
+      <c r="AC219" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD219" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF219">
+        <v>3</v>
+      </c>
+      <c r="AG219">
+        <v>3</v>
+      </c>
+      <c r="AH219" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI219" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="220" spans="1:35">
       <c r="A220">
         <v>8</v>
       </c>
@@ -23832,7 +23979,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="221" spans="1:31">
+    <row r="221" spans="1:35">
       <c r="A221">
         <v>9</v>
       </c>
@@ -23915,7 +24062,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="222" spans="1:31">
+    <row r="222" spans="1:35">
       <c r="A222">
         <v>10</v>
       </c>
@@ -23965,7 +24112,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="223" spans="1:31">
+    <row r="223" spans="1:35">
       <c r="A223">
         <v>11</v>
       </c>
@@ -24015,7 +24162,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="224" spans="1:31">
+    <row r="224" spans="1:35">
       <c r="A224">
         <v>12</v>
       </c>
@@ -24065,7 +24212,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="225" spans="1:31">
+    <row r="225" spans="1:35">
       <c r="A225">
         <v>13</v>
       </c>
@@ -24139,7 +24286,7 @@
         <v>0.51111111111111118</v>
       </c>
     </row>
-    <row r="226" spans="1:31">
+    <row r="226" spans="1:35">
       <c r="A226">
         <v>14</v>
       </c>
@@ -24189,7 +24336,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="227" spans="1:31">
+    <row r="227" spans="1:35">
       <c r="A227">
         <v>15</v>
       </c>
@@ -24239,7 +24386,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="228" spans="1:31">
+    <row r="228" spans="1:35">
       <c r="A228">
         <v>16</v>
       </c>
@@ -24322,7 +24469,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="229" spans="1:31">
+    <row r="229" spans="1:35">
       <c r="A229">
         <v>17</v>
       </c>
@@ -24405,7 +24552,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="230" spans="1:31">
+    <row r="230" spans="1:35">
       <c r="A230">
         <v>18</v>
       </c>
@@ -24455,7 +24602,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="231" spans="1:31">
+    <row r="231" spans="1:35">
       <c r="A231">
         <v>19</v>
       </c>
@@ -24505,7 +24652,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="232" spans="1:31">
+    <row r="232" spans="1:35">
       <c r="A232">
         <v>20</v>
       </c>
@@ -24555,7 +24702,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="233" spans="1:31">
+    <row r="233" spans="1:35">
       <c r="A233">
         <v>21</v>
       </c>
@@ -24628,8 +24775,26 @@
       <c r="AB233" s="53">
         <v>0.42430555555555555</v>
       </c>
-    </row>
-    <row r="234" spans="1:31">
+      <c r="AC233" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD233" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF233">
+        <v>3</v>
+      </c>
+      <c r="AG233">
+        <v>7</v>
+      </c>
+      <c r="AH233" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI233" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="234" spans="1:35">
       <c r="A234">
         <v>22</v>
       </c>
@@ -24679,7 +24844,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="235" spans="1:31">
+    <row r="235" spans="1:35">
       <c r="A235">
         <v>23</v>
       </c>
@@ -24729,7 +24894,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="236" spans="1:31">
+    <row r="236" spans="1:35">
       <c r="A236">
         <v>24</v>
       </c>
@@ -24779,7 +24944,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="237" spans="1:31">
+    <row r="237" spans="1:35">
       <c r="A237">
         <v>25</v>
       </c>
@@ -24829,7 +24994,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="238" spans="1:31">
+    <row r="238" spans="1:35">
       <c r="A238">
         <v>26</v>
       </c>
@@ -24879,7 +25044,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="239" spans="1:31">
+    <row r="239" spans="1:35">
       <c r="A239">
         <v>27</v>
       </c>
@@ -24929,7 +25094,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="240" spans="1:31">
+    <row r="240" spans="1:35">
       <c r="A240">
         <v>28</v>
       </c>
@@ -26638,7 +26803,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="273" spans="1:28">
+    <row r="273" spans="1:34">
       <c r="A273">
         <v>61</v>
       </c>
@@ -26688,7 +26853,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="274" spans="1:28">
+    <row r="274" spans="1:34">
       <c r="A274">
         <v>62</v>
       </c>
@@ -26741,7 +26906,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="275" spans="1:28">
+    <row r="275" spans="1:34">
       <c r="A275">
         <v>63</v>
       </c>
@@ -26791,7 +26956,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="276" spans="1:28">
+    <row r="276" spans="1:34">
       <c r="A276">
         <v>64</v>
       </c>
@@ -26841,7 +27006,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="277" spans="1:28">
+    <row r="277" spans="1:34">
       <c r="A277">
         <v>65</v>
       </c>
@@ -26891,7 +27056,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="278" spans="1:28">
+    <row r="278" spans="1:34">
       <c r="A278">
         <v>66</v>
       </c>
@@ -26941,7 +27106,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="279" spans="1:28">
+    <row r="279" spans="1:34">
       <c r="A279">
         <v>67</v>
       </c>
@@ -26991,7 +27156,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="280" spans="1:28">
+    <row r="280" spans="1:34">
       <c r="A280">
         <v>68</v>
       </c>
@@ -27041,7 +27206,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="281" spans="1:28">
+    <row r="281" spans="1:34">
       <c r="A281">
         <v>69</v>
       </c>
@@ -27091,7 +27256,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="282" spans="1:28">
+    <row r="282" spans="1:34">
       <c r="A282">
         <v>70</v>
       </c>
@@ -27165,7 +27330,7 @@
         <v>0.5854166666666667</v>
       </c>
     </row>
-    <row r="283" spans="1:28">
+    <row r="283" spans="1:34">
       <c r="A283">
         <v>71</v>
       </c>
@@ -27215,7 +27380,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="284" spans="1:28">
+    <row r="284" spans="1:34">
       <c r="A284">
         <v>72</v>
       </c>
@@ -27265,7 +27430,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="285" spans="1:28">
+    <row r="285" spans="1:34">
       <c r="A285">
         <v>73</v>
       </c>
@@ -27315,7 +27480,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="286" spans="1:28">
+    <row r="286" spans="1:34">
       <c r="A286">
         <v>74</v>
       </c>
@@ -27365,7 +27530,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="287" spans="1:28">
+    <row r="287" spans="1:34">
       <c r="A287">
         <v>75</v>
       </c>
@@ -27415,7 +27580,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="288" spans="1:28">
+    <row r="288" spans="1:34">
       <c r="A288">
         <v>76</v>
       </c>
@@ -27487,6 +27652,21 @@
       </c>
       <c r="AB288" s="53">
         <v>0.42430555555555555</v>
+      </c>
+      <c r="AC288" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD288" s="53">
+        <v>0.87777777777777777</v>
+      </c>
+      <c r="AF288">
+        <v>3</v>
+      </c>
+      <c r="AG288">
+        <v>8</v>
+      </c>
+      <c r="AH288" s="8">
+        <v>0.87777777777777777</v>
       </c>
     </row>
     <row r="289" spans="1:21">
@@ -31544,7 +31724,7 @@
       <c r="AD368" s="4"/>
       <c r="AE368"/>
     </row>
-    <row r="369" spans="1:28">
+    <row r="369" spans="1:35">
       <c r="A369">
         <v>1</v>
       </c>
@@ -31585,7 +31765,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="370" spans="1:28">
+    <row r="370" spans="1:35">
       <c r="A370">
         <v>2</v>
       </c>
@@ -31644,7 +31824,7 @@
         <v>0.84791666666666676</v>
       </c>
     </row>
-    <row r="371" spans="1:28">
+    <row r="371" spans="1:35">
       <c r="A371">
         <v>3</v>
       </c>
@@ -31679,7 +31859,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="372" spans="1:28">
+    <row r="372" spans="1:35">
       <c r="A372">
         <v>4</v>
       </c>
@@ -31737,8 +31917,26 @@
       <c r="AB372" s="53">
         <v>0.51388888888888895</v>
       </c>
-    </row>
-    <row r="373" spans="1:28">
+      <c r="AC372" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD372" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF372">
+        <v>3</v>
+      </c>
+      <c r="AG372">
+        <v>2</v>
+      </c>
+      <c r="AH372" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI372" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="373" spans="1:35">
       <c r="A373">
         <v>5</v>
       </c>
@@ -31773,7 +31971,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="374" spans="1:28">
+    <row r="374" spans="1:35">
       <c r="A374">
         <v>6</v>
       </c>
@@ -31808,7 +32006,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="375" spans="1:28">
+    <row r="375" spans="1:35">
       <c r="A375">
         <v>7</v>
       </c>
@@ -31843,7 +32041,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="376" spans="1:28">
+    <row r="376" spans="1:35">
       <c r="A376">
         <v>8</v>
       </c>
@@ -31878,7 +32076,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="377" spans="1:28">
+    <row r="377" spans="1:35">
       <c r="A377">
         <v>9</v>
       </c>
@@ -31913,7 +32111,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="378" spans="1:28">
+    <row r="378" spans="1:35">
       <c r="A378">
         <v>10</v>
       </c>
@@ -31948,7 +32146,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="379" spans="1:28">
+    <row r="379" spans="1:35">
       <c r="A379">
         <v>11</v>
       </c>
@@ -31983,7 +32181,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="380" spans="1:28">
+    <row r="380" spans="1:35">
       <c r="A380">
         <v>12</v>
       </c>
@@ -32018,7 +32216,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="381" spans="1:28">
+    <row r="381" spans="1:35">
       <c r="A381">
         <v>13</v>
       </c>
@@ -32053,7 +32251,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="382" spans="1:28">
+    <row r="382" spans="1:35">
       <c r="A382">
         <v>14</v>
       </c>
@@ -32088,7 +32286,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="383" spans="1:28">
+    <row r="383" spans="1:35">
       <c r="A383">
         <v>15</v>
       </c>
@@ -32123,7 +32321,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="384" spans="1:28">
+    <row r="384" spans="1:35">
       <c r="A384">
         <v>16</v>
       </c>
@@ -32158,7 +32356,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="385" spans="1:28">
+    <row r="385" spans="1:35">
       <c r="A385">
         <v>17</v>
       </c>
@@ -32193,7 +32391,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="386" spans="1:28">
+    <row r="386" spans="1:35">
       <c r="A386">
         <v>18</v>
       </c>
@@ -32228,7 +32426,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="387" spans="1:28">
+    <row r="387" spans="1:35">
       <c r="A387">
         <v>19</v>
       </c>
@@ -32263,7 +32461,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="388" spans="1:28">
+    <row r="388" spans="1:35">
       <c r="A388">
         <v>20</v>
       </c>
@@ -32298,7 +32496,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="389" spans="1:28">
+    <row r="389" spans="1:35">
       <c r="A389">
         <v>21</v>
       </c>
@@ -32333,7 +32531,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="390" spans="1:28">
+    <row r="390" spans="1:35">
       <c r="A390">
         <v>22</v>
       </c>
@@ -32391,8 +32589,26 @@
       <c r="AB390" s="53">
         <v>0.51458333333333328</v>
       </c>
-    </row>
-    <row r="391" spans="1:28">
+      <c r="AC390" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD390" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF390">
+        <v>3</v>
+      </c>
+      <c r="AG390">
+        <v>21</v>
+      </c>
+      <c r="AH390" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI390" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="391" spans="1:35">
       <c r="A391">
         <v>23</v>
       </c>
@@ -32427,7 +32643,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="392" spans="1:28">
+    <row r="392" spans="1:35">
       <c r="A392">
         <v>24</v>
       </c>
@@ -32462,7 +32678,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="393" spans="1:28">
+    <row r="393" spans="1:35">
       <c r="A393">
         <v>25</v>
       </c>
@@ -32497,7 +32713,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="394" spans="1:28">
+    <row r="394" spans="1:35">
       <c r="A394">
         <v>26</v>
       </c>
@@ -32532,7 +32748,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="395" spans="1:28">
+    <row r="395" spans="1:35">
       <c r="A395">
         <v>27</v>
       </c>
@@ -32567,7 +32783,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="396" spans="1:28">
+    <row r="396" spans="1:35">
       <c r="A396">
         <v>28</v>
       </c>
@@ -32602,7 +32818,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="397" spans="1:28">
+    <row r="397" spans="1:35">
       <c r="A397">
         <v>29</v>
       </c>
@@ -32637,7 +32853,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="398" spans="1:28">
+    <row r="398" spans="1:35">
       <c r="A398">
         <v>30</v>
       </c>
@@ -32672,7 +32888,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="399" spans="1:28">
+    <row r="399" spans="1:35">
       <c r="A399">
         <v>31</v>
       </c>
@@ -32707,7 +32923,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="400" spans="1:28">
+    <row r="400" spans="1:35">
       <c r="A400">
         <v>32</v>
       </c>
@@ -33856,7 +34072,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="433" spans="1:30">
+    <row r="433" spans="1:35">
       <c r="A433">
         <v>65</v>
       </c>
@@ -33891,7 +34107,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="434" spans="1:30">
+    <row r="434" spans="1:35">
       <c r="A434">
         <v>66</v>
       </c>
@@ -33926,7 +34142,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="435" spans="1:30">
+    <row r="435" spans="1:35">
       <c r="A435">
         <v>67</v>
       </c>
@@ -33961,7 +34177,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="436" spans="1:30">
+    <row r="436" spans="1:35">
       <c r="A436">
         <v>68</v>
       </c>
@@ -33996,7 +34212,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="437" spans="1:30">
+    <row r="437" spans="1:35">
       <c r="A437">
         <v>69</v>
       </c>
@@ -34054,8 +34270,26 @@
       <c r="AB437" s="53">
         <v>0.51527777777777783</v>
       </c>
-    </row>
-    <row r="438" spans="1:30">
+      <c r="AC437" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD437" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF437">
+        <v>3</v>
+      </c>
+      <c r="AG437">
+        <v>22</v>
+      </c>
+      <c r="AH437" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI437" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="438" spans="1:35">
       <c r="A438">
         <v>70</v>
       </c>
@@ -34081,7 +34315,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="439" spans="1:30">
+    <row r="439" spans="1:35">
       <c r="A439">
         <v>71</v>
       </c>
@@ -34116,7 +34350,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="440" spans="1:30">
+    <row r="440" spans="1:35">
       <c r="A440">
         <v>72</v>
       </c>
@@ -34151,7 +34385,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="441" spans="1:30">
+    <row r="441" spans="1:35">
       <c r="A441">
         <v>73</v>
       </c>
@@ -34186,7 +34420,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="442" spans="1:30">
+    <row r="442" spans="1:35">
       <c r="A442">
         <v>74</v>
       </c>
@@ -34221,7 +34455,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="443" spans="1:30" s="37" customFormat="1">
+    <row r="443" spans="1:35" s="37" customFormat="1">
       <c r="A443" s="37">
         <v>75</v>
       </c>
@@ -34272,7 +34506,7 @@
       <c r="AC443" s="59"/>
       <c r="AD443" s="58"/>
     </row>
-    <row r="444" spans="1:30">
+    <row r="444" spans="1:35">
       <c r="A444">
         <v>1</v>
       </c>
@@ -34313,7 +34547,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="445" spans="1:30">
+    <row r="445" spans="1:35">
       <c r="A445">
         <v>2</v>
       </c>
@@ -34348,7 +34582,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="446" spans="1:30">
+    <row r="446" spans="1:35">
       <c r="A446">
         <v>3</v>
       </c>
@@ -34383,7 +34617,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="447" spans="1:30">
+    <row r="447" spans="1:35">
       <c r="A447">
         <v>4</v>
       </c>
@@ -34418,7 +34652,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="448" spans="1:30">
+    <row r="448" spans="1:35">
       <c r="A448">
         <v>5</v>
       </c>
@@ -34453,7 +34687,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="449" spans="1:28">
+    <row r="449" spans="1:35">
       <c r="A449">
         <v>6</v>
       </c>
@@ -34488,7 +34722,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="450" spans="1:28">
+    <row r="450" spans="1:35">
       <c r="A450">
         <v>7</v>
       </c>
@@ -34523,7 +34757,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="451" spans="1:28">
+    <row r="451" spans="1:35">
       <c r="A451">
         <v>8</v>
       </c>
@@ -34558,7 +34792,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="452" spans="1:28">
+    <row r="452" spans="1:35">
       <c r="A452">
         <v>9</v>
       </c>
@@ -34593,7 +34827,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="453" spans="1:28">
+    <row r="453" spans="1:35">
       <c r="A453">
         <v>10</v>
       </c>
@@ -34628,7 +34862,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="454" spans="1:28">
+    <row r="454" spans="1:35">
       <c r="A454">
         <v>11</v>
       </c>
@@ -34686,8 +34920,26 @@
       <c r="AB454" s="53">
         <v>0.51597222222222217</v>
       </c>
-    </row>
-    <row r="455" spans="1:28">
+      <c r="AC454" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD454" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF454">
+        <v>3</v>
+      </c>
+      <c r="AG454">
+        <v>14</v>
+      </c>
+      <c r="AH454" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI454" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="455" spans="1:35">
       <c r="A455">
         <v>12</v>
       </c>
@@ -34722,7 +34974,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="456" spans="1:28">
+    <row r="456" spans="1:35">
       <c r="A456">
         <v>13</v>
       </c>
@@ -34757,7 +35009,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="457" spans="1:28">
+    <row r="457" spans="1:35">
       <c r="A457">
         <v>14</v>
       </c>
@@ -34792,7 +35044,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="458" spans="1:28">
+    <row r="458" spans="1:35">
       <c r="A458">
         <v>15</v>
       </c>
@@ -34827,7 +35079,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="459" spans="1:28">
+    <row r="459" spans="1:35">
       <c r="A459">
         <v>16</v>
       </c>
@@ -34862,7 +35114,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="460" spans="1:28">
+    <row r="460" spans="1:35">
       <c r="A460">
         <v>17</v>
       </c>
@@ -34900,7 +35152,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="461" spans="1:28">
+    <row r="461" spans="1:35">
       <c r="A461">
         <v>18</v>
       </c>
@@ -34935,7 +35187,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="462" spans="1:28">
+    <row r="462" spans="1:35">
       <c r="A462">
         <v>19</v>
       </c>
@@ -34970,7 +35222,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="463" spans="1:28">
+    <row r="463" spans="1:35">
       <c r="A463">
         <v>20</v>
       </c>
@@ -35005,7 +35257,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="464" spans="1:28">
+    <row r="464" spans="1:35">
       <c r="A464">
         <v>21</v>
       </c>
@@ -35040,7 +35292,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="465" spans="1:31">
+    <row r="465" spans="1:35">
       <c r="A465">
         <v>22</v>
       </c>
@@ -35075,7 +35327,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="466" spans="1:31">
+    <row r="466" spans="1:35">
       <c r="A466">
         <v>23</v>
       </c>
@@ -35110,7 +35362,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="467" spans="1:31">
+    <row r="467" spans="1:35">
       <c r="A467">
         <v>24</v>
       </c>
@@ -35168,8 +35420,26 @@
       <c r="AB467" s="53">
         <v>0.51666666666666672</v>
       </c>
-    </row>
-    <row r="468" spans="1:31">
+      <c r="AC467" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD467" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF467">
+        <v>3</v>
+      </c>
+      <c r="AG467">
+        <v>19</v>
+      </c>
+      <c r="AH467" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI467" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="468" spans="1:35">
       <c r="A468">
         <v>25</v>
       </c>
@@ -35204,7 +35474,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="469" spans="1:31">
+    <row r="469" spans="1:35">
       <c r="A469">
         <v>26</v>
       </c>
@@ -35257,7 +35527,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="470" spans="1:31">
+    <row r="470" spans="1:35">
       <c r="A470">
         <v>27</v>
       </c>
@@ -35292,7 +35562,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="471" spans="1:31">
+    <row r="471" spans="1:35">
       <c r="A471">
         <v>28</v>
       </c>
@@ -35327,7 +35597,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="472" spans="1:31">
+    <row r="472" spans="1:35">
       <c r="A472">
         <v>29</v>
       </c>
@@ -35362,7 +35632,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="473" spans="1:31">
+    <row r="473" spans="1:35">
       <c r="A473">
         <v>30</v>
       </c>
@@ -35397,7 +35667,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="474" spans="1:31">
+    <row r="474" spans="1:35">
       <c r="A474">
         <v>31</v>
       </c>
@@ -35432,7 +35702,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="475" spans="1:31">
+    <row r="475" spans="1:35">
       <c r="A475">
         <v>32</v>
       </c>
@@ -35467,7 +35737,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="476" spans="1:31">
+    <row r="476" spans="1:35">
       <c r="A476">
         <v>33</v>
       </c>
@@ -35502,7 +35772,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="477" spans="1:31">
+    <row r="477" spans="1:35">
       <c r="A477">
         <v>34</v>
       </c>
@@ -35560,8 +35830,26 @@
       <c r="AB477" s="53">
         <v>0.51736111111111105</v>
       </c>
-    </row>
-    <row r="478" spans="1:31">
+      <c r="AC477" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD477" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF477">
+        <v>3</v>
+      </c>
+      <c r="AG477">
+        <v>11</v>
+      </c>
+      <c r="AH477" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI477" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="478" spans="1:35">
       <c r="A478">
         <v>35</v>
       </c>
@@ -35596,7 +35884,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="479" spans="1:31">
+    <row r="479" spans="1:35">
       <c r="A479">
         <v>36</v>
       </c>
@@ -35631,7 +35919,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="480" spans="1:31">
+    <row r="480" spans="1:35">
       <c r="A480">
         <v>37</v>
       </c>
@@ -36226,7 +36514,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="497" spans="1:28">
+    <row r="497" spans="1:35">
       <c r="A497">
         <v>54</v>
       </c>
@@ -36261,7 +36549,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="498" spans="1:28">
+    <row r="498" spans="1:35">
       <c r="A498">
         <v>55</v>
       </c>
@@ -36296,7 +36584,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="499" spans="1:28">
+    <row r="499" spans="1:35">
       <c r="A499">
         <v>56</v>
       </c>
@@ -36331,7 +36619,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="500" spans="1:28">
+    <row r="500" spans="1:35">
       <c r="A500">
         <v>57</v>
       </c>
@@ -36366,7 +36654,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="501" spans="1:28">
+    <row r="501" spans="1:35">
       <c r="A501">
         <v>58</v>
       </c>
@@ -36401,7 +36689,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="502" spans="1:28">
+    <row r="502" spans="1:35">
       <c r="A502">
         <v>59</v>
       </c>
@@ -36436,7 +36724,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="503" spans="1:28">
+    <row r="503" spans="1:35">
       <c r="A503">
         <v>60</v>
       </c>
@@ -36471,7 +36759,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="504" spans="1:28">
+    <row r="504" spans="1:35">
       <c r="A504">
         <v>61</v>
       </c>
@@ -36506,7 +36794,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="505" spans="1:28">
+    <row r="505" spans="1:35">
       <c r="A505">
         <v>62</v>
       </c>
@@ -36541,7 +36829,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="506" spans="1:28">
+    <row r="506" spans="1:35">
       <c r="A506">
         <v>63</v>
       </c>
@@ -36576,7 +36864,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="507" spans="1:28">
+    <row r="507" spans="1:35">
       <c r="A507">
         <v>64</v>
       </c>
@@ -36611,7 +36899,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="508" spans="1:28">
+    <row r="508" spans="1:35">
       <c r="A508">
         <v>65</v>
       </c>
@@ -36669,8 +36957,26 @@
       <c r="AB508" s="53">
         <v>0.42430555555555555</v>
       </c>
-    </row>
-    <row r="509" spans="1:28">
+      <c r="AC508" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD508" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF508">
+        <v>2</v>
+      </c>
+      <c r="AG508">
+        <v>24</v>
+      </c>
+      <c r="AH508" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI508" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="509" spans="1:35">
       <c r="A509">
         <v>66</v>
       </c>
@@ -36705,7 +37011,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="510" spans="1:28">
+    <row r="510" spans="1:35">
       <c r="A510">
         <v>67</v>
       </c>
@@ -36740,7 +37046,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="511" spans="1:28">
+    <row r="511" spans="1:35">
       <c r="A511">
         <v>68</v>
       </c>
@@ -36775,7 +37081,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="512" spans="1:28">
+    <row r="512" spans="1:35">
       <c r="A512">
         <v>69</v>
       </c>
@@ -37450,7 +37756,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="529" spans="1:28">
+    <row r="529" spans="1:35">
       <c r="A529">
         <v>9</v>
       </c>
@@ -37494,7 +37800,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="530" spans="1:28">
+    <row r="530" spans="1:35">
       <c r="A530">
         <v>10</v>
       </c>
@@ -37538,7 +37844,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="531" spans="1:28">
+    <row r="531" spans="1:35">
       <c r="A531">
         <v>11</v>
       </c>
@@ -37605,8 +37911,27 @@
       <c r="AB531" s="53">
         <v>0.46597222222222223</v>
       </c>
-    </row>
-    <row r="532" spans="1:28">
+      <c r="AC531" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD531" s="70">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AE531" s="9"/>
+      <c r="AF531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG531" s="9">
+        <v>32</v>
+      </c>
+      <c r="AH531" s="71">
+        <v>43020</v>
+      </c>
+      <c r="AI531" s="72">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="532" spans="1:35">
       <c r="A532">
         <v>12</v>
       </c>
@@ -37673,8 +37998,26 @@
       <c r="AB532" s="53">
         <v>0.43472222222222223</v>
       </c>
-    </row>
-    <row r="533" spans="1:28">
+      <c r="AC532" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD532" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF532">
+        <v>3</v>
+      </c>
+      <c r="AG532">
+        <v>27</v>
+      </c>
+      <c r="AH532" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI532" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="533" spans="1:35">
       <c r="A533">
         <v>13</v>
       </c>
@@ -37718,7 +38061,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="534" spans="1:28">
+    <row r="534" spans="1:35">
       <c r="A534">
         <v>14</v>
       </c>
@@ -37762,7 +38105,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="535" spans="1:28">
+    <row r="535" spans="1:35">
       <c r="A535">
         <v>15</v>
       </c>
@@ -37806,7 +38149,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="536" spans="1:28">
+    <row r="536" spans="1:35">
       <c r="A536">
         <v>16</v>
       </c>
@@ -37850,7 +38193,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="537" spans="1:28">
+    <row r="537" spans="1:35">
       <c r="A537">
         <v>17</v>
       </c>
@@ -37894,7 +38237,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="538" spans="1:28">
+    <row r="538" spans="1:35">
       <c r="A538">
         <v>18</v>
       </c>
@@ -37938,7 +38281,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="539" spans="1:28">
+    <row r="539" spans="1:35">
       <c r="A539">
         <v>19</v>
       </c>
@@ -37982,7 +38325,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="540" spans="1:28">
+    <row r="540" spans="1:35">
       <c r="A540">
         <v>20</v>
       </c>
@@ -38049,8 +38392,27 @@
       <c r="AB540" s="53">
         <v>0.46597222222222223</v>
       </c>
-    </row>
-    <row r="541" spans="1:28">
+      <c r="AC540" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD540" s="70">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AE540" s="9"/>
+      <c r="AF540" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG540" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH540" s="71">
+        <v>43020</v>
+      </c>
+      <c r="AI540" s="72">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="541" spans="1:35">
       <c r="A541">
         <v>21</v>
       </c>
@@ -38094,7 +38456,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="542" spans="1:28">
+    <row r="542" spans="1:35">
       <c r="A542">
         <v>22</v>
       </c>
@@ -38138,7 +38500,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="543" spans="1:28">
+    <row r="543" spans="1:35">
       <c r="A543">
         <v>23</v>
       </c>
@@ -38182,7 +38544,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="544" spans="1:28">
+    <row r="544" spans="1:35">
       <c r="A544">
         <v>24</v>
       </c>
@@ -40350,7 +40712,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="593" spans="1:30">
+    <row r="593" spans="1:35">
       <c r="A593">
         <v>73</v>
       </c>
@@ -40417,8 +40779,26 @@
       <c r="AB593" s="53">
         <v>0.47430555555555554</v>
       </c>
-    </row>
-    <row r="594" spans="1:30">
+      <c r="AC593" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD593" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF593" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG593">
+        <v>12</v>
+      </c>
+      <c r="AH593" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI593" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="594" spans="1:35">
       <c r="A594">
         <v>74</v>
       </c>
@@ -40462,7 +40842,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="595" spans="1:30">
+    <row r="595" spans="1:35">
       <c r="A595">
         <v>75</v>
       </c>
@@ -40506,7 +40886,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="596" spans="1:30">
+    <row r="596" spans="1:35">
       <c r="A596">
         <v>76</v>
       </c>
@@ -40550,7 +40930,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="597" spans="1:30">
+    <row r="597" spans="1:35">
       <c r="A597">
         <v>77</v>
       </c>
@@ -40588,7 +40968,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="598" spans="1:30">
+    <row r="598" spans="1:35">
       <c r="A598">
         <v>78</v>
       </c>
@@ -40632,7 +41012,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="599" spans="1:30">
+    <row r="599" spans="1:35">
       <c r="A599">
         <v>1</v>
       </c>
@@ -40682,7 +41062,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="600" spans="1:30">
+    <row r="600" spans="1:35">
       <c r="A600">
         <v>2</v>
       </c>
@@ -40726,7 +41106,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="601" spans="1:30">
+    <row r="601" spans="1:35">
       <c r="A601">
         <v>3</v>
       </c>
@@ -40800,7 +41180,7 @@
         <v>0.39930555555555558</v>
       </c>
     </row>
-    <row r="602" spans="1:30">
+    <row r="602" spans="1:35">
       <c r="A602">
         <v>4</v>
       </c>
@@ -40844,7 +41224,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="603" spans="1:30">
+    <row r="603" spans="1:35">
       <c r="A603">
         <v>5</v>
       </c>
@@ -40888,7 +41268,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="604" spans="1:30">
+    <row r="604" spans="1:35">
       <c r="A604">
         <v>6</v>
       </c>
@@ -40932,7 +41312,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="605" spans="1:30">
+    <row r="605" spans="1:35">
       <c r="A605">
         <v>7</v>
       </c>
@@ -40976,7 +41356,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="606" spans="1:30">
+    <row r="606" spans="1:35">
       <c r="A606">
         <v>8</v>
       </c>
@@ -41020,7 +41400,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="607" spans="1:30">
+    <row r="607" spans="1:35">
       <c r="A607">
         <v>9</v>
       </c>
@@ -41064,7 +41444,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="608" spans="1:30">
+    <row r="608" spans="1:35">
       <c r="A608">
         <v>10</v>
       </c>
@@ -41108,7 +41488,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="609" spans="1:28">
+    <row r="609" spans="1:35">
       <c r="A609">
         <v>11</v>
       </c>
@@ -41152,7 +41532,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="610" spans="1:28">
+    <row r="610" spans="1:35">
       <c r="A610">
         <v>12</v>
       </c>
@@ -41196,7 +41576,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="611" spans="1:28">
+    <row r="611" spans="1:35">
       <c r="A611">
         <v>13</v>
       </c>
@@ -41240,7 +41620,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="612" spans="1:28">
+    <row r="612" spans="1:35">
       <c r="A612">
         <v>14</v>
       </c>
@@ -41287,7 +41667,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="613" spans="1:28">
+    <row r="613" spans="1:35">
       <c r="A613">
         <v>15</v>
       </c>
@@ -41331,7 +41711,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="614" spans="1:28">
+    <row r="614" spans="1:35">
       <c r="A614">
         <v>16</v>
       </c>
@@ -41375,7 +41755,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="615" spans="1:28">
+    <row r="615" spans="1:35">
       <c r="A615">
         <v>17</v>
       </c>
@@ -41419,7 +41799,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="616" spans="1:28">
+    <row r="616" spans="1:35">
       <c r="A616">
         <v>18</v>
       </c>
@@ -41463,7 +41843,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="617" spans="1:28">
+    <row r="617" spans="1:35">
       <c r="A617">
         <v>19</v>
       </c>
@@ -41507,7 +41887,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="618" spans="1:28">
+    <row r="618" spans="1:35">
       <c r="A618">
         <v>20</v>
       </c>
@@ -41575,7 +41955,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="619" spans="1:28">
+    <row r="619" spans="1:35">
       <c r="A619">
         <v>21</v>
       </c>
@@ -41619,7 +41999,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="620" spans="1:28">
+    <row r="620" spans="1:35">
       <c r="A620">
         <v>22</v>
       </c>
@@ -41663,7 +42043,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="621" spans="1:28">
+    <row r="621" spans="1:35">
       <c r="A621">
         <v>23</v>
       </c>
@@ -41707,7 +42087,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="622" spans="1:28">
+    <row r="622" spans="1:35">
       <c r="A622">
         <v>24</v>
       </c>
@@ -41751,7 +42131,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="623" spans="1:28">
+    <row r="623" spans="1:35">
       <c r="A623">
         <v>25</v>
       </c>
@@ -41795,7 +42175,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="624" spans="1:28">
+    <row r="624" spans="1:35">
       <c r="A624">
         <v>26</v>
       </c>
@@ -41861,6 +42241,25 @@
       </c>
       <c r="AB624" s="53">
         <v>0.46666666666666662</v>
+      </c>
+      <c r="AC624" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD624" s="70">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AE624" s="9"/>
+      <c r="AF624" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG624" s="9">
+        <v>18</v>
+      </c>
+      <c r="AH624" s="71">
+        <v>43020</v>
+      </c>
+      <c r="AI624" s="72">
+        <v>0.84583333333333333</v>
       </c>
     </row>
     <row r="625" spans="1:21">
@@ -42567,7 +42966,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="641" spans="1:28">
+    <row r="641" spans="1:35">
       <c r="A641">
         <v>43</v>
       </c>
@@ -42611,7 +43010,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="642" spans="1:28">
+    <row r="642" spans="1:35">
       <c r="A642">
         <v>44</v>
       </c>
@@ -42655,7 +43054,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="643" spans="1:28">
+    <row r="643" spans="1:35">
       <c r="A643">
         <v>45</v>
       </c>
@@ -42699,7 +43098,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="644" spans="1:28">
+    <row r="644" spans="1:35">
       <c r="A644">
         <v>46</v>
       </c>
@@ -42766,8 +43165,26 @@
       <c r="AB644" s="53">
         <v>0.47361111111111115</v>
       </c>
-    </row>
-    <row r="645" spans="1:28">
+      <c r="AC644" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD644" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF644">
+        <v>3</v>
+      </c>
+      <c r="AG644">
+        <v>13</v>
+      </c>
+      <c r="AH644" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI644" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="645" spans="1:35">
       <c r="A645">
         <v>47</v>
       </c>
@@ -42811,7 +43228,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="646" spans="1:28">
+    <row r="646" spans="1:35">
       <c r="A646">
         <v>48</v>
       </c>
@@ -42855,7 +43272,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="647" spans="1:28">
+    <row r="647" spans="1:35">
       <c r="A647">
         <v>49</v>
       </c>
@@ -42922,8 +43339,26 @@
       <c r="AB647" s="53">
         <v>0.43333333333333335</v>
       </c>
-    </row>
-    <row r="648" spans="1:28">
+      <c r="AC647" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD647" s="53">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AF647">
+        <v>3</v>
+      </c>
+      <c r="AG647">
+        <v>28</v>
+      </c>
+      <c r="AH647" s="69">
+        <v>43020</v>
+      </c>
+      <c r="AI647" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="648" spans="1:35">
       <c r="A648">
         <v>50</v>
       </c>
@@ -42967,7 +43402,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="649" spans="1:28">
+    <row r="649" spans="1:35">
       <c r="A649">
         <v>51</v>
       </c>
@@ -43011,7 +43446,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="650" spans="1:28">
+    <row r="650" spans="1:35">
       <c r="A650">
         <v>52</v>
       </c>
@@ -43055,7 +43490,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="651" spans="1:28">
+    <row r="651" spans="1:35">
       <c r="A651">
         <v>53</v>
       </c>
@@ -43099,7 +43534,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="652" spans="1:28">
+    <row r="652" spans="1:35">
       <c r="A652">
         <v>54</v>
       </c>
@@ -43143,7 +43578,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="653" spans="1:28">
+    <row r="653" spans="1:35">
       <c r="A653">
         <v>55</v>
       </c>
@@ -43190,7 +43625,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="654" spans="1:28">
+    <row r="654" spans="1:35">
       <c r="A654">
         <v>56</v>
       </c>
@@ -43234,7 +43669,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="655" spans="1:28">
+    <row r="655" spans="1:35">
       <c r="A655">
         <v>57</v>
       </c>
@@ -43278,7 +43713,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="656" spans="1:28">
+    <row r="656" spans="1:35">
       <c r="A656">
         <v>58</v>
       </c>
@@ -45454,7 +45889,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="705" spans="1:28">
+    <row r="705" spans="1:35">
       <c r="A705">
         <v>28</v>
       </c>
@@ -45498,7 +45933,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="706" spans="1:28">
+    <row r="706" spans="1:35">
       <c r="A706">
         <v>29</v>
       </c>
@@ -45542,7 +45977,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="707" spans="1:28">
+    <row r="707" spans="1:35">
       <c r="A707">
         <v>30</v>
       </c>
@@ -45586,7 +46021,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="708" spans="1:28">
+    <row r="708" spans="1:35">
       <c r="A708">
         <v>31</v>
       </c>
@@ -45653,8 +46088,27 @@
       <c r="AB708" s="53">
         <v>0.4381944444444445</v>
       </c>
-    </row>
-    <row r="709" spans="1:28">
+      <c r="AC708" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD708" s="70">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AE708" s="9"/>
+      <c r="AF708" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG708" s="9">
+        <v>15</v>
+      </c>
+      <c r="AH708" s="71">
+        <v>43020</v>
+      </c>
+      <c r="AI708" s="72">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="709" spans="1:35">
       <c r="A709">
         <v>32</v>
       </c>
@@ -45692,7 +46146,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="710" spans="1:28">
+    <row r="710" spans="1:35">
       <c r="A710">
         <v>33</v>
       </c>
@@ -45730,7 +46184,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="711" spans="1:28">
+    <row r="711" spans="1:35">
       <c r="A711">
         <v>34</v>
       </c>
@@ -45774,7 +46228,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="712" spans="1:28">
+    <row r="712" spans="1:35">
       <c r="A712">
         <v>35</v>
       </c>
@@ -45818,7 +46272,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="713" spans="1:28">
+    <row r="713" spans="1:35">
       <c r="A713">
         <v>36</v>
       </c>
@@ -45862,7 +46316,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="714" spans="1:28">
+    <row r="714" spans="1:35">
       <c r="A714">
         <v>37</v>
       </c>
@@ -45906,7 +46360,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="715" spans="1:28">
+    <row r="715" spans="1:35">
       <c r="A715">
         <v>38</v>
       </c>
@@ -45950,7 +46404,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="716" spans="1:28">
+    <row r="716" spans="1:35">
       <c r="A716">
         <v>39</v>
       </c>
@@ -45994,7 +46448,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="717" spans="1:28">
+    <row r="717" spans="1:35">
       <c r="A717">
         <v>40</v>
       </c>
@@ -46038,7 +46492,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="718" spans="1:28">
+    <row r="718" spans="1:35">
       <c r="A718">
         <v>41</v>
       </c>
@@ -46082,7 +46536,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="719" spans="1:28">
+    <row r="719" spans="1:35">
       <c r="A719">
         <v>42</v>
       </c>
@@ -46126,7 +46580,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="720" spans="1:28">
+    <row r="720" spans="1:35">
       <c r="A720">
         <v>43</v>
       </c>
@@ -46170,7 +46624,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="721" spans="1:28">
+    <row r="721" spans="1:35">
       <c r="A721">
         <v>44</v>
       </c>
@@ -46214,7 +46668,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="722" spans="1:28">
+    <row r="722" spans="1:35">
       <c r="A722">
         <v>45</v>
       </c>
@@ -46258,7 +46712,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="723" spans="1:28">
+    <row r="723" spans="1:35">
       <c r="A723">
         <v>46</v>
       </c>
@@ -46302,7 +46756,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="724" spans="1:28">
+    <row r="724" spans="1:35">
       <c r="A724">
         <v>47</v>
       </c>
@@ -46346,7 +46800,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="725" spans="1:28">
+    <row r="725" spans="1:35">
       <c r="A725">
         <v>48</v>
       </c>
@@ -46390,7 +46844,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="726" spans="1:28">
+    <row r="726" spans="1:35">
       <c r="A726">
         <v>49</v>
       </c>
@@ -46434,7 +46888,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="727" spans="1:28">
+    <row r="727" spans="1:35">
       <c r="A727">
         <v>50</v>
       </c>
@@ -46478,7 +46932,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="728" spans="1:28">
+    <row r="728" spans="1:35">
       <c r="A728">
         <v>51</v>
       </c>
@@ -46522,7 +46976,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="729" spans="1:28">
+    <row r="729" spans="1:35">
       <c r="A729">
         <v>52</v>
       </c>
@@ -46566,7 +47020,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="730" spans="1:28">
+    <row r="730" spans="1:35">
       <c r="A730">
         <v>53</v>
       </c>
@@ -46610,7 +47064,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="731" spans="1:28">
+    <row r="731" spans="1:35">
       <c r="A731">
         <v>54</v>
       </c>
@@ -46654,7 +47108,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="732" spans="1:28">
+    <row r="732" spans="1:35">
       <c r="A732">
         <v>55</v>
       </c>
@@ -46701,7 +47155,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="733" spans="1:28">
+    <row r="733" spans="1:35">
       <c r="A733">
         <v>56</v>
       </c>
@@ -46768,8 +47222,27 @@
       <c r="AB733" s="53">
         <v>0.46666666666666662</v>
       </c>
-    </row>
-    <row r="734" spans="1:28">
+      <c r="AC733" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD733" s="70">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AE733" s="9"/>
+      <c r="AF733" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG733" s="9">
+        <v>17</v>
+      </c>
+      <c r="AH733" s="71">
+        <v>43020</v>
+      </c>
+      <c r="AI733" s="72">
+        <v>0.84583333333333333</v>
+      </c>
+    </row>
+    <row r="734" spans="1:35">
       <c r="A734">
         <v>57</v>
       </c>
@@ -46813,7 +47286,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="735" spans="1:28">
+    <row r="735" spans="1:35">
       <c r="A735">
         <v>58</v>
       </c>
@@ -46857,7 +47330,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="736" spans="1:28">
+    <row r="736" spans="1:35">
       <c r="A736">
         <v>59</v>
       </c>
@@ -47617,7 +48090,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="753" spans="1:28">
+    <row r="753" spans="1:35">
       <c r="A753">
         <v>6</v>
       </c>
@@ -47661,7 +48134,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="754" spans="1:28">
+    <row r="754" spans="1:35">
       <c r="A754">
         <v>7</v>
       </c>
@@ -47705,7 +48178,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="755" spans="1:28">
+    <row r="755" spans="1:35">
       <c r="A755">
         <v>8</v>
       </c>
@@ -47749,7 +48222,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="756" spans="1:28">
+    <row r="756" spans="1:35">
       <c r="A756">
         <v>9</v>
       </c>
@@ -47793,7 +48266,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="757" spans="1:28">
+    <row r="757" spans="1:35">
       <c r="A757">
         <v>10</v>
       </c>
@@ -47837,7 +48310,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="758" spans="1:28">
+    <row r="758" spans="1:35">
       <c r="A758">
         <v>11</v>
       </c>
@@ -47881,7 +48354,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="759" spans="1:28">
+    <row r="759" spans="1:35">
       <c r="A759">
         <v>12</v>
       </c>
@@ -47925,7 +48398,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="760" spans="1:28">
+    <row r="760" spans="1:35">
       <c r="A760">
         <v>13</v>
       </c>
@@ -47969,7 +48442,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="761" spans="1:28">
+    <row r="761" spans="1:35">
       <c r="A761">
         <v>14</v>
       </c>
@@ -48013,7 +48486,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="762" spans="1:28">
+    <row r="762" spans="1:35">
       <c r="A762">
         <v>15</v>
       </c>
@@ -48057,7 +48530,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="763" spans="1:28">
+    <row r="763" spans="1:35">
       <c r="A763">
         <v>16</v>
       </c>
@@ -48101,7 +48574,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="764" spans="1:28">
+    <row r="764" spans="1:35">
       <c r="A764">
         <v>17</v>
       </c>
@@ -48145,7 +48618,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="765" spans="1:28">
+    <row r="765" spans="1:35">
       <c r="A765">
         <v>18</v>
       </c>
@@ -48189,7 +48662,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="766" spans="1:28">
+    <row r="766" spans="1:35">
       <c r="A766">
         <v>19</v>
       </c>
@@ -48257,8 +48730,26 @@
       <c r="AB766" s="53">
         <v>0.60416666666666663</v>
       </c>
-    </row>
-    <row r="767" spans="1:28">
+      <c r="AC766" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD766" s="53">
+        <v>0.87569444444444444</v>
+      </c>
+      <c r="AF766">
+        <v>3</v>
+      </c>
+      <c r="AG766">
+        <v>20</v>
+      </c>
+      <c r="AH766" s="69">
+        <v>43021</v>
+      </c>
+      <c r="AI766" s="8">
+        <v>0.87916666666666676</v>
+      </c>
+    </row>
+    <row r="767" spans="1:35">
       <c r="A767">
         <v>20</v>
       </c>
@@ -48302,7 +48793,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="768" spans="1:28">
+    <row r="768" spans="1:35">
       <c r="A768">
         <v>21</v>
       </c>
@@ -48346,7 +48837,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="769" spans="1:28">
+    <row r="769" spans="1:35">
       <c r="A769">
         <v>22</v>
       </c>
@@ -48390,7 +48881,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="770" spans="1:28">
+    <row r="770" spans="1:35">
       <c r="A770">
         <v>23</v>
       </c>
@@ -48434,7 +48925,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="771" spans="1:28">
+    <row r="771" spans="1:35">
       <c r="A771">
         <v>24</v>
       </c>
@@ -48478,7 +48969,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="772" spans="1:28">
+    <row r="772" spans="1:35">
       <c r="A772">
         <v>25</v>
       </c>
@@ -48522,7 +49013,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="773" spans="1:28">
+    <row r="773" spans="1:35">
       <c r="A773">
         <v>26</v>
       </c>
@@ -48566,7 +49057,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="774" spans="1:28">
+    <row r="774" spans="1:35">
       <c r="A774">
         <v>27</v>
       </c>
@@ -48610,7 +49101,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="775" spans="1:28">
+    <row r="775" spans="1:35">
       <c r="A775">
         <v>28</v>
       </c>
@@ -48654,7 +49145,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="776" spans="1:28">
+    <row r="776" spans="1:35">
       <c r="A776">
         <v>29</v>
       </c>
@@ -48698,7 +49189,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="777" spans="1:28">
+    <row r="777" spans="1:35">
       <c r="A777">
         <v>30</v>
       </c>
@@ -48766,8 +49257,26 @@
       <c r="AB777" s="53">
         <v>0.60416666666666663</v>
       </c>
-    </row>
-    <row r="778" spans="1:28">
+      <c r="AC777" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD777" s="53">
+        <v>0.87569444444444444</v>
+      </c>
+      <c r="AF777">
+        <v>3</v>
+      </c>
+      <c r="AG777">
+        <v>31</v>
+      </c>
+      <c r="AH777" s="69">
+        <v>43021</v>
+      </c>
+      <c r="AI777" s="8">
+        <v>0.87916666666666676</v>
+      </c>
+    </row>
+    <row r="778" spans="1:35">
       <c r="A778">
         <v>31</v>
       </c>
@@ -48811,7 +49320,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="779" spans="1:28">
+    <row r="779" spans="1:35">
       <c r="A779">
         <v>32</v>
       </c>
@@ -48855,7 +49364,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="780" spans="1:28">
+    <row r="780" spans="1:35">
       <c r="A780">
         <v>33</v>
       </c>
@@ -48899,7 +49408,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="781" spans="1:28">
+    <row r="781" spans="1:35">
       <c r="A781">
         <v>34</v>
       </c>
@@ -48943,7 +49452,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="782" spans="1:28">
+    <row r="782" spans="1:35">
       <c r="A782">
         <v>35</v>
       </c>
@@ -48987,7 +49496,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="783" spans="1:28">
+    <row r="783" spans="1:35">
       <c r="A783">
         <v>36</v>
       </c>
@@ -49031,7 +49540,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="784" spans="1:28">
+    <row r="784" spans="1:35">
       <c r="A784">
         <v>37</v>
       </c>
@@ -49075,7 +49584,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="785" spans="1:31">
+    <row r="785" spans="1:35">
       <c r="A785">
         <v>38</v>
       </c>
@@ -49119,7 +49628,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="786" spans="1:31">
+    <row r="786" spans="1:35">
       <c r="A786">
         <v>39</v>
       </c>
@@ -49163,7 +49672,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="787" spans="1:31">
+    <row r="787" spans="1:35">
       <c r="A787">
         <v>40</v>
       </c>
@@ -49207,7 +49716,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="788" spans="1:31">
+    <row r="788" spans="1:35">
       <c r="A788">
         <v>41</v>
       </c>
@@ -49254,7 +49763,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="789" spans="1:31">
+    <row r="789" spans="1:35">
       <c r="A789">
         <v>42</v>
       </c>
@@ -49298,7 +49807,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="790" spans="1:31">
+    <row r="790" spans="1:35">
       <c r="A790">
         <v>43</v>
       </c>
@@ -49342,7 +49851,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="791" spans="1:31">
+    <row r="791" spans="1:35">
       <c r="A791">
         <v>44</v>
       </c>
@@ -49386,7 +49895,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="792" spans="1:31">
+    <row r="792" spans="1:35">
       <c r="A792">
         <v>45</v>
       </c>
@@ -49430,7 +49939,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="793" spans="1:31">
+    <row r="793" spans="1:35">
       <c r="A793">
         <v>46</v>
       </c>
@@ -49474,7 +49983,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="794" spans="1:31">
+    <row r="794" spans="1:35">
       <c r="A794">
         <v>47</v>
       </c>
@@ -49518,7 +50027,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="795" spans="1:31">
+    <row r="795" spans="1:35">
       <c r="A795">
         <v>48</v>
       </c>
@@ -49562,7 +50071,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="796" spans="1:31">
+    <row r="796" spans="1:35">
       <c r="A796">
         <v>49</v>
       </c>
@@ -49606,7 +50115,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="797" spans="1:31">
+    <row r="797" spans="1:35">
       <c r="A797">
         <v>50</v>
       </c>
@@ -49650,7 +50159,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="798" spans="1:31">
+    <row r="798" spans="1:35">
       <c r="A798">
         <v>51</v>
       </c>
@@ -49727,7 +50236,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="799" spans="1:31">
+    <row r="799" spans="1:35">
       <c r="A799">
         <v>52</v>
       </c>
@@ -49804,7 +50313,7 @@
         <v>1777</v>
       </c>
     </row>
-    <row r="800" spans="1:31">
+    <row r="800" spans="1:35">
       <c r="A800">
         <v>53</v>
       </c>
@@ -49870,6 +50379,25 @@
       </c>
       <c r="AB800" s="53">
         <v>0.43402777777777773</v>
+      </c>
+      <c r="AC800" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD800" s="70">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="AE800" s="9"/>
+      <c r="AF800" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG800" s="9">
+        <v>16</v>
+      </c>
+      <c r="AH800" s="71">
+        <v>43020</v>
+      </c>
+      <c r="AI800" s="72">
+        <v>0.84583333333333333</v>
       </c>
     </row>
     <row r="801" spans="1:21">
@@ -52025,7 +52553,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="849" spans="1:28">
+    <row r="849" spans="1:35">
       <c r="A849">
         <v>30</v>
       </c>
@@ -52069,7 +52597,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="850" spans="1:28">
+    <row r="850" spans="1:35">
       <c r="A850">
         <v>31</v>
       </c>
@@ -52113,7 +52641,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="851" spans="1:28">
+    <row r="851" spans="1:35">
       <c r="A851">
         <v>32</v>
       </c>
@@ -52157,7 +52685,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="852" spans="1:28">
+    <row r="852" spans="1:35">
       <c r="A852">
         <v>33</v>
       </c>
@@ -52201,7 +52729,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="853" spans="1:28">
+    <row r="853" spans="1:35">
       <c r="A853">
         <v>34</v>
       </c>
@@ -52245,7 +52773,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="854" spans="1:28">
+    <row r="854" spans="1:35">
       <c r="A854">
         <v>35</v>
       </c>
@@ -52289,7 +52817,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="855" spans="1:28">
+    <row r="855" spans="1:35">
       <c r="A855">
         <v>36</v>
       </c>
@@ -52333,7 +52861,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="856" spans="1:28">
+    <row r="856" spans="1:35">
       <c r="A856">
         <v>37</v>
       </c>
@@ -52377,7 +52905,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="857" spans="1:28">
+    <row r="857" spans="1:35">
       <c r="A857">
         <v>38</v>
       </c>
@@ -52421,7 +52949,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="858" spans="1:28">
+    <row r="858" spans="1:35">
       <c r="A858">
         <v>39</v>
       </c>
@@ -52465,7 +52993,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="859" spans="1:28">
+    <row r="859" spans="1:35">
       <c r="A859">
         <v>40</v>
       </c>
@@ -52533,8 +53061,27 @@
       <c r="AB859" s="53">
         <v>0.60486111111111118</v>
       </c>
-    </row>
-    <row r="860" spans="1:28">
+      <c r="AC859" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD859" s="70">
+        <v>0.87569444444444444</v>
+      </c>
+      <c r="AE859" s="9"/>
+      <c r="AF859" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG859" s="9">
+        <v>30</v>
+      </c>
+      <c r="AH859" s="71">
+        <v>43021</v>
+      </c>
+      <c r="AI859" s="72">
+        <v>0.87916666666666676</v>
+      </c>
+    </row>
+    <row r="860" spans="1:35">
       <c r="A860">
         <v>41</v>
       </c>
@@ -52578,7 +53125,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="861" spans="1:28">
+    <row r="861" spans="1:35">
       <c r="A861">
         <v>42</v>
       </c>
@@ -52622,7 +53169,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="862" spans="1:28">
+    <row r="862" spans="1:35">
       <c r="A862">
         <v>43</v>
       </c>
@@ -52666,7 +53213,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="863" spans="1:28">
+    <row r="863" spans="1:35">
       <c r="A863">
         <v>44</v>
       </c>
@@ -52710,7 +53257,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="864" spans="1:28">
+    <row r="864" spans="1:35">
       <c r="A864">
         <v>45</v>
       </c>
@@ -55658,7 +56205,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="929" spans="1:28">
+    <row r="929" spans="1:35">
       <c r="A929">
         <v>33</v>
       </c>
@@ -55702,7 +56249,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="930" spans="1:28">
+    <row r="930" spans="1:35">
       <c r="A930">
         <v>34</v>
       </c>
@@ -55746,7 +56293,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="931" spans="1:28">
+    <row r="931" spans="1:35">
       <c r="A931">
         <v>35</v>
       </c>
@@ -55790,7 +56337,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="932" spans="1:28">
+    <row r="932" spans="1:35">
       <c r="A932">
         <v>36</v>
       </c>
@@ -55834,7 +56381,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="933" spans="1:28">
+    <row r="933" spans="1:35">
       <c r="A933">
         <v>37</v>
       </c>
@@ -55878,7 +56425,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="934" spans="1:28">
+    <row r="934" spans="1:35">
       <c r="A934">
         <v>38</v>
       </c>
@@ -55922,7 +56469,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="935" spans="1:28">
+    <row r="935" spans="1:35">
       <c r="A935">
         <v>39</v>
       </c>
@@ -55966,7 +56513,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="936" spans="1:28">
+    <row r="936" spans="1:35">
       <c r="A936">
         <v>40</v>
       </c>
@@ -56010,7 +56557,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="937" spans="1:28">
+    <row r="937" spans="1:35">
       <c r="A937">
         <v>41</v>
       </c>
@@ -56054,7 +56601,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="938" spans="1:28">
+    <row r="938" spans="1:35">
       <c r="A938">
         <v>42</v>
       </c>
@@ -56098,7 +56645,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="939" spans="1:28">
+    <row r="939" spans="1:35">
       <c r="A939">
         <v>43</v>
       </c>
@@ -56166,8 +56713,27 @@
       <c r="AB939" s="53">
         <v>0.60486111111111118</v>
       </c>
-    </row>
-    <row r="940" spans="1:28">
+      <c r="AC939" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD939" s="70">
+        <v>0.87569444444444444</v>
+      </c>
+      <c r="AE939" s="9"/>
+      <c r="AF939" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG939" s="9">
+        <v>29</v>
+      </c>
+      <c r="AH939" s="71">
+        <v>43021</v>
+      </c>
+      <c r="AI939" s="72">
+        <v>0.87916666666666676</v>
+      </c>
+    </row>
+    <row r="940" spans="1:35">
       <c r="A940">
         <v>44</v>
       </c>
@@ -56211,7 +56777,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="941" spans="1:28">
+    <row r="941" spans="1:35">
       <c r="A941">
         <v>45</v>
       </c>
@@ -56255,7 +56821,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="942" spans="1:28">
+    <row r="942" spans="1:35">
       <c r="A942">
         <v>46</v>
       </c>
@@ -56299,7 +56865,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="943" spans="1:28">
+    <row r="943" spans="1:35">
       <c r="A943">
         <v>47</v>
       </c>
@@ -56343,7 +56909,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="944" spans="1:28">
+    <row r="944" spans="1:35">
       <c r="A944">
         <v>48</v>
       </c>
@@ -62909,7 +63475,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="1089" spans="1:28">
+    <row r="1089" spans="1:35">
       <c r="A1089">
         <v>42</v>
       </c>
@@ -62953,7 +63519,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="1090" spans="1:28">
+    <row r="1090" spans="1:35">
       <c r="A1090">
         <v>43</v>
       </c>
@@ -62997,7 +63563,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="1091" spans="1:28">
+    <row r="1091" spans="1:35">
       <c r="A1091">
         <v>44</v>
       </c>
@@ -63041,7 +63607,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="1092" spans="1:28">
+    <row r="1092" spans="1:35">
       <c r="A1092">
         <v>45</v>
       </c>
@@ -63109,7 +63675,7 @@
         <v>0.72638888888888886</v>
       </c>
     </row>
-    <row r="1093" spans="1:28">
+    <row r="1093" spans="1:35">
       <c r="A1093">
         <v>46</v>
       </c>
@@ -63153,7 +63719,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="1094" spans="1:28">
+    <row r="1094" spans="1:35">
       <c r="A1094">
         <v>47</v>
       </c>
@@ -63197,7 +63763,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="1095" spans="1:28">
+    <row r="1095" spans="1:35">
       <c r="A1095">
         <v>48</v>
       </c>
@@ -63241,7 +63807,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="1096" spans="1:28">
+    <row r="1096" spans="1:35">
       <c r="A1096">
         <v>49</v>
       </c>
@@ -63285,7 +63851,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="1097" spans="1:28">
+    <row r="1097" spans="1:35">
       <c r="A1097">
         <v>50</v>
       </c>
@@ -63353,8 +63919,27 @@
       <c r="AB1097" s="53">
         <v>0.60555555555555551</v>
       </c>
-    </row>
-    <row r="1098" spans="1:28">
+      <c r="AC1097" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD1097" s="70">
+        <v>0.87569444444444444</v>
+      </c>
+      <c r="AE1097" s="9"/>
+      <c r="AF1097" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG1097" s="9">
+        <v>25</v>
+      </c>
+      <c r="AH1097" s="71">
+        <v>43021</v>
+      </c>
+      <c r="AI1097" s="72">
+        <v>0.87916666666666676</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:35">
       <c r="A1098">
         <v>51</v>
       </c>
@@ -63401,7 +63986,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="1099" spans="1:28">
+    <row r="1099" spans="1:35">
       <c r="A1099">
         <v>52</v>
       </c>
@@ -63448,7 +64033,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="1100" spans="1:28">
+    <row r="1100" spans="1:35">
       <c r="A1100">
         <v>53</v>
       </c>
@@ -63492,7 +64077,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="1101" spans="1:28">
+    <row r="1101" spans="1:35">
       <c r="A1101">
         <v>54</v>
       </c>
@@ -63536,7 +64121,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="1102" spans="1:28">
+    <row r="1102" spans="1:35">
       <c r="A1102">
         <v>55</v>
       </c>
@@ -63580,7 +64165,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="1103" spans="1:28">
+    <row r="1103" spans="1:35">
       <c r="A1103">
         <v>56</v>
       </c>
@@ -63624,7 +64209,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="1104" spans="1:28">
+    <row r="1104" spans="1:35">
       <c r="A1104">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
updating trikinetics data into master spreadsheet!
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14887" uniqueCount="1784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14894" uniqueCount="1784">
   <si>
     <t>Site</t>
   </si>
@@ -5486,8 +5486,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="463">
+  <cellStyleXfs count="465">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6102,7 +6104,7 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="463">
+  <cellStyles count="465">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6334,6 +6336,7 @@
     <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6565,6 +6568,7 @@
     <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6832,7 +6836,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11965,9 +11969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1910"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="T1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF35" sqref="AF35"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1089" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X1107" sqref="X1107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13847,7 +13851,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:35">
       <c r="A33">
         <v>33</v>
       </c>
@@ -13898,7 +13902,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:35">
       <c r="A34">
         <v>34</v>
       </c>
@@ -13949,7 +13953,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:35">
       <c r="A35">
         <v>35</v>
       </c>
@@ -14029,8 +14033,20 @@
       <c r="AD35" s="53">
         <v>0.84027777777777779</v>
       </c>
-    </row>
-    <row r="36" spans="1:31">
+      <c r="AF35">
+        <v>4</v>
+      </c>
+      <c r="AG35">
+        <v>5</v>
+      </c>
+      <c r="AH35" s="69">
+        <v>43022</v>
+      </c>
+      <c r="AI35" s="8">
+        <v>0.84027777777777779</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35">
       <c r="A36">
         <v>36</v>
       </c>
@@ -14114,7 +14130,7 @@
         <v>1757</v>
       </c>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:35">
       <c r="A37">
         <v>37</v>
       </c>
@@ -14165,7 +14181,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:35">
       <c r="A38">
         <v>38</v>
       </c>
@@ -14216,7 +14232,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:35">
       <c r="A39">
         <v>39</v>
       </c>
@@ -14291,7 +14307,7 @@
         <v>0.47361111111111115</v>
       </c>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:35">
       <c r="A40">
         <v>40</v>
       </c>
@@ -14342,7 +14358,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:35">
       <c r="A41">
         <v>41</v>
       </c>
@@ -14393,7 +14409,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:35">
       <c r="A42">
         <v>42</v>
       </c>
@@ -14444,7 +14460,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:35">
       <c r="A43">
         <v>43</v>
       </c>
@@ -14495,7 +14511,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:35">
       <c r="A44">
         <v>44</v>
       </c>
@@ -14547,7 +14563,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:35">
       <c r="A45">
         <v>45</v>
       </c>
@@ -14592,7 +14608,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:35">
       <c r="A46">
         <v>46</v>
       </c>
@@ -14643,7 +14659,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:35">
       <c r="A47">
         <v>47</v>
       </c>
@@ -14694,7 +14710,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:35">
       <c r="A48">
         <v>48</v>
       </c>
@@ -41954,6 +41970,24 @@
       <c r="AB618" s="53">
         <v>0.66666666666666663</v>
       </c>
+      <c r="AC618" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD618" s="53">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="AF618">
+        <v>4</v>
+      </c>
+      <c r="AG618">
+        <v>31</v>
+      </c>
+      <c r="AH618" s="69">
+        <v>43022</v>
+      </c>
+      <c r="AI618" s="8">
+        <v>0.84027777777777779</v>
+      </c>
     </row>
     <row r="619" spans="1:35">
       <c r="A619">
@@ -51825,7 +51859,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="833" spans="1:28">
+    <row r="833" spans="1:35">
       <c r="A833">
         <v>14</v>
       </c>
@@ -51869,7 +51903,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="834" spans="1:28">
+    <row r="834" spans="1:35">
       <c r="A834">
         <v>15</v>
       </c>
@@ -51913,7 +51947,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="835" spans="1:28">
+    <row r="835" spans="1:35">
       <c r="A835">
         <v>16</v>
       </c>
@@ -51957,7 +51991,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="836" spans="1:28">
+    <row r="836" spans="1:35">
       <c r="A836">
         <v>17</v>
       </c>
@@ -52001,7 +52035,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="837" spans="1:28">
+    <row r="837" spans="1:35">
       <c r="A837">
         <v>18</v>
       </c>
@@ -52045,7 +52079,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="838" spans="1:28">
+    <row r="838" spans="1:35">
       <c r="A838">
         <v>19</v>
       </c>
@@ -52089,7 +52123,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="839" spans="1:28">
+    <row r="839" spans="1:35">
       <c r="A839">
         <v>20</v>
       </c>
@@ -52133,7 +52167,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="840" spans="1:28">
+    <row r="840" spans="1:35">
       <c r="A840">
         <v>21</v>
       </c>
@@ -52200,8 +52234,27 @@
       <c r="AB840" s="53">
         <v>0.66805555555555562</v>
       </c>
-    </row>
-    <row r="841" spans="1:28">
+      <c r="AC840" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD840" s="70">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="AE840" s="9"/>
+      <c r="AF840" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG840" s="9">
+        <v>16</v>
+      </c>
+      <c r="AH840" s="71">
+        <v>43022</v>
+      </c>
+      <c r="AI840" s="72">
+        <v>0.84027777777777779</v>
+      </c>
+    </row>
+    <row r="841" spans="1:35">
       <c r="A841">
         <v>22</v>
       </c>
@@ -52245,7 +52298,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="842" spans="1:28">
+    <row r="842" spans="1:35">
       <c r="A842">
         <v>23</v>
       </c>
@@ -52289,7 +52342,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="843" spans="1:28">
+    <row r="843" spans="1:35">
       <c r="A843">
         <v>24</v>
       </c>
@@ -52333,7 +52386,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="844" spans="1:28">
+    <row r="844" spans="1:35">
       <c r="A844">
         <v>25</v>
       </c>
@@ -52377,7 +52430,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="845" spans="1:28">
+    <row r="845" spans="1:35">
       <c r="A845">
         <v>26</v>
       </c>
@@ -52421,7 +52474,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="846" spans="1:28">
+    <row r="846" spans="1:35">
       <c r="A846">
         <v>27</v>
       </c>
@@ -52465,7 +52518,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="847" spans="1:28">
+    <row r="847" spans="1:35">
       <c r="A847">
         <v>28</v>
       </c>
@@ -52509,7 +52562,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="848" spans="1:28">
+    <row r="848" spans="1:35">
       <c r="A848">
         <v>29</v>
       </c>
@@ -58405,7 +58458,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="977" spans="1:28">
+    <row r="977" spans="1:35">
       <c r="A977">
         <v>4</v>
       </c>
@@ -58449,7 +58502,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="978" spans="1:28">
+    <row r="978" spans="1:35">
       <c r="A978">
         <v>5</v>
       </c>
@@ -58493,7 +58546,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="979" spans="1:28">
+    <row r="979" spans="1:35">
       <c r="A979">
         <v>6</v>
       </c>
@@ -58537,7 +58590,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="980" spans="1:28">
+    <row r="980" spans="1:35">
       <c r="A980">
         <v>7</v>
       </c>
@@ -58581,7 +58634,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="981" spans="1:28">
+    <row r="981" spans="1:35">
       <c r="A981">
         <v>8</v>
       </c>
@@ -58648,8 +58701,27 @@
       <c r="AB981" s="53">
         <v>0.66805555555555562</v>
       </c>
-    </row>
-    <row r="982" spans="1:28">
+      <c r="AC981" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD981" s="70">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="AE981" s="9"/>
+      <c r="AF981" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG981" s="9">
+        <v>30</v>
+      </c>
+      <c r="AH981" s="71">
+        <v>43022</v>
+      </c>
+      <c r="AI981" s="72">
+        <v>0.84027777777777779</v>
+      </c>
+    </row>
+    <row r="982" spans="1:35">
       <c r="A982">
         <v>9</v>
       </c>
@@ -58693,7 +58765,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="983" spans="1:28">
+    <row r="983" spans="1:35">
       <c r="A983">
         <v>10</v>
       </c>
@@ -58737,7 +58809,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="984" spans="1:28">
+    <row r="984" spans="1:35">
       <c r="A984">
         <v>11</v>
       </c>
@@ -58781,7 +58853,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="985" spans="1:28">
+    <row r="985" spans="1:35">
       <c r="A985">
         <v>12</v>
       </c>
@@ -58825,7 +58897,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="986" spans="1:28">
+    <row r="986" spans="1:35">
       <c r="A986">
         <v>13</v>
       </c>
@@ -58892,8 +58964,27 @@
       <c r="AB986" s="53">
         <v>0.66875000000000007</v>
       </c>
-    </row>
-    <row r="987" spans="1:28">
+      <c r="AC986" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD986" s="70">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="AE986" s="9"/>
+      <c r="AF986" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG986" s="9">
+        <v>11</v>
+      </c>
+      <c r="AH986" s="71">
+        <v>43022</v>
+      </c>
+      <c r="AI986" s="72">
+        <v>0.84027777777777779</v>
+      </c>
+    </row>
+    <row r="987" spans="1:35">
       <c r="A987">
         <v>14</v>
       </c>
@@ -58937,7 +59028,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="988" spans="1:28">
+    <row r="988" spans="1:35">
       <c r="A988">
         <v>15</v>
       </c>
@@ -58981,7 +59072,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="989" spans="1:28">
+    <row r="989" spans="1:35">
       <c r="A989">
         <v>16</v>
       </c>
@@ -59025,7 +59116,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="990" spans="1:28">
+    <row r="990" spans="1:35">
       <c r="A990">
         <v>17</v>
       </c>
@@ -59092,8 +59183,27 @@
       <c r="AB990" s="53">
         <v>0.66805555555555562</v>
       </c>
-    </row>
-    <row r="991" spans="1:28">
+      <c r="AC990" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD990" s="70">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="AE990" s="9"/>
+      <c r="AF990" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG990" s="9">
+        <v>32</v>
+      </c>
+      <c r="AH990" s="71">
+        <v>43022</v>
+      </c>
+      <c r="AI990" s="72">
+        <v>0.84027777777777779</v>
+      </c>
+    </row>
+    <row r="991" spans="1:35">
       <c r="A991">
         <v>18</v>
       </c>
@@ -59137,7 +59247,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="992" spans="1:28">
+    <row r="992" spans="1:35">
       <c r="A992">
         <v>19</v>
       </c>
@@ -62723,7 +62833,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="1073" spans="1:28">
+    <row r="1073" spans="1:35">
       <c r="A1073">
         <v>25</v>
       </c>
@@ -62767,7 +62877,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="1074" spans="1:28">
+    <row r="1074" spans="1:35">
       <c r="A1074">
         <v>26</v>
       </c>
@@ -62811,7 +62921,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="1075" spans="1:28">
+    <row r="1075" spans="1:35">
       <c r="A1075">
         <v>27</v>
       </c>
@@ -62855,7 +62965,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="1076" spans="1:28">
+    <row r="1076" spans="1:35">
       <c r="A1076">
         <v>28</v>
       </c>
@@ -62922,8 +63032,27 @@
       <c r="AB1076" s="53">
         <v>0.66805555555555562</v>
       </c>
-    </row>
-    <row r="1077" spans="1:28">
+      <c r="AC1076" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD1076" s="70">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="AE1076" s="9"/>
+      <c r="AF1076" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG1076" s="9">
+        <v>6</v>
+      </c>
+      <c r="AH1076" s="71">
+        <v>43022</v>
+      </c>
+      <c r="AI1076" s="72">
+        <v>0.84027777777777779</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:35">
       <c r="A1077">
         <v>29</v>
       </c>
@@ -62991,7 +63120,7 @@
         <v>0.72569444444444453</v>
       </c>
     </row>
-    <row r="1078" spans="1:28">
+    <row r="1078" spans="1:35">
       <c r="A1078">
         <v>30</v>
       </c>
@@ -63035,7 +63164,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="1079" spans="1:28">
+    <row r="1079" spans="1:35">
       <c r="A1079">
         <v>31</v>
       </c>
@@ -63079,7 +63208,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="1080" spans="1:28">
+    <row r="1080" spans="1:35">
       <c r="A1080">
         <v>33</v>
       </c>
@@ -63123,7 +63252,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="1081" spans="1:28">
+    <row r="1081" spans="1:35">
       <c r="A1081">
         <v>34</v>
       </c>
@@ -63167,7 +63296,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="1082" spans="1:28">
+    <row r="1082" spans="1:35">
       <c r="A1082">
         <v>35</v>
       </c>
@@ -63211,7 +63340,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="1083" spans="1:28">
+    <row r="1083" spans="1:35">
       <c r="A1083">
         <v>36</v>
       </c>
@@ -63255,7 +63384,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="1084" spans="1:28">
+    <row r="1084" spans="1:35">
       <c r="A1084">
         <v>37</v>
       </c>
@@ -63299,7 +63428,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="1085" spans="1:28">
+    <row r="1085" spans="1:35">
       <c r="A1085">
         <v>38</v>
       </c>
@@ -63343,7 +63472,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="1086" spans="1:28">
+    <row r="1086" spans="1:35">
       <c r="A1086">
         <v>39</v>
       </c>
@@ -63387,7 +63516,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="1087" spans="1:28">
+    <row r="1087" spans="1:35">
       <c r="A1087">
         <v>40</v>
       </c>
@@ -63431,7 +63560,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="1088" spans="1:28">
+    <row r="1088" spans="1:35">
       <c r="A1088">
         <v>41</v>
       </c>
@@ -64253,7 +64382,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="1105" spans="1:28">
+    <row r="1105" spans="1:35">
       <c r="A1105">
         <v>58</v>
       </c>
@@ -64297,7 +64426,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="1106" spans="1:28">
+    <row r="1106" spans="1:35">
       <c r="A1106">
         <v>59</v>
       </c>
@@ -64341,7 +64470,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="1107" spans="1:28">
+    <row r="1107" spans="1:35">
       <c r="A1107">
         <v>60</v>
       </c>
@@ -64408,8 +64537,27 @@
       <c r="AB1107" s="53">
         <v>0.66736111111111107</v>
       </c>
-    </row>
-    <row r="1108" spans="1:28">
+      <c r="AC1107" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD1107" s="70">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="AE1107" s="9"/>
+      <c r="AF1107" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG1107" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH1107" s="71">
+        <v>43022</v>
+      </c>
+      <c r="AI1107" s="72">
+        <v>0.84027777777777779</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:35">
       <c r="A1108">
         <v>61</v>
       </c>
@@ -64447,7 +64595,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="1109" spans="1:28">
+    <row r="1109" spans="1:35">
       <c r="A1109">
         <v>62</v>
       </c>
@@ -64491,7 +64639,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="1110" spans="1:28">
+    <row r="1110" spans="1:35">
       <c r="A1110">
         <v>63</v>
       </c>
@@ -64535,7 +64683,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="1111" spans="1:28">
+    <row r="1111" spans="1:35">
       <c r="A1111">
         <v>64</v>
       </c>
@@ -64573,7 +64721,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="1112" spans="1:28">
+    <row r="1112" spans="1:35">
       <c r="A1112">
         <v>65</v>
       </c>
@@ -64617,7 +64765,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="1113" spans="1:28">
+    <row r="1113" spans="1:35">
       <c r="A1113">
         <v>66</v>
       </c>
@@ -64661,7 +64809,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="1114" spans="1:28">
+    <row r="1114" spans="1:35">
       <c r="A1114">
         <v>67</v>
       </c>
@@ -64705,7 +64853,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="1115" spans="1:28">
+    <row r="1115" spans="1:35">
       <c r="A1115">
         <v>68</v>
       </c>
@@ -64749,7 +64897,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="1116" spans="1:28">
+    <row r="1116" spans="1:35">
       <c r="A1116">
         <v>69</v>
       </c>
@@ -64793,7 +64941,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="1117" spans="1:28">
+    <row r="1117" spans="1:35">
       <c r="A1117">
         <v>70</v>
       </c>
@@ -64837,7 +64985,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="1118" spans="1:28">
+    <row r="1118" spans="1:35">
       <c r="A1118">
         <v>71</v>
       </c>
@@ -64881,7 +65029,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="1119" spans="1:28">
+    <row r="1119" spans="1:35">
       <c r="A1119">
         <v>72</v>
       </c>
@@ -64925,7 +65073,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="1120" spans="1:28">
+    <row r="1120" spans="1:35">
       <c r="A1120">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
updating repository layout and adding in datasets
</commit_message>
<xml_diff>
--- a/Data/2017-08-24_rhagoletis_data_sheet.xlsx
+++ b/Data/2017-08-24_rhagoletis_data_sheet.xlsx
@@ -11969,9 +11969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1910"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1089" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X1107" sqref="X1107"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1880" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1906" sqref="K1906:K1910"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -96506,6 +96506,9 @@
       <c r="J1906" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K1906" s="9">
+        <v>7000</v>
+      </c>
     </row>
     <row r="1907" spans="1:11">
       <c r="A1907">
@@ -96532,6 +96535,9 @@
       <c r="J1907" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K1907" s="9">
+        <v>7000</v>
+      </c>
     </row>
     <row r="1908" spans="1:11">
       <c r="A1908">
@@ -96558,6 +96564,9 @@
       <c r="J1908" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K1908" s="9">
+        <v>7000</v>
+      </c>
     </row>
     <row r="1909" spans="1:11">
       <c r="A1909">
@@ -96581,6 +96590,9 @@
       <c r="J1909" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K1909" s="9">
+        <v>7000</v>
+      </c>
     </row>
     <row r="1910" spans="1:11">
       <c r="A1910">
@@ -96606,6 +96618,9 @@
       </c>
       <c r="J1910" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="K1910" s="9">
+        <v>7000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>